<commit_message>
Add 2019 and 2020 values from the the BASE projection
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_Demands_LED.xlsx
+++ b/SuppXLS/Scen_SYS_Demands_LED.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F1D81DF-B5B0-48CD-ABB2-D649B5A58587}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A03B6E-5DC3-473F-8F4B-122B5C68F09B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="191">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -4763,10 +4763,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCA64845-990F-4F8F-9F7F-F4DBD3794313}">
-  <dimension ref="B2:AF12"/>
+  <dimension ref="B2:AF21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4902,7 +4902,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="4" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:32" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="D4" s="4" t="s">
         <v>85</v>
       </c>
@@ -4911,111 +4911,111 @@
         <v>TRAPS</v>
       </c>
       <c r="F4" s="4">
-        <v>2050</v>
+        <v>2020</v>
       </c>
       <c r="G4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.24919348706604891</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.14102260336618419</v>
       </c>
       <c r="H4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>4.9819686530101315</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>2.8193762108637852</v>
       </c>
       <c r="I4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.91879999280394731</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.51996369762144268</v>
       </c>
       <c r="J4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.42626389455684793</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.2412295956815371</v>
       </c>
       <c r="K4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.33606627740388867</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.19018531303154435</v>
       </c>
       <c r="L4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.16886184308995011</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>9.5561633661176384E-2</v>
       </c>
       <c r="M4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.48421342433443482</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.27402416687719383</v>
       </c>
       <c r="N4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.797027696417964</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.45105079601868803</v>
       </c>
       <c r="O4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.32993189380189941</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.18671376666095213</v>
       </c>
       <c r="P4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.37397423428835075</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.21163803569729758</v>
       </c>
       <c r="Q4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.65087888007008443</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.36834282959899767</v>
       </c>
       <c r="R4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.57573664768678368</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.32581863140183054</v>
       </c>
       <c r="S4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.50671859445735434</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.28676020471389613</v>
       </c>
       <c r="T4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>2.1428455103494626</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>1.2126707484972317</v>
       </c>
       <c r="U4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.65608914938754559</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.37129140482878509</v>
       </c>
       <c r="V4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.78233315899855904</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.44273492088669852</v>
       </c>
       <c r="W4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.7132297701493322</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.40362820139863753</v>
       </c>
       <c r="X4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.47360747597162428</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.26802209006972721</v>
       </c>
       <c r="Y4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.0585444755924167</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.59904734864666986</v>
       </c>
       <c r="Z4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.13585620127114331</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>7.6883209959732524E-2</v>
       </c>
       <c r="AA4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.56690203368669112</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.32081898120752922</v>
       </c>
       <c r="AB4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.29655213802722385</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.1678236258531208</v>
       </c>
       <c r="AC4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.26145480029802121</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.14796147778469043</v>
       </c>
       <c r="AD4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.29162652995454996</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.16503614500140071</v>
       </c>
       <c r="AE4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.56570516301302765</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.32014165283799628</v>
       </c>
       <c r="AF4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.2713201852314594</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.15354445783325901</v>
       </c>
     </row>
     <row r="5" spans="2:32" x14ac:dyDescent="0.2">
@@ -5023,926 +5023,1970 @@
         <v>85</v>
       </c>
       <c r="E5" s="4" t="str">
+        <f>DEMANDS!$F$17</f>
+        <v>TRAPS</v>
+      </c>
+      <c r="F5" s="4">
+        <v>2050</v>
+      </c>
+      <c r="G5" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.24919348706604891</v>
+      </c>
+      <c r="H5" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>4.9819686530101315</v>
+      </c>
+      <c r="I5" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.91879999280394731</v>
+      </c>
+      <c r="J5" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.42626389455684793</v>
+      </c>
+      <c r="K5" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.33606627740388867</v>
+      </c>
+      <c r="L5" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.16886184308995011</v>
+      </c>
+      <c r="M5" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.48421342433443482</v>
+      </c>
+      <c r="N5" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.797027696417964</v>
+      </c>
+      <c r="O5" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.32993189380189941</v>
+      </c>
+      <c r="P5" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.37397423428835075</v>
+      </c>
+      <c r="Q5" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.65087888007008443</v>
+      </c>
+      <c r="R5" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.57573664768678368</v>
+      </c>
+      <c r="S5" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.50671859445735434</v>
+      </c>
+      <c r="T5" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>2.1428455103494626</v>
+      </c>
+      <c r="U5" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.65608914938754559</v>
+      </c>
+      <c r="V5" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.78233315899855904</v>
+      </c>
+      <c r="W5" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.7132297701493322</v>
+      </c>
+      <c r="X5" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.47360747597162428</v>
+      </c>
+      <c r="Y5" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>1.0585444755924167</v>
+      </c>
+      <c r="Z5" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.13585620127114331</v>
+      </c>
+      <c r="AA5" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.56690203368669112</v>
+      </c>
+      <c r="AB5" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.29655213802722385</v>
+      </c>
+      <c r="AC5" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.26145480029802121</v>
+      </c>
+      <c r="AD5" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.29162652995454996</v>
+      </c>
+      <c r="AE5" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.56570516301302765</v>
+      </c>
+      <c r="AF5" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.2713201852314594</v>
+      </c>
+    </row>
+    <row r="6" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="D6" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E6" s="4" t="str">
         <f>DEMANDS!$F$18</f>
         <v>TRAPM</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F6" s="4">
+        <v>2020</v>
+      </c>
+      <c r="G6" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.32193664473309486</v>
+      </c>
+      <c r="H6" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>5.637813854608976</v>
+      </c>
+      <c r="I6" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>1.1480382927336128</v>
+      </c>
+      <c r="J6" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.54522568908947855</v>
+      </c>
+      <c r="K6" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.41020881320348074</v>
+      </c>
+      <c r="L6" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.21133746790128183</v>
+      </c>
+      <c r="M6" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.56924850267004323</v>
+      </c>
+      <c r="N6" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.98828046988197249</v>
+      </c>
+      <c r="O6" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.41882409160736161</v>
+      </c>
+      <c r="P6" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.47278848560105868</v>
+      </c>
+      <c r="Q6" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.83850274795415447</v>
+      </c>
+      <c r="R6" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.71154373932557857</v>
+      </c>
+      <c r="S6" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.64533477367968184</v>
+      </c>
+      <c r="T6" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>2.6080003354214218</v>
+      </c>
+      <c r="U6" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.8535978085319772</v>
+      </c>
+      <c r="V6" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.96137078018953437</v>
+      </c>
+      <c r="W6" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.932415749736074</v>
+      </c>
+      <c r="X6" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.58823966562202801</v>
+      </c>
+      <c r="Y6" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>1.3170332096303565</v>
+      </c>
+      <c r="Z6" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.17261327906182664</v>
+      </c>
+      <c r="AA6" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.72941378774211518</v>
+      </c>
+      <c r="AB6" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.39273887171064176</v>
+      </c>
+      <c r="AC6" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.32039449419408184</v>
+      </c>
+      <c r="AD6" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.34813170258514758</v>
+      </c>
+      <c r="AE6" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.64114085295794276</v>
+      </c>
+      <c r="AF6" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.35260315962707711</v>
+      </c>
+    </row>
+    <row r="7" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="D7" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E7" s="4" t="str">
+        <f>DEMANDS!$F$18</f>
+        <v>TRAPM</v>
+      </c>
+      <c r="F7" s="4">
         <v>2050</v>
       </c>
-      <c r="G5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="G7" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.42806487464250859</v>
       </c>
-      <c r="H5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="H7" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>7.4963509759251048</v>
       </c>
-      <c r="I5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="I7" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>1.5264955881963764</v>
       </c>
-      <c r="J5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="J7" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.72496241130132655</v>
       </c>
-      <c r="K5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="K7" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.54543646109867361</v>
       </c>
-      <c r="L5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="L7" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.2810060556462261</v>
       </c>
-      <c r="M5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="M7" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.75690448081146366</v>
       </c>
-      <c r="N5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="N7" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>1.3140726983795172</v>
       </c>
-      <c r="O5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="O7" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.55689181459850601</v>
       </c>
-      <c r="P5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="P7" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.62864587530576854</v>
       </c>
-      <c r="Q5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="Q7" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>1.1149199060205524</v>
       </c>
-      <c r="R5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="R7" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.94610814444434155</v>
       </c>
-      <c r="S5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="S7" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.85807302000885533</v>
       </c>
-      <c r="T5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="T7" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>3.4677423490430845</v>
       </c>
-      <c r="U5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="U7" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>1.134991138418852</v>
       </c>
-      <c r="V5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="V7" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>1.2782920777719677</v>
       </c>
-      <c r="W5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="W7" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>1.2397918582905652</v>
       </c>
-      <c r="X5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="X7" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.78215618769651429</v>
       </c>
-      <c r="Y5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="Y7" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>1.7512006321860119</v>
       </c>
-      <c r="Z5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="Z7" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.22951621964157642</v>
       </c>
-      <c r="AA5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="AA7" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.96986915506685767</v>
       </c>
-      <c r="AB5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="AB7" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.52220745490292342</v>
       </c>
-      <c r="AC5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="AC7" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.42601434548417128</v>
       </c>
-      <c r="AD5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="AD7" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.46289528099462979</v>
       </c>
-      <c r="AE5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="AE7" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.85249654967724642</v>
       </c>
-      <c r="AF5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="AF7" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.46884077905903881</v>
       </c>
     </row>
-    <row r="6" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="D6" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E6" s="4" t="str">
+    <row r="8" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="D8" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E8" s="4" t="str">
         <f>DEMANDS!$F$19</f>
         <v>TRAPL</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F8" s="4">
+        <v>2020</v>
+      </c>
+      <c r="G8" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.27435547637321495</v>
+      </c>
+      <c r="H8" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>4.8874675973215007</v>
+      </c>
+      <c r="I8" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.98750716185845822</v>
+      </c>
+      <c r="J8" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.47552429060912443</v>
+      </c>
+      <c r="K8" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.35331078909799174</v>
+      </c>
+      <c r="L8" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.18192405921838437</v>
+      </c>
+      <c r="M8" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.49433293928500699</v>
+      </c>
+      <c r="N8" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.84062004677085977</v>
+      </c>
+      <c r="O8" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.36232197941731037</v>
+      </c>
+      <c r="P8" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.40153594290187117</v>
+      </c>
+      <c r="Q8" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.71368599033539704</v>
+      </c>
+      <c r="R8" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.61113233633908892</v>
+      </c>
+      <c r="S8" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.54794246709160832</v>
+      </c>
+      <c r="T8" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>2.2342931214267647</v>
+      </c>
+      <c r="U8" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.74304638421703217</v>
+      </c>
+      <c r="V8" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.82312954869858934</v>
+      </c>
+      <c r="W8" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.79632066689536773</v>
+      </c>
+      <c r="X8" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.5014811864865022</v>
+      </c>
+      <c r="Y8" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>1.1393573908292929</v>
+      </c>
+      <c r="Z8" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.14698615350023855</v>
+      </c>
+      <c r="AA8" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.63179454507028443</v>
+      </c>
+      <c r="AB8" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.33116307912916793</v>
+      </c>
+      <c r="AC8" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.27602684102814479</v>
+      </c>
+      <c r="AD8" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.2952095661319819</v>
+      </c>
+      <c r="AE8" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.54379756531765255</v>
+      </c>
+      <c r="AF8" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.31412261464919838</v>
+      </c>
+    </row>
+    <row r="9" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="D9" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E9" s="4" t="str">
+        <f>DEMANDS!$F$19</f>
+        <v>TRAPL</v>
+      </c>
+      <c r="F9" s="4">
         <v>2050</v>
       </c>
-      <c r="G6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="G9" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.36429509503519336</v>
       </c>
-      <c r="H6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="H9" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>6.4896844647839922</v>
       </c>
-      <c r="I6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="I9" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>1.3112332224336185</v>
       </c>
-      <c r="J6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="J9" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.63141136794128272</v>
       </c>
-      <c r="K6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="K9" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.46913365533234114</v>
       </c>
-      <c r="L6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="L9" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.24156267379184618</v>
       </c>
-      <c r="M6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="M9" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.65638589568697026</v>
       </c>
-      <c r="N6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="N9" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>1.1161933556970411</v>
       </c>
-      <c r="O6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="O9" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.48109890741023575</v>
       </c>
-      <c r="P6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="P9" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.53316805049116955</v>
       </c>
-      <c r="Q6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="Q9" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.94764758885601152</v>
       </c>
-      <c r="R6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="R9" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.81147464409594539</v>
       </c>
-      <c r="S6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="S9" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.72756977830985914</v>
       </c>
-      <c r="T6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="T9" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>2.9667424021068545</v>
       </c>
-      <c r="U6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="U9" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.98663295055089162</v>
       </c>
-      <c r="V6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="V9" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>1.0929690966383923</v>
       </c>
-      <c r="W6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="W9" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>1.0573716874909749</v>
       </c>
-      <c r="X6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="X9" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.66587749187461598</v>
       </c>
-      <c r="Y6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="Y9" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>1.5128632183983965</v>
       </c>
-      <c r="Z6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="Z9" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.19517137206835286</v>
       </c>
-      <c r="AA6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="AA9" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.83891036869992042</v>
       </c>
-      <c r="AB6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="AB9" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.43972545027457505</v>
       </c>
-      <c r="AC6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="AC9" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.36651436892706152</v>
       </c>
-      <c r="AD6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="AD9" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.39198560338942773</v>
       </c>
-      <c r="AE6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="AE9" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.7220660886966046</v>
       </c>
-      <c r="AF6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="AF9" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.41709875548708081</v>
       </c>
     </row>
-    <row r="7" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="D7" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E7" s="4" t="str">
+    <row r="10" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="D10" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10" s="4" t="str">
         <f>DEMANDS!$F$20</f>
         <v>TRAF</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F10" s="4">
+        <v>2020</v>
+      </c>
+      <c r="G10" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.17991488188042462</v>
+      </c>
+      <c r="H10" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>2.6871723541686299</v>
+      </c>
+      <c r="I10" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.48763398226070803</v>
+      </c>
+      <c r="J10" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.3135901348759621</v>
+      </c>
+      <c r="K10" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.22335515894815736</v>
+      </c>
+      <c r="L10" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.10778652622510916</v>
+      </c>
+      <c r="M10" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.2824588239748011</v>
+      </c>
+      <c r="N10" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.43704621254646414</v>
+      </c>
+      <c r="O10" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.20559159765702764</v>
+      </c>
+      <c r="P10" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.23409610092244049</v>
+      </c>
+      <c r="Q10" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.47314719217489071</v>
+      </c>
+      <c r="R10" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.31213492756751032</v>
+      </c>
+      <c r="S10" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.30715715583422787</v>
+      </c>
+      <c r="T10" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>1.643458450750628</v>
+      </c>
+      <c r="U10" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.44716269403431846</v>
+      </c>
+      <c r="V10" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.50383886577623815</v>
+      </c>
+      <c r="W10" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.41246493081645397</v>
+      </c>
+      <c r="X10" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.38312416759737483</v>
+      </c>
+      <c r="Y10" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.61177286314532875</v>
+      </c>
+      <c r="Z10" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>8.1588596696128737E-2</v>
+      </c>
+      <c r="AA10" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.34456408847334713</v>
+      </c>
+      <c r="AB10" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.15301315083761008</v>
+      </c>
+      <c r="AC10" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.16686146187994025</v>
+      </c>
+      <c r="AD10" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.1939549663563945</v>
+      </c>
+      <c r="AE10" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.40532554878448751</v>
+      </c>
+      <c r="AF10" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.15629751581539669</v>
+      </c>
+    </row>
+    <row r="11" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="D11" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" s="4" t="str">
+        <f>DEMANDS!$F$20</f>
+        <v>TRAF</v>
+      </c>
+      <c r="F11" s="4">
         <v>2050</v>
       </c>
-      <c r="G7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="G11" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.14827528364690531</v>
       </c>
-      <c r="H7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="H11" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>2.2146097024218854</v>
       </c>
-      <c r="I7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="I11" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.40187930136669486</v>
       </c>
-      <c r="J7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="J11" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.2584425796889217</v>
       </c>
-      <c r="K7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="K11" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.18407620982153458</v>
       </c>
-      <c r="L7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="L11" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>8.8831327249319483E-2</v>
       </c>
-      <c r="M7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="M11" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.23278598082436783</v>
       </c>
-      <c r="N7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="N11" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.36018783135017274</v>
       </c>
-      <c r="O7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="O11" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.16943652542470969</v>
       </c>
-      <c r="P7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="P11" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.19292826364402085</v>
       </c>
-      <c r="Q7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="Q11" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.38994013943269012</v>
       </c>
-      <c r="R7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="R11" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.25724328325401569</v>
       </c>
-      <c r="S7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="S11" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.25314089601418438</v>
       </c>
-      <c r="T7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="T11" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>1.3544419750052186</v>
       </c>
-      <c r="U7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="U11" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.36852524149902982</v>
       </c>
-      <c r="V7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="V11" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.41523441504387931</v>
       </c>
-      <c r="W7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="W11" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.33992938200553119</v>
       </c>
-      <c r="X7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="X11" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.31574844742549418</v>
       </c>
-      <c r="Y7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="Y11" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.50418727935269625</v>
       </c>
-      <c r="Z7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="Z11" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>6.7240531694936503E-2</v>
       </c>
-      <c r="AA7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="AA11" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.28396949390144766</v>
       </c>
-      <c r="AB7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="AB11" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.12610445620186289</v>
       </c>
-      <c r="AC7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="AC11" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.1375174211904778</v>
       </c>
-      <c r="AD7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="AD11" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.15984629704136455</v>
       </c>
-      <c r="AE7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="AE11" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.33404552245600816</v>
       </c>
-      <c r="AF7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="AF11" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.12881123700615976</v>
       </c>
     </row>
-    <row r="8" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="D8" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E8" s="4" t="str">
+    <row r="12" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="D12" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E12" s="4" t="str">
         <f>DEMANDS!$F$21</f>
         <v>TTURS</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F12" s="4">
+        <v>2020</v>
+      </c>
+      <c r="G12" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.13064779508364899</v>
+      </c>
+      <c r="H12" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>3.0919251481787136</v>
+      </c>
+      <c r="I12" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.51060312297639665</v>
+      </c>
+      <c r="J12" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.22771801450398094</v>
+      </c>
+      <c r="K12" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.1943630348521006</v>
+      </c>
+      <c r="L12" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>9.3795533767547012E-2</v>
+      </c>
+      <c r="M12" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.29576354987636128</v>
+      </c>
+      <c r="N12" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.4475877985016371</v>
+      </c>
+      <c r="O12" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.1789052334805798</v>
+      </c>
+      <c r="P12" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.20370977252820086</v>
+      </c>
+      <c r="Q12" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.3435826806631439</v>
+      </c>
+      <c r="R12" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.32683749411207558</v>
+      </c>
+      <c r="S12" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.27266175557601846</v>
+      </c>
+      <c r="T12" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>1.2457757890372787</v>
+      </c>
+      <c r="U12" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.33895865011628784</v>
+      </c>
+      <c r="V12" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.44725505188660325</v>
+      </c>
+      <c r="W12" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.3661429011624644</v>
+      </c>
+      <c r="X12" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.26660117757391238</v>
+      </c>
+      <c r="Y12" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.5921925929827917</v>
+      </c>
+      <c r="Z12" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>7.3534707118324452E-2</v>
+      </c>
+      <c r="AA12" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.29948801716050255</v>
+      </c>
+      <c r="AB12" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.14811584497082575</v>
+      </c>
+      <c r="AC12" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.15038999597426655</v>
+      </c>
+      <c r="AD12" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.17480900790929571</v>
+      </c>
+      <c r="AE12" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.36531447683124091</v>
+      </c>
+      <c r="AF12" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.14086885317580392</v>
+      </c>
+    </row>
+    <row r="13" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="D13" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E13" s="4" t="str">
+        <f>DEMANDS!$F$21</f>
+        <v>TTURS</v>
+      </c>
+      <c r="F13" s="4">
         <v>2050</v>
       </c>
-      <c r="G8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="G13" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>9.2353600579585193E-2</v>
       </c>
-      <c r="H8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="H13" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>2.18565051154552</v>
       </c>
-      <c r="I8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="I13" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.36094016622216002</v>
       </c>
-      <c r="J8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="J13" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.160971553655473</v>
       </c>
-      <c r="K8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="K13" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.13739325701343899</v>
       </c>
-      <c r="L8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="L13" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>6.6303111018221506E-2</v>
       </c>
-      <c r="M8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="M13" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.20907225210952099</v>
       </c>
-      <c r="N8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="N13" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.31639527280693802</v>
       </c>
-      <c r="O8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="O13" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.126466294083908</v>
       </c>
-      <c r="P8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="P13" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.14400037102947</v>
       </c>
-      <c r="Q8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="Q13" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.24287511041201201</v>
       </c>
-      <c r="R8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="R13" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.23103810796296301</v>
       </c>
-      <c r="S8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="S13" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.19274182814699201</v>
       </c>
-      <c r="T8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="T13" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.880626263602864</v>
       </c>
-      <c r="U8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="U13" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.239606430141375</v>
       </c>
-      <c r="V8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="V13" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.31616005760135901</v>
       </c>
-      <c r="W8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="W13" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.25882270135028701</v>
       </c>
-      <c r="X8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="X13" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.18845766705778599</v>
       </c>
-      <c r="Y8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="Y13" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.418614934630201</v>
       </c>
-      <c r="Z8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="Z13" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>5.1980938259190403E-2</v>
       </c>
-      <c r="AA8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="AA13" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.21170504023817699</v>
       </c>
-      <c r="AB8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="AB13" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.10470158778558201</v>
       </c>
-      <c r="AC8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="AC13" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.106309162052679</v>
       </c>
-      <c r="AD8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="AD13" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.12357071379453501</v>
       </c>
-      <c r="AE8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="AE13" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.25823709659708599</v>
       </c>
-      <c r="AF8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="AF13" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>9.95787628254481E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="D9" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E9" s="4" t="str">
+    <row r="14" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="D14" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E14" s="4" t="str">
         <f>DEMANDS!$F$22</f>
         <v>TNAV</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F14" s="4">
+        <v>2020</v>
+      </c>
+      <c r="G14" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>5.2718404005341085E-2</v>
+      </c>
+      <c r="H14" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>1.2476395718090449</v>
+      </c>
+      <c r="I14" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.20603624964526826</v>
+      </c>
+      <c r="J14" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>9.1887737410560083E-2</v>
+      </c>
+      <c r="K14" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>7.8428487740468913E-2</v>
+      </c>
+      <c r="L14" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>3.7847947145898689E-2</v>
+      </c>
+      <c r="M14" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.11934516233092786</v>
+      </c>
+      <c r="N14" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.18060859254580502</v>
+      </c>
+      <c r="O14" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>7.2191026042654344E-2</v>
+      </c>
+      <c r="P14" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>8.2200040812796554E-2</v>
+      </c>
+      <c r="Q14" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.13864092047508789</v>
+      </c>
+      <c r="R14" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.13188397896544479</v>
+      </c>
+      <c r="S14" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.11002323137607345</v>
+      </c>
+      <c r="T14" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.502689779835093</v>
+      </c>
+      <c r="U14" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.13677505270176574</v>
+      </c>
+      <c r="V14" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.18047432414524345</v>
+      </c>
+      <c r="W14" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.14774431803316512</v>
+      </c>
+      <c r="X14" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.1075776945079131</v>
+      </c>
+      <c r="Y14" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.23895886146297882</v>
+      </c>
+      <c r="Z14" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>2.9672390535149896E-2</v>
+      </c>
+      <c r="AA14" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.12084804242824863</v>
+      </c>
+      <c r="AB14" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>5.9767032040341748E-2</v>
+      </c>
+      <c r="AC14" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>6.0684687109007783E-2</v>
+      </c>
+      <c r="AD14" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>7.0538135732292298E-2</v>
+      </c>
+      <c r="AE14" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.14741003601521568</v>
+      </c>
+      <c r="AF14" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>5.6842758875006463E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="D15" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" s="4" t="str">
+        <f>DEMANDS!$F$22</f>
+        <v>TNAV</v>
+      </c>
+      <c r="F15" s="4">
         <v>2050</v>
       </c>
-      <c r="G9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="G15" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>4.2004379525771102E-2</v>
       </c>
-      <c r="H9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="H15" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.99408028513777102</v>
       </c>
-      <c r="I9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="I15" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.16416325549782501</v>
       </c>
-      <c r="J9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="J15" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>7.3213282321037701E-2</v>
       </c>
-      <c r="K9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="K15" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>6.2489372105217399E-2</v>
       </c>
-      <c r="L9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="L15" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>3.0156063450376601E-2</v>
       </c>
-      <c r="M9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="M15" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>9.5090501840783506E-2</v>
       </c>
-      <c r="N9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="N15" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.143903291650118</v>
       </c>
-      <c r="O9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="O15" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>5.75195572298293E-2</v>
       </c>
-      <c r="P9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="P15" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>6.5494427922832596E-2</v>
       </c>
-      <c r="Q9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="Q15" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.110464759912835</v>
       </c>
-      <c r="R9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="R15" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.105081039730871</v>
       </c>
-      <c r="S9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="S15" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>8.7663078095158206E-2</v>
       </c>
-      <c r="T9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="T15" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.40052753292342302</v>
       </c>
-      <c r="U9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="U15" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.108978094685117</v>
       </c>
-      <c r="V9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="V15" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.14379631077765201</v>
       </c>
-      <c r="W9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="W15" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.117718063066032</v>
       </c>
-      <c r="X9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="X15" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>8.5714550618035304E-2</v>
       </c>
-      <c r="Y9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="Y15" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.190394965426499</v>
       </c>
-      <c r="Z9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="Z15" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>2.36420350158753E-2</v>
       </c>
-      <c r="AA9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="AA15" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>9.6287949813282703E-2</v>
       </c>
-      <c r="AB9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="AB15" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>4.7620506430678201E-2</v>
       </c>
-      <c r="AC9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="AC15" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>4.8351665359049598E-2</v>
       </c>
-      <c r="AD9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="AD15" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>5.6202585799816303E-2</v>
       </c>
-      <c r="AE9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="AE15" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.117451717583548</v>
       </c>
-      <c r="AF9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="AF15" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>4.5290536808279797E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="D10" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E10" s="4" t="str">
+    <row r="16" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="D16" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E16" s="4" t="str">
         <f>DEMANDS!$F$23</f>
         <v>TOTH</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F16" s="4">
+        <v>2020</v>
+      </c>
+      <c r="G16" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.16235731275947515</v>
+      </c>
+      <c r="H16" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>3.8423660957334085</v>
+      </c>
+      <c r="I16" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.63453157307374231</v>
+      </c>
+      <c r="J16" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.28298743869437681</v>
+      </c>
+      <c r="K16" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.24153687414440531</v>
+      </c>
+      <c r="L16" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.11656064154461539</v>
+      </c>
+      <c r="M16" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.3675483014419349</v>
+      </c>
+      <c r="N16" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.55622180337699523</v>
+      </c>
+      <c r="O16" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.22232731082767995</v>
+      </c>
+      <c r="P16" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.25315215790168288</v>
+      </c>
+      <c r="Q16" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.42697361028901426</v>
+      </c>
+      <c r="R16" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.40616420062123709</v>
+      </c>
+      <c r="S16" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.3388394721798389</v>
+      </c>
+      <c r="T16" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>1.5481379481330504</v>
+      </c>
+      <c r="U16" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.4212272815949526</v>
+      </c>
+      <c r="V16" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.55580829585310521</v>
+      </c>
+      <c r="W16" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.45500942040877851</v>
+      </c>
+      <c r="X16" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.33130793169298151</v>
+      </c>
+      <c r="Y16" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.73592361793165129</v>
+      </c>
+      <c r="Z16" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>9.1382311003734881E-2</v>
+      </c>
+      <c r="AA16" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.37217673393347922</v>
+      </c>
+      <c r="AB16" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.18406503187570397</v>
+      </c>
+      <c r="AC16" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.18689114191829229</v>
+      </c>
+      <c r="AD16" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.21723689061978846</v>
+      </c>
+      <c r="AE16" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.45397992926309294</v>
+      </c>
+      <c r="AF16" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.17505912318297531</v>
+      </c>
+    </row>
+    <row r="17" spans="4:32" x14ac:dyDescent="0.2">
+      <c r="D17" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E17" s="4" t="str">
+        <f>DEMANDS!$F$23</f>
+        <v>TOTH</v>
+      </c>
+      <c r="F17" s="4">
         <v>2050</v>
       </c>
-      <c r="G10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="G17" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.26045346019004401</v>
       </c>
-      <c r="H10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="H17" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>6.1639203553045512</v>
       </c>
-      <c r="I10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="I17" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>1.0179149987024101</v>
       </c>
-      <c r="J10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="J17" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.45396820349853301</v>
       </c>
-      <c r="K10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="K17" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.38747324382976506</v>
       </c>
-      <c r="L10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="L17" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.18698647998221901</v>
       </c>
-      <c r="M10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="M17" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.58962066611279595</v>
       </c>
-      <c r="N10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="N17" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.89229053413382609</v>
       </c>
-      <c r="O10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="O17" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.35665727903246103</v>
       </c>
-      <c r="P10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="P17" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.40610647195022492</v>
       </c>
-      <c r="Q10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="Q17" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.68495069497951599</v>
       </c>
-      <c r="R10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="R17" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.65156825805464502</v>
       </c>
-      <c r="S10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="S17" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.54356598713202597</v>
       </c>
-      <c r="T10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="T17" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>2.4835215524915499</v>
       </c>
-      <c r="U10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="U17" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.67573243947675998</v>
       </c>
-      <c r="V10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="V17" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.89162718572295807</v>
       </c>
-      <c r="W10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="W17" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.72992571723638999</v>
       </c>
-      <c r="X10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="X17" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.53148389642096905</v>
       </c>
-      <c r="Y10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="Y17" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>1.1805680290473299</v>
       </c>
-      <c r="Z10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="Z17" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.146595423985277</v>
       </c>
-      <c r="AA10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="AA17" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.59704559349789399</v>
       </c>
-      <c r="AB10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="AB17" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.29527696435231898</v>
       </c>
-      <c r="AC10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="AC17" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.29981060762935702</v>
       </c>
-      <c r="AD10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="AD17" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.34849123135384003</v>
       </c>
-      <c r="AE10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="AE17" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.72827420843415902</v>
       </c>
-      <c r="AF10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="AF17" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.28082969344526898</v>
       </c>
     </row>
-    <row r="11" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="D11" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E11" s="4" t="str">
+    <row r="18" spans="4:32" x14ac:dyDescent="0.2">
+      <c r="D18" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" s="4" t="str">
         <f>DEMANDS!$F$24</f>
         <v>TAVIDOM</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F18" s="4">
+        <v>2020</v>
+      </c>
+      <c r="G18" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.13395677260860595</v>
+      </c>
+      <c r="I18" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="J18" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="K18" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="L18" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="M18" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="N18" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="O18" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="P18" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Q18" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R18" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S18" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>4.6779068407982807E-2</v>
+      </c>
+      <c r="T18" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>4.6352277307537207E-4</v>
+      </c>
+      <c r="U18" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>4.6529102661710439E-2</v>
+      </c>
+      <c r="V18" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W18" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X18" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y18" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z18" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA18" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>9.2704554615074527E-5</v>
+      </c>
+      <c r="AB18" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AC18" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AD18" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AE18" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AF18" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="4:32" x14ac:dyDescent="0.2">
+      <c r="D19" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19" s="4" t="str">
+        <f>DEMANDS!$F$24</f>
+        <v>TAVIDOM</v>
+      </c>
+      <c r="F19" s="4">
         <v>2050</v>
       </c>
-      <c r="G11" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="H11" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="G19" s="4">
+        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.13599128494106499</v>
       </c>
-      <c r="I11" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="J11" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="K11" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="L11" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="M11" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="N11" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="O11" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="P11" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="Q11" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="R11" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="S11" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="I19" s="4">
+        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="J19" s="4">
+        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="K19" s="4">
+        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="L19" s="4">
+        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="M19" s="4">
+        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="N19" s="4">
+        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="O19" s="4">
+        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="P19" s="4">
+        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Q19" s="4">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R19" s="4">
+        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S19" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>4.7489540821759602E-2</v>
       </c>
-      <c r="T11" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="T19" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>4.7056267691773199E-4</v>
       </c>
-      <c r="U11" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="U19" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>4.7235778638893701E-2</v>
       </c>
-      <c r="V11" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="W11" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="X11" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="Y11" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="Z11" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="AA11" s="16">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="V19" s="4">
+        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W19" s="4">
+        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X19" s="4">
+        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y19" s="4">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z19" s="4">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA19" s="16">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>9.4112535383546506E-5</v>
       </c>
-      <c r="AB11" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="AC11" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="AD11" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="AE11" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="AF11" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="D12" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E12" s="4" t="str">
+      <c r="AB19" s="4">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AC19" s="4">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AD19" s="4">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AE19" s="4">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AF19" s="4">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="4:32" x14ac:dyDescent="0.2">
+      <c r="D20" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E20" s="4" t="str">
         <f>DEMANDS!$F$25</f>
         <v>TAVIINT</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F20" s="4">
+        <v>2020</v>
+      </c>
+      <c r="G20" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H20" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>41.184477806263274</v>
+      </c>
+      <c r="I20" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="J20" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="K20" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="L20" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="M20" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="N20" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="O20" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="P20" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Q20" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R20" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S20" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>2.4385793540260186</v>
+      </c>
+      <c r="T20" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>2.2547565653239303</v>
+      </c>
+      <c r="U20" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.24571396736982151</v>
+      </c>
+      <c r="V20" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W20" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X20" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y20" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z20" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA20" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0.70149337318584271</v>
+      </c>
+      <c r="AB20" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AC20" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AD20" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AE20" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AF20" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="4:32" x14ac:dyDescent="0.2">
+      <c r="D21" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E21" s="4" t="str">
+        <f>DEMANDS!$F$25</f>
+        <v>TAVIINT</v>
+      </c>
+      <c r="F21" s="4">
         <v>2050</v>
       </c>
-      <c r="G12" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="H12" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="G21" s="4">
+        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>40.411547456014503</v>
       </c>
-      <c r="I12" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="J12" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="K12" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="L12" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="M12" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="N12" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="O12" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="P12" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="Q12" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="R12" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="S12" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="I21" s="4">
+        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="J21" s="4">
+        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="K21" s="4">
+        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="L21" s="4">
+        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="M21" s="4">
+        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="N21" s="4">
+        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="O21" s="4">
+        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="P21" s="4">
+        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Q21" s="4">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R21" s="4">
+        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S21" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>2.3928132767411898</v>
       </c>
-      <c r="T12" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="T21" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>2.2124403851853902</v>
       </c>
-      <c r="U12" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="U21" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.24110252653151398</v>
       </c>
-      <c r="V12" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="W12" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="X12" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="Y12" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="Z12" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="AA12" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="V21" s="4">
+        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W21" s="4">
+        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X21" s="4">
+        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y21" s="4">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z21" s="4">
+        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA21" s="15">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.68832808501139198</v>
       </c>
-      <c r="AB12" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="AC12" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="AD12" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="AE12" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="AF12" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+      <c r="AB21" s="4">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AC21" s="4">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AD21" s="4">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AE21" s="4">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AF21" s="4">
+        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
     </row>
@@ -6719,10 +7763,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C1:I56"/>
+  <dimension ref="C1:Q57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6732,10 +7776,12 @@
     <col min="5" max="5" width="10.7109375" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="53.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.85546875" customWidth="1"/>
+    <col min="11" max="12" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>190</v>
       </c>
@@ -6743,7 +7789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="14" t="s">
         <v>1</v>
       </c>
@@ -6763,10 +7809,16 @@
         <v>2018</v>
       </c>
       <c r="I2" s="14">
+        <v>2019</v>
+      </c>
+      <c r="J2" s="14">
+        <v>2020</v>
+      </c>
+      <c r="K2" s="14">
         <v>2050</v>
       </c>
     </row>
-    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D3" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -6785,10 +7837,17 @@
         <v>2.0712927345907701</v>
       </c>
       <c r="I3">
+        <v>2.0621875420000002</v>
+      </c>
+      <c r="J3">
+        <v>2.2653176519999998</v>
+      </c>
+      <c r="K3">
         <v>1.35257371315</v>
       </c>
-    </row>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="O3" s="2"/>
+    </row>
+    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D4" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -6807,10 +7866,17 @@
         <v>22.2490403410117</v>
       </c>
       <c r="I4">
+        <v>21.66628807</v>
+      </c>
+      <c r="J4">
+        <v>22.058152969999998</v>
+      </c>
+      <c r="K4">
         <v>16.999477698500002</v>
       </c>
-    </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="O4" s="2"/>
+    </row>
+    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D5" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -6829,10 +7895,17 @@
         <v>1.2014578872914701</v>
       </c>
       <c r="I5">
+        <v>1.2266704420000001</v>
+      </c>
+      <c r="J5">
+        <v>0.82191421200000003</v>
+      </c>
+      <c r="K5">
         <v>1.5123719028</v>
       </c>
-    </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="O5" s="2"/>
+    </row>
+    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D6" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -6851,10 +7924,17 @@
         <v>6.6890404714869804</v>
       </c>
       <c r="I6">
+        <v>6.4509543440000003</v>
+      </c>
+      <c r="J6">
+        <v>5.7840131420000001</v>
+      </c>
+      <c r="K6">
         <v>4.7096123024500001</v>
       </c>
-    </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="O6" s="2"/>
+    </row>
+    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D7" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -6873,10 +7953,17 @@
         <v>0.67287296253748397</v>
       </c>
       <c r="I7">
+        <v>0.68901566299999994</v>
+      </c>
+      <c r="J7">
+        <v>1.2574088990000001</v>
+      </c>
+      <c r="K7">
         <v>1.1058949143000001</v>
       </c>
-    </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="O7" s="2"/>
+    </row>
+    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D8" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -6895,10 +7982,17 @@
         <v>10.5976971594968</v>
       </c>
       <c r="I8">
+        <v>10.01814809</v>
+      </c>
+      <c r="J8">
+        <v>10.12574641</v>
+      </c>
+      <c r="K8">
         <v>8.6539440184999989</v>
       </c>
-    </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="O8" s="2"/>
+    </row>
+    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D9" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -6917,10 +8011,17 @@
         <v>1.14056826967015</v>
       </c>
       <c r="I9">
+        <v>1.166030828</v>
+      </c>
+      <c r="J9">
+        <v>1.449528948</v>
+      </c>
+      <c r="K9">
         <v>1.5435020469</v>
       </c>
-    </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="O9" s="2"/>
+    </row>
+    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D10" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -6939,10 +8040,17 @@
         <v>17.770098364755199</v>
       </c>
       <c r="I10">
+        <v>17.35242646</v>
+      </c>
+      <c r="J10">
+        <v>14.23391084</v>
+      </c>
+      <c r="K10">
         <v>8.8850491823775997</v>
       </c>
-    </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="O10" s="2"/>
+    </row>
+    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D11" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -6961,10 +8069,17 @@
         <v>19.5397050142764</v>
       </c>
       <c r="I11">
+        <v>20.047656180000001</v>
+      </c>
+      <c r="J11">
+        <v>18.18372415</v>
+      </c>
+      <c r="K11">
         <v>11.597079862500001</v>
       </c>
-    </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="O11" s="2"/>
+    </row>
+    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D12" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -6983,10 +8098,17 @@
         <v>1.28965569884044</v>
       </c>
       <c r="I12">
+        <v>1.3174050900000001</v>
+      </c>
+      <c r="J12">
+        <v>2.2668447500000002</v>
+      </c>
+      <c r="K12">
         <v>0.55274769385</v>
       </c>
-    </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="O12" s="2"/>
+    </row>
+    <row r="13" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D13" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -7005,10 +8127,17 @@
         <v>4.2689583715443504</v>
       </c>
       <c r="I13">
+        <v>6.5958660199999999</v>
+      </c>
+      <c r="J13">
+        <v>7.0076904100000004</v>
+      </c>
+      <c r="K13">
         <v>15.964089531500001</v>
       </c>
-    </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="O13" s="2"/>
+    </row>
+    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D14" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -7027,10 +8156,17 @@
         <v>0.16518244671693</v>
       </c>
       <c r="I14">
+        <v>0.190364161</v>
+      </c>
+      <c r="J14">
+        <v>0.186509807</v>
+      </c>
+      <c r="K14">
         <v>3.6153808350000004E-2</v>
       </c>
-    </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="O14" s="2"/>
+    </row>
+    <row r="15" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D15" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -7049,10 +8185,17 @@
         <v>4.2546573385120396</v>
       </c>
       <c r="I15">
+        <v>3.3313444579999998</v>
+      </c>
+      <c r="J15">
+        <v>3.4153449619999998</v>
+      </c>
+      <c r="K15">
         <v>4.3738132234500009</v>
       </c>
-    </row>
-    <row r="16" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="O15" s="2"/>
+    </row>
+    <row r="16" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D16" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -7071,10 +8214,17 @@
         <v>4.0239683065477196</v>
       </c>
       <c r="I16">
+        <v>4.1335439039999997</v>
+      </c>
+      <c r="J16">
+        <v>4.0998448639999996</v>
+      </c>
+      <c r="K16">
         <v>4.2364449446000005</v>
       </c>
-    </row>
-    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="O16" s="2"/>
+    </row>
+    <row r="17" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D17" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -7092,11 +8242,18 @@
         <f>VLOOKUP(F17,'BY-Demands'!$I$5:$J$65,2,FALSE)</f>
         <v>14.5565610923972</v>
       </c>
-      <c r="I17" s="1">
+      <c r="I17">
+        <v>14.87639834</v>
+      </c>
+      <c r="J17">
+        <v>10.76129175</v>
+      </c>
+      <c r="K17" s="1">
         <v>19.015702110918735</v>
       </c>
-    </row>
-    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="O17" s="2"/>
+    </row>
+    <row r="18" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D18" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -7114,11 +8271,18 @@
         <f>VLOOKUP(F18,'BY-Demands'!$I$5:$J$65,2,FALSE)</f>
         <v>31.276118540281001</v>
       </c>
-      <c r="I18" s="1">
+      <c r="I18">
+        <v>31.984256429999999</v>
+      </c>
+      <c r="J18">
+        <v>23.13677727</v>
+      </c>
+      <c r="K18" s="1">
         <v>30.763946334612658</v>
       </c>
-    </row>
-    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="O18" s="2"/>
+    </row>
+    <row r="19" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -7136,11 +8300,18 @@
         <f>VLOOKUP(F19,'BY-Demands'!$I$5:$J$65,2,FALSE)</f>
         <v>27.131577542973599</v>
       </c>
-      <c r="I19" s="1">
+      <c r="I19">
+        <v>27.52133693</v>
+      </c>
+      <c r="J19">
+        <v>19.908389740000001</v>
+      </c>
+      <c r="K19" s="1">
         <v>26.43478755446861</v>
       </c>
-    </row>
-    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="O19" s="2"/>
+    </row>
+    <row r="20" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D20" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -7158,11 +8329,18 @@
         <f>VLOOKUP(F20,'BY-Demands'!$I$5:$J$65,2,FALSE)</f>
         <v>11.625551</v>
       </c>
-      <c r="I20" s="1">
+      <c r="I20">
+        <v>14.23064449</v>
+      </c>
+      <c r="J20">
+        <v>11.754512350000001</v>
+      </c>
+      <c r="K20" s="1">
         <v>9.6873790239635298</v>
       </c>
-    </row>
-    <row r="21" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="O20" s="2"/>
+    </row>
+    <row r="21" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D21" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -7181,11 +8359,18 @@
         <v>7.7245727925227703</v>
       </c>
       <c r="I21">
+        <v>10.927548</v>
+      </c>
+      <c r="J21">
+        <v>10.927548</v>
+      </c>
+      <c r="K21">
         <f>H21</f>
         <v>7.7245727925227703</v>
       </c>
-    </row>
-    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="O21" s="2"/>
+    </row>
+    <row r="22" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D22" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -7204,11 +8389,18 @@
         <v>3.5132998087277199</v>
       </c>
       <c r="I22">
-        <f t="shared" ref="I22:I28" si="0">H22</f>
+        <v>4.2966351471015702</v>
+      </c>
+      <c r="J22">
+        <v>4.4094344637268001</v>
+      </c>
+      <c r="K22">
+        <f t="shared" ref="K22:K28" si="0">H22</f>
         <v>3.5132998087277199</v>
       </c>
-    </row>
-    <row r="23" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="O22" s="2"/>
+    </row>
+    <row r="23" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D23" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -7227,11 +8419,18 @@
         <v>21.784659175997099</v>
       </c>
       <c r="I23">
+        <v>13.63038308</v>
+      </c>
+      <c r="J23">
+        <v>13.57977245</v>
+      </c>
+      <c r="K23">
         <f t="shared" si="0"/>
         <v>21.784659175997099</v>
       </c>
-    </row>
-    <row r="24" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="O23" s="2"/>
+    </row>
+    <row r="24" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D24" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -7250,11 +8449,18 @@
         <v>0.23349320028657899</v>
       </c>
       <c r="I24">
+        <v>0.23</v>
+      </c>
+      <c r="J24">
+        <v>0.23</v>
+      </c>
+      <c r="K24">
         <f t="shared" si="0"/>
         <v>0.23349320028657899</v>
       </c>
-    </row>
-    <row r="25" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="O24" s="2"/>
+    </row>
+    <row r="25" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D25" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -7273,11 +8479,18 @@
         <v>45.935836654432002</v>
       </c>
       <c r="I25">
+        <v>46.104277330000002</v>
+      </c>
+      <c r="J25">
+        <v>46.814427170000002</v>
+      </c>
+      <c r="K25">
         <f t="shared" si="0"/>
         <v>45.935836654432002</v>
       </c>
-    </row>
-    <row r="26" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="O25" s="2"/>
+    </row>
+    <row r="26" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D26" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -7296,11 +8509,18 @@
         <v>206.79888500000001</v>
       </c>
       <c r="I26">
+        <v>218.95666940000001</v>
+      </c>
+      <c r="J26">
+        <v>225.3003382</v>
+      </c>
+      <c r="K26">
         <f t="shared" si="0"/>
         <v>206.79888500000001</v>
       </c>
-    </row>
-    <row r="27" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="O26" s="2"/>
+    </row>
+    <row r="27" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D27" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -7319,11 +8539,18 @@
         <v>766.351721</v>
       </c>
       <c r="I27">
+        <v>776.01961870000002</v>
+      </c>
+      <c r="J27">
+        <v>788.3008562</v>
+      </c>
+      <c r="K27">
         <f t="shared" si="0"/>
         <v>766.351721</v>
       </c>
-    </row>
-    <row r="28" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="O27" s="2"/>
+    </row>
+    <row r="28" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D28" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -7342,11 +8569,18 @@
         <v>724.42972899999995</v>
       </c>
       <c r="I28">
+        <v>729.04047590000005</v>
+      </c>
+      <c r="J28">
+        <v>739.68368569999996</v>
+      </c>
+      <c r="K28">
         <f t="shared" si="0"/>
         <v>724.42972899999995</v>
       </c>
-    </row>
-    <row r="29" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="O28" s="2"/>
+    </row>
+    <row r="29" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D29" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -7364,11 +8598,22 @@
         <f>VLOOKUP(F29,'BY-Demands'!$I$5:$J$65,2,FALSE)</f>
         <v>12.7133829170957</v>
       </c>
-      <c r="I29">
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29">
         <v>8.3303707615599745</v>
       </c>
-    </row>
-    <row r="30" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="O29" s="2"/>
+      <c r="P29" t="str">
+        <f>IF(P66&lt;&gt;"",P66*$H29,"")</f>
+        <v/>
+      </c>
+      <c r="Q29" t="str">
+        <f t="shared" ref="Q29" si="1">IF(Q66&lt;&gt;"",Q66*$H29,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D30" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -7386,11 +8631,22 @@
         <f>VLOOKUP(F30,'BY-Demands'!$I$5:$J$65,2,FALSE)</f>
         <v>11.4839387329157</v>
       </c>
-      <c r="I30">
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30">
         <v>7.5247845525179748</v>
       </c>
-    </row>
-    <row r="31" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="O30" s="2"/>
+      <c r="P30" t="str">
+        <f>IF(P67&lt;&gt;"",P67*$H30,"")</f>
+        <v/>
+      </c>
+      <c r="Q30" t="str">
+        <f>IF(Q67&lt;&gt;"",Q67*$H30,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D31" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -7408,11 +8664,22 @@
         <f>VLOOKUP(F31,'BY-Demands'!$I$5:$J$65,2,FALSE)</f>
         <v>8.8153537670115707</v>
       </c>
-      <c r="I31">
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31">
         <v>5.7762096629087072</v>
       </c>
-    </row>
-    <row r="32" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="O31" s="2"/>
+      <c r="P31" t="str">
+        <f>IF(P68&lt;&gt;"",P68*$H31,"")</f>
+        <v/>
+      </c>
+      <c r="Q31" t="str">
+        <f>IF(Q68&lt;&gt;"",Q68*$H31,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D32" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -7430,11 +8697,22 @@
         <f>VLOOKUP(F32,'BY-Demands'!$I$5:$J$65,2,FALSE)</f>
         <v>4.3126302226859501</v>
       </c>
-      <c r="I32">
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32">
         <v>2.8258260553410754</v>
       </c>
-    </row>
-    <row r="33" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="O32" s="2"/>
+      <c r="P32" t="str">
+        <f>IF(P69&lt;&gt;"",P69*$H32,"")</f>
+        <v/>
+      </c>
+      <c r="Q32" t="str">
+        <f>IF(Q69&lt;&gt;"",Q69*$H32,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D33" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -7452,11 +8730,22 @@
         <f>VLOOKUP(F33,'BY-Demands'!$I$5:$J$65,2,FALSE)</f>
         <v>1.3178746133407899</v>
       </c>
-      <c r="I33">
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33">
         <v>0.86352973225925755</v>
       </c>
-    </row>
-    <row r="34" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="O33" s="2"/>
+      <c r="P33" t="str">
+        <f>IF(P70&lt;&gt;"",P70*$H33,"")</f>
+        <v/>
+      </c>
+      <c r="Q33" t="str">
+        <f>IF(Q70&lt;&gt;"",Q70*$H33,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D34" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -7474,11 +8763,22 @@
         <f>VLOOKUP(F34,'BY-Demands'!$I$5:$J$65,2,FALSE)</f>
         <v>1.2331093201030401</v>
       </c>
-      <c r="I34">
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34">
         <v>0.80798776317929155</v>
       </c>
-    </row>
-    <row r="35" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="O34" s="2"/>
+      <c r="P34" t="str">
+        <f>IF(P71&lt;&gt;"",P71*$H34,"")</f>
+        <v/>
+      </c>
+      <c r="Q34" t="str">
+        <f>IF(Q71&lt;&gt;"",Q71*$H34,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D35" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -7496,11 +8796,22 @@
         <f>VLOOKUP(F35,'BY-Demands'!$I$5:$J$65,2,FALSE)</f>
         <v>35.9977015327608</v>
       </c>
-      <c r="I35">
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35">
         <v>23.587286108700724</v>
       </c>
-    </row>
-    <row r="36" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="O35" s="2"/>
+      <c r="P35" t="str">
+        <f>IF(P72&lt;&gt;"",P72*$H35,"")</f>
+        <v/>
+      </c>
+      <c r="Q35" t="str">
+        <f>IF(Q72&lt;&gt;"",Q72*$H35,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D36" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -7518,11 +8829,22 @@
         <f>VLOOKUP(F36,'BY-Demands'!$I$5:$J$65,2,FALSE)</f>
         <v>0.84071163403600102</v>
       </c>
-      <c r="I36">
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36">
         <v>0.55087144494553486</v>
       </c>
-    </row>
-    <row r="37" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="O36" s="2"/>
+      <c r="P36" t="str">
+        <f>IF(P73&lt;&gt;"",P73*$H36,"")</f>
+        <v/>
+      </c>
+      <c r="Q36" t="str">
+        <f>IF(Q73&lt;&gt;"",Q73*$H36,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D37" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -7540,11 +8862,22 @@
         <f>VLOOKUP(F37,'BY-Demands'!$I$5:$J$65,2,FALSE)</f>
         <v>2.5953782987835501</v>
       </c>
-      <c r="I37">
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37">
         <v>1.7006066461478033</v>
       </c>
-    </row>
-    <row r="38" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="O37" s="2"/>
+      <c r="P37" t="str">
+        <f>IF(P74&lt;&gt;"",P74*$H37,"")</f>
+        <v/>
+      </c>
+      <c r="Q37" t="str">
+        <f>IF(Q74&lt;&gt;"",Q74*$H37,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D38" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -7562,11 +8895,22 @@
         <f>VLOOKUP(F38,'BY-Demands'!$I$5:$J$65,2,FALSE)</f>
         <v>1.1448908452668201</v>
       </c>
-      <c r="I38">
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38">
         <v>0.75018311632173929</v>
       </c>
-    </row>
-    <row r="39" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="O38" s="2"/>
+      <c r="P38" t="str">
+        <f>IF(P75&lt;&gt;"",P75*$H38,"")</f>
+        <v/>
+      </c>
+      <c r="Q38" t="str">
+        <f>IF(Q75&lt;&gt;"",Q75*$H38,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D39" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -7584,11 +8928,22 @@
         <f>VLOOKUP(F39,'BY-Demands'!$I$5:$J$65,2,FALSE)</f>
         <v>8.0991705816317694</v>
       </c>
-      <c r="I39">
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39">
         <v>5.3069347641179023</v>
       </c>
-    </row>
-    <row r="40" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="O39" s="2"/>
+      <c r="P39" t="str">
+        <f>IF(P76&lt;&gt;"",P76*$H39,"")</f>
+        <v/>
+      </c>
+      <c r="Q39" t="str">
+        <f>IF(Q76&lt;&gt;"",Q76*$H39,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D40" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -7606,11 +8961,13 @@
         <f>VLOOKUP(F40,'BY-Demands'!$I$5:$J$65,2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="I40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D41" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -7627,33 +8984,11 @@
       <c r="H41">
         <v>7.8120000000000003</v>
       </c>
-      <c r="I41">
+      <c r="K41">
         <v>32.865000000000002</v>
       </c>
     </row>
-    <row r="42" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D42" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
-        <v>IE,National</v>
-      </c>
-      <c r="E42" t="s">
-        <v>85</v>
-      </c>
-      <c r="F42" t="s">
-        <v>160</v>
-      </c>
-      <c r="G42" t="s">
-        <v>161</v>
-      </c>
-      <c r="H42" s="2">
-        <f>VLOOKUP(F42,'BY-Demands'!$I$5:$J$65,2,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="I42">
-        <v>10.047893325490021</v>
-      </c>
-    </row>
-    <row r="43" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D43" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -7662,20 +8997,22 @@
         <v>85</v>
       </c>
       <c r="F43" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G43" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H43" s="2">
         <f>VLOOKUP(F43,'BY-Demands'!$I$5:$J$65,2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="I43">
-        <v>16.878788423834521</v>
-      </c>
-    </row>
-    <row r="44" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43">
+        <v>10.047893325490021</v>
+      </c>
+    </row>
+    <row r="44" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D44" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -7684,20 +9021,22 @@
         <v>85</v>
       </c>
       <c r="F44" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G44" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H44" s="2">
         <f>VLOOKUP(F44,'BY-Demands'!$I$5:$J$65,2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="I44">
-        <v>14.214862498864701</v>
-      </c>
-    </row>
-    <row r="45" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44">
+        <v>16.878788423834521</v>
+      </c>
+    </row>
+    <row r="45" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D45" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -7706,20 +9045,22 @@
         <v>85</v>
       </c>
       <c r="F45" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G45" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H45" s="2">
         <f>VLOOKUP(F45,'BY-Demands'!$I$5:$J$65,2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="I45">
-        <v>0.179228357755223</v>
-      </c>
-    </row>
-    <row r="46" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45">
+        <v>14.214862498864701</v>
+      </c>
+    </row>
+    <row r="46" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D46" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -7728,20 +9069,22 @@
         <v>85</v>
       </c>
       <c r="F46" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G46" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H46" s="2">
         <f>VLOOKUP(F46,'BY-Demands'!$I$5:$J$65,2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="I46">
-        <v>0.30107381041032272</v>
-      </c>
-    </row>
-    <row r="47" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46">
+        <v>0.179228357755223</v>
+      </c>
+    </row>
+    <row r="47" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D47" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -7750,20 +9093,22 @@
         <v>85</v>
       </c>
       <c r="F47" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G47" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H47" s="2">
         <f>VLOOKUP(F47,'BY-Demands'!$I$5:$J$65,2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="I47">
-        <v>0.2535562807901901</v>
-      </c>
-    </row>
-    <row r="48" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47">
+        <v>0.30107381041032272</v>
+      </c>
+    </row>
+    <row r="48" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D48" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -7772,20 +9117,22 @@
         <v>85</v>
       </c>
       <c r="F48" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G48" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H48" s="2">
         <f>VLOOKUP(F48,'BY-Demands'!$I$5:$J$65,2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="I48">
-        <v>5.3250910380053398</v>
-      </c>
-    </row>
-    <row r="49" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48">
+        <v>0.2535562807901901</v>
+      </c>
+    </row>
+    <row r="49" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D49" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -7794,20 +9141,22 @@
         <v>85</v>
       </c>
       <c r="F49" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G49" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H49" s="2">
         <f>VLOOKUP(F49,'BY-Demands'!$I$5:$J$65,2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="I49">
-        <v>8.9452666401358414</v>
-      </c>
-    </row>
-    <row r="50" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49">
+        <v>5.3250910380053398</v>
+      </c>
+    </row>
+    <row r="50" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D50" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -7816,20 +9165,22 @@
         <v>85</v>
       </c>
       <c r="F50" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G50" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H50" s="2">
         <f>VLOOKUP(F50,'BY-Demands'!$I$5:$J$65,2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="I50">
-        <v>7.5334634283143167</v>
-      </c>
-    </row>
-    <row r="51" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50">
+        <v>8.9452666401358414</v>
+      </c>
+    </row>
+    <row r="51" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D51" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -7838,20 +9189,22 @@
         <v>85</v>
       </c>
       <c r="F51" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G51" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H51" s="2">
         <f>VLOOKUP(F51,'BY-Demands'!$I$5:$J$65,2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="I51">
-        <v>0.89996641800005883</v>
-      </c>
-    </row>
-    <row r="52" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51">
+        <v>7.5334634283143167</v>
+      </c>
+    </row>
+    <row r="52" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D52" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -7860,20 +9213,22 @@
         <v>85</v>
       </c>
       <c r="F52" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G52" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H52" s="2">
         <f>VLOOKUP(F52,'BY-Demands'!$I$5:$J$65,2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="I52">
-        <v>1.5117937925797396</v>
-      </c>
-    </row>
-    <row r="53" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52">
+        <v>0.89996641800005883</v>
+      </c>
+    </row>
+    <row r="53" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D53" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -7882,20 +9237,22 @@
         <v>85</v>
       </c>
       <c r="F53" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G53" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="H53" s="2">
         <f>VLOOKUP(F53,'BY-Demands'!$I$5:$J$65,2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="I53">
-        <v>1.2731921479513455</v>
-      </c>
-    </row>
-    <row r="54" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53">
+        <v>1.5117937925797396</v>
+      </c>
+    </row>
+    <row r="54" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D54" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -7904,20 +9261,22 @@
         <v>85</v>
       </c>
       <c r="F54" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G54" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H54" s="2">
         <f>VLOOKUP(F54,'BY-Demands'!$I$5:$J$65,2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="I54">
-        <v>1.4030879288454441</v>
-      </c>
-    </row>
-    <row r="55" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
+      <c r="K54">
+        <v>1.2731921479513455</v>
+      </c>
+    </row>
+    <row r="55" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D55" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -7926,20 +9285,22 @@
         <v>85</v>
       </c>
       <c r="F55" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G55" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="H55" s="2">
         <f>VLOOKUP(F55,'BY-Demands'!$I$5:$J$65,2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="I55">
-        <v>2.3569541916751464</v>
-      </c>
-    </row>
-    <row r="56" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+      <c r="K55">
+        <v>1.4030879288454441</v>
+      </c>
+    </row>
+    <row r="56" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D56" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -7948,16 +9309,42 @@
         <v>85</v>
       </c>
       <c r="F56" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G56" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H56" s="2">
         <f>VLOOKUP(F56,'BY-Demands'!$I$5:$J$65,2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="I56">
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+      <c r="K56">
+        <v>2.3569541916751464</v>
+      </c>
+    </row>
+    <row r="57" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D57" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
+        <v>IE,National</v>
+      </c>
+      <c r="E57" t="s">
+        <v>85</v>
+      </c>
+      <c r="F57" t="s">
+        <v>188</v>
+      </c>
+      <c r="G57" t="s">
+        <v>189</v>
+      </c>
+      <c r="H57" s="2">
+        <f>VLOOKUP(F57,'BY-Demands'!$I$5:$J$65,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
+      <c r="K57">
         <v>1.9849635477078642</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Include intensity change in the LED scenario
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_Demands_LED.xlsx
+++ b/SuppXLS/Scen_SYS_Demands_LED.xlsx
@@ -5,18 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A03B6E-5DC3-473F-8F4B-122B5C68F09B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3936600B-22EE-4D29-AF31-DFC1182F110D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BY-Demands" sheetId="5" r:id="rId1"/>
     <sheet name="REG_TRA_DEMANDS" sheetId="6" r:id="rId2"/>
     <sheet name="Regions" sheetId="7" r:id="rId3"/>
     <sheet name="DEMANDS" sheetId="1" r:id="rId4"/>
+    <sheet name="Residential" sheetId="8" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" localSheetId="0" hidden="1">#REF!</definedName>
@@ -83,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="200">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -675,17 +676,46 @@
   <si>
     <t>~TFM_INS-TS</t>
   </si>
+  <si>
+    <t>~TFM_INS</t>
+  </si>
+  <si>
+    <t>Pset_PN</t>
+  </si>
+  <si>
+    <t>Other_indexes</t>
+  </si>
+  <si>
+    <t>*Unit</t>
+  </si>
+  <si>
+    <t>INPUT</t>
+  </si>
+  <si>
+    <t>PJ/000 dwelling</t>
+  </si>
+  <si>
+    <t>Pset_CI</t>
+  </si>
+  <si>
+    <t>*N*</t>
+  </si>
+  <si>
+    <t>*,-*N*</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0E+00"/>
+    <numFmt numFmtId="167" formatCode="\Te\x\t"/>
+    <numFmt numFmtId="168" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -773,8 +803,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -817,8 +867,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF1F497D"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD8E3F4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -885,12 +953,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="7">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -926,8 +1026,24 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="13" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Attrib" xfId="2" xr:uid="{16EBE39D-6598-42BD-A97C-1EF313EA2EC2}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{B46BF257-55DB-413D-9B8E-80136AD91CC6}"/>
   </cellStyles>
@@ -4765,8 +4881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCA64845-990F-4F8F-9F7F-F4DBD3794313}">
   <dimension ref="B2:AF21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7765,8 +7881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:Q57"/>
   <sheetViews>
-    <sheetView topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8395,7 +8511,7 @@
         <v>4.4094344637268001</v>
       </c>
       <c r="K22">
-        <f t="shared" ref="K22:K28" si="0">H22</f>
+        <f t="shared" ref="K22:K25" si="0">H22</f>
         <v>3.5132998087277199</v>
       </c>
       <c r="O22" s="2"/>
@@ -8515,8 +8631,7 @@
         <v>225.3003382</v>
       </c>
       <c r="K26">
-        <f t="shared" si="0"/>
-        <v>206.79888500000001</v>
+        <v>740.74997310000003</v>
       </c>
       <c r="O26" s="2"/>
     </row>
@@ -8545,8 +8660,7 @@
         <v>788.3008562</v>
       </c>
       <c r="K27">
-        <f t="shared" si="0"/>
-        <v>766.351721</v>
+        <v>1244.336665</v>
       </c>
       <c r="O27" s="2"/>
     </row>
@@ -8575,8 +8689,7 @@
         <v>739.68368569999996</v>
       </c>
       <c r="K28">
-        <f t="shared" si="0"/>
-        <v>724.42972899999995</v>
+        <v>1047.9469349999999</v>
       </c>
       <c r="O28" s="2"/>
     </row>
@@ -8605,11 +8718,11 @@
       </c>
       <c r="O29" s="2"/>
       <c r="P29" t="str">
-        <f>IF(P66&lt;&gt;"",P66*$H29,"")</f>
+        <f t="shared" ref="P29:P39" si="1">IF(P66&lt;&gt;"",P66*$H29,"")</f>
         <v/>
       </c>
       <c r="Q29" t="str">
-        <f t="shared" ref="Q29" si="1">IF(Q66&lt;&gt;"",Q66*$H29,"")</f>
+        <f t="shared" ref="Q29" si="2">IF(Q66&lt;&gt;"",Q66*$H29,"")</f>
         <v/>
       </c>
     </row>
@@ -8638,11 +8751,11 @@
       </c>
       <c r="O30" s="2"/>
       <c r="P30" t="str">
-        <f>IF(P67&lt;&gt;"",P67*$H30,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q30" t="str">
-        <f>IF(Q67&lt;&gt;"",Q67*$H30,"")</f>
+        <f t="shared" ref="Q30:Q39" si="3">IF(Q67&lt;&gt;"",Q67*$H30,"")</f>
         <v/>
       </c>
     </row>
@@ -8671,11 +8784,11 @@
       </c>
       <c r="O31" s="2"/>
       <c r="P31" t="str">
-        <f>IF(P68&lt;&gt;"",P68*$H31,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q31" t="str">
-        <f>IF(Q68&lt;&gt;"",Q68*$H31,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -8704,11 +8817,11 @@
       </c>
       <c r="O32" s="2"/>
       <c r="P32" t="str">
-        <f>IF(P69&lt;&gt;"",P69*$H32,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q32" t="str">
-        <f>IF(Q69&lt;&gt;"",Q69*$H32,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -8737,11 +8850,11 @@
       </c>
       <c r="O33" s="2"/>
       <c r="P33" t="str">
-        <f>IF(P70&lt;&gt;"",P70*$H33,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q33" t="str">
-        <f>IF(Q70&lt;&gt;"",Q70*$H33,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -8770,11 +8883,11 @@
       </c>
       <c r="O34" s="2"/>
       <c r="P34" t="str">
-        <f>IF(P71&lt;&gt;"",P71*$H34,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q34" t="str">
-        <f>IF(Q71&lt;&gt;"",Q71*$H34,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -8803,11 +8916,11 @@
       </c>
       <c r="O35" s="2"/>
       <c r="P35" t="str">
-        <f>IF(P72&lt;&gt;"",P72*$H35,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q35" t="str">
-        <f>IF(Q72&lt;&gt;"",Q72*$H35,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -8836,11 +8949,11 @@
       </c>
       <c r="O36" s="2"/>
       <c r="P36" t="str">
-        <f>IF(P73&lt;&gt;"",P73*$H36,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q36" t="str">
-        <f>IF(Q73&lt;&gt;"",Q73*$H36,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -8869,11 +8982,11 @@
       </c>
       <c r="O37" s="2"/>
       <c r="P37" t="str">
-        <f>IF(P74&lt;&gt;"",P74*$H37,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q37" t="str">
-        <f>IF(Q74&lt;&gt;"",Q74*$H37,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -8902,11 +9015,11 @@
       </c>
       <c r="O38" s="2"/>
       <c r="P38" t="str">
-        <f>IF(P75&lt;&gt;"",P75*$H38,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q38" t="str">
-        <f>IF(Q75&lt;&gt;"",Q75*$H38,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -8935,11 +9048,11 @@
       </c>
       <c r="O39" s="2"/>
       <c r="P39" t="str">
-        <f>IF(P76&lt;&gt;"",P76*$H39,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q39" t="str">
-        <f>IF(Q76&lt;&gt;"",Q76*$H39,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -9351,4 +9464,1163 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1E982DE-1A8D-4D0C-9CD3-51B0DFFDA372}">
+  <dimension ref="C4:N51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="14.7109375" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+    </row>
+    <row r="5" spans="3:14" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="C5" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="G5" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="H5" s="30" t="str">
+        <f>IF(Regions!D5&lt;&gt;"",Regions!D5,"*")</f>
+        <v>National</v>
+      </c>
+      <c r="I5" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" s="30" t="s">
+        <v>197</v>
+      </c>
+      <c r="K5" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="L5" s="30" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="6" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C6" s="31" t="s">
+        <v>194</v>
+      </c>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31" t="s">
+        <v>196</v>
+      </c>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="N6" s="33"/>
+    </row>
+    <row r="7" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" t="s">
+        <v>195</v>
+      </c>
+      <c r="F7" s="36">
+        <v>2020</v>
+      </c>
+      <c r="G7" s="34">
+        <v>1.6534164675637491E-2</v>
+      </c>
+      <c r="H7" s="34">
+        <v>1.6534164675637491E-2</v>
+      </c>
+      <c r="I7" t="s">
+        <v>160</v>
+      </c>
+      <c r="J7" t="s">
+        <v>160</v>
+      </c>
+      <c r="K7" t="s">
+        <v>199</v>
+      </c>
+      <c r="L7" s="32"/>
+    </row>
+    <row r="8" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" t="s">
+        <v>195</v>
+      </c>
+      <c r="F8" s="36">
+        <v>2020</v>
+      </c>
+      <c r="G8" s="34">
+        <v>2.9990596485367418E-2</v>
+      </c>
+      <c r="H8" s="34">
+        <v>2.9990596485367418E-2</v>
+      </c>
+      <c r="I8" t="s">
+        <v>162</v>
+      </c>
+      <c r="J8" t="s">
+        <v>162</v>
+      </c>
+      <c r="K8" t="s">
+        <v>199</v>
+      </c>
+      <c r="L8" s="32"/>
+    </row>
+    <row r="9" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" t="s">
+        <v>195</v>
+      </c>
+      <c r="F9" s="36">
+        <v>2020</v>
+      </c>
+      <c r="G9" s="34">
+        <v>5.2849616307060754E-2</v>
+      </c>
+      <c r="H9" s="34">
+        <v>5.2849616307060754E-2</v>
+      </c>
+      <c r="I9" t="s">
+        <v>164</v>
+      </c>
+      <c r="J9" t="s">
+        <v>164</v>
+      </c>
+      <c r="K9" t="s">
+        <v>199</v>
+      </c>
+      <c r="L9" s="32"/>
+    </row>
+    <row r="10" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" t="s">
+        <v>195</v>
+      </c>
+      <c r="F10" s="36">
+        <v>2020</v>
+      </c>
+      <c r="G10" s="34">
+        <v>0</v>
+      </c>
+      <c r="H10" s="34">
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>166</v>
+      </c>
+      <c r="J10" t="s">
+        <v>166</v>
+      </c>
+      <c r="K10" t="s">
+        <v>199</v>
+      </c>
+      <c r="L10" s="32"/>
+    </row>
+    <row r="11" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" t="s">
+        <v>195</v>
+      </c>
+      <c r="F11" s="36">
+        <v>2020</v>
+      </c>
+      <c r="G11" s="34">
+        <v>0</v>
+      </c>
+      <c r="H11" s="34">
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>168</v>
+      </c>
+      <c r="J11" t="s">
+        <v>168</v>
+      </c>
+      <c r="K11" t="s">
+        <v>199</v>
+      </c>
+      <c r="L11" s="32"/>
+    </row>
+    <row r="12" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" t="s">
+        <v>195</v>
+      </c>
+      <c r="F12" s="36">
+        <v>2020</v>
+      </c>
+      <c r="G12" s="34">
+        <v>0</v>
+      </c>
+      <c r="H12" s="34">
+        <v>0</v>
+      </c>
+      <c r="I12" t="s">
+        <v>170</v>
+      </c>
+      <c r="J12" t="s">
+        <v>170</v>
+      </c>
+      <c r="K12" t="s">
+        <v>199</v>
+      </c>
+      <c r="L12" s="32"/>
+    </row>
+    <row r="13" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" t="s">
+        <v>195</v>
+      </c>
+      <c r="F13" s="36">
+        <v>2020</v>
+      </c>
+      <c r="G13" s="34">
+        <v>1.3128101846771158E-2</v>
+      </c>
+      <c r="H13" s="34">
+        <v>1.3128101846771158E-2</v>
+      </c>
+      <c r="I13" t="s">
+        <v>172</v>
+      </c>
+      <c r="J13" t="s">
+        <v>172</v>
+      </c>
+      <c r="K13" t="s">
+        <v>199</v>
+      </c>
+      <c r="L13" s="32"/>
+    </row>
+    <row r="14" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" t="s">
+        <v>195</v>
+      </c>
+      <c r="F14" s="36">
+        <v>2020</v>
+      </c>
+      <c r="G14" s="34">
+        <v>1.0994534987992988E-2</v>
+      </c>
+      <c r="H14" s="34">
+        <v>1.0994534987992988E-2</v>
+      </c>
+      <c r="I14" t="s">
+        <v>174</v>
+      </c>
+      <c r="J14" t="s">
+        <v>174</v>
+      </c>
+      <c r="K14" t="s">
+        <v>199</v>
+      </c>
+      <c r="L14" s="32"/>
+    </row>
+    <row r="15" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" t="s">
+        <v>195</v>
+      </c>
+      <c r="F15" s="36">
+        <v>2020</v>
+      </c>
+      <c r="G15" s="34">
+        <v>1.4648486376153701E-2</v>
+      </c>
+      <c r="H15" s="34">
+        <v>1.4648486376153701E-2</v>
+      </c>
+      <c r="I15" t="s">
+        <v>176</v>
+      </c>
+      <c r="J15" t="s">
+        <v>176</v>
+      </c>
+      <c r="K15" t="s">
+        <v>199</v>
+      </c>
+      <c r="L15" s="32"/>
+    </row>
+    <row r="16" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" t="s">
+        <v>195</v>
+      </c>
+      <c r="F16" s="36">
+        <v>2020</v>
+      </c>
+      <c r="G16" s="34">
+        <v>6.4458708104453747E-4</v>
+      </c>
+      <c r="H16" s="34">
+        <v>6.4458708104453747E-4</v>
+      </c>
+      <c r="I16" t="s">
+        <v>178</v>
+      </c>
+      <c r="J16" t="s">
+        <v>178</v>
+      </c>
+      <c r="K16" t="s">
+        <v>199</v>
+      </c>
+      <c r="L16" s="32"/>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" t="s">
+        <v>195</v>
+      </c>
+      <c r="F17" s="36">
+        <v>2020</v>
+      </c>
+      <c r="G17" s="34">
+        <v>9.1487081392159866E-4</v>
+      </c>
+      <c r="H17" s="34">
+        <v>9.1487081392159866E-4</v>
+      </c>
+      <c r="I17" t="s">
+        <v>180</v>
+      </c>
+      <c r="J17" t="s">
+        <v>180</v>
+      </c>
+      <c r="K17" t="s">
+        <v>199</v>
+      </c>
+      <c r="L17" s="32"/>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" t="s">
+        <v>195</v>
+      </c>
+      <c r="F18" s="36">
+        <v>2020</v>
+      </c>
+      <c r="G18" s="34">
+        <v>1.5069837916185766E-3</v>
+      </c>
+      <c r="H18" s="34">
+        <v>1.5069837916185766E-3</v>
+      </c>
+      <c r="I18" t="s">
+        <v>182</v>
+      </c>
+      <c r="J18" t="s">
+        <v>182</v>
+      </c>
+      <c r="K18" t="s">
+        <v>199</v>
+      </c>
+      <c r="L18" s="32"/>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" t="s">
+        <v>195</v>
+      </c>
+      <c r="F19" s="36">
+        <v>2020</v>
+      </c>
+      <c r="G19" s="34">
+        <v>1.9923424990874787E-4</v>
+      </c>
+      <c r="H19" s="34">
+        <v>1.9923424990874787E-4</v>
+      </c>
+      <c r="I19" t="s">
+        <v>184</v>
+      </c>
+      <c r="J19" t="s">
+        <v>184</v>
+      </c>
+      <c r="K19" t="s">
+        <v>199</v>
+      </c>
+      <c r="L19" s="32"/>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" t="s">
+        <v>195</v>
+      </c>
+      <c r="F20" s="36">
+        <v>2020</v>
+      </c>
+      <c r="G20" s="34">
+        <v>3.8001436556751221E-4</v>
+      </c>
+      <c r="H20" s="34">
+        <v>3.8001436556751221E-4</v>
+      </c>
+      <c r="I20" t="s">
+        <v>186</v>
+      </c>
+      <c r="J20" t="s">
+        <v>186</v>
+      </c>
+      <c r="K20" t="s">
+        <v>199</v>
+      </c>
+      <c r="L20" s="32"/>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" t="s">
+        <v>195</v>
+      </c>
+      <c r="F21" s="36">
+        <v>2020</v>
+      </c>
+      <c r="G21" s="34">
+        <v>4.7050395502371922E-4</v>
+      </c>
+      <c r="H21" s="34">
+        <v>4.7050395502371922E-4</v>
+      </c>
+      <c r="I21" t="s">
+        <v>188</v>
+      </c>
+      <c r="J21" t="s">
+        <v>188</v>
+      </c>
+      <c r="K21" t="s">
+        <v>199</v>
+      </c>
+      <c r="L21" s="32"/>
+    </row>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>195</v>
+      </c>
+      <c r="F22">
+        <v>2050</v>
+      </c>
+      <c r="G22" s="35">
+        <v>9.0742204224041785E-3</v>
+      </c>
+      <c r="H22">
+        <v>9.0742204224041785E-3</v>
+      </c>
+      <c r="I22" t="s">
+        <v>160</v>
+      </c>
+      <c r="J22" t="s">
+        <v>160</v>
+      </c>
+      <c r="K22" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="23" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>195</v>
+      </c>
+      <c r="F23">
+        <v>2050</v>
+      </c>
+      <c r="G23" s="35">
+        <v>9.0742204224041785E-3</v>
+      </c>
+      <c r="H23">
+        <v>9.0742204224041785E-3</v>
+      </c>
+      <c r="I23" t="s">
+        <v>162</v>
+      </c>
+      <c r="J23" t="s">
+        <v>162</v>
+      </c>
+      <c r="K23" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="24" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>195</v>
+      </c>
+      <c r="F24">
+        <v>2050</v>
+      </c>
+      <c r="G24" s="35">
+        <v>9.0742204224041785E-3</v>
+      </c>
+      <c r="H24">
+        <v>9.0742204224041785E-3</v>
+      </c>
+      <c r="I24" t="s">
+        <v>164</v>
+      </c>
+      <c r="J24" t="s">
+        <v>164</v>
+      </c>
+      <c r="K24" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="25" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>195</v>
+      </c>
+      <c r="F25">
+        <v>2050</v>
+      </c>
+      <c r="G25" s="35">
+        <v>1.6186055838098693E-4</v>
+      </c>
+      <c r="H25">
+        <v>1.6186055838098693E-4</v>
+      </c>
+      <c r="I25" t="s">
+        <v>166</v>
+      </c>
+      <c r="J25" t="s">
+        <v>166</v>
+      </c>
+      <c r="K25" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="26" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>195</v>
+      </c>
+      <c r="F26">
+        <v>2050</v>
+      </c>
+      <c r="G26" s="35">
+        <v>1.6186055838098693E-4</v>
+      </c>
+      <c r="H26">
+        <v>1.6186055838098693E-4</v>
+      </c>
+      <c r="I26" t="s">
+        <v>168</v>
+      </c>
+      <c r="J26" t="s">
+        <v>168</v>
+      </c>
+      <c r="K26" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="27" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>195</v>
+      </c>
+      <c r="F27">
+        <v>2050</v>
+      </c>
+      <c r="G27" s="35">
+        <v>1.6186055838098693E-4</v>
+      </c>
+      <c r="H27">
+        <v>1.6186055838098693E-4</v>
+      </c>
+      <c r="I27" t="s">
+        <v>170</v>
+      </c>
+      <c r="J27" t="s">
+        <v>170</v>
+      </c>
+      <c r="K27" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="28" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>195</v>
+      </c>
+      <c r="F28">
+        <v>2050</v>
+      </c>
+      <c r="G28" s="35">
+        <v>4.809072736236774E-3</v>
+      </c>
+      <c r="H28">
+        <v>4.809072736236774E-3</v>
+      </c>
+      <c r="I28" t="s">
+        <v>172</v>
+      </c>
+      <c r="J28" t="s">
+        <v>172</v>
+      </c>
+      <c r="K28" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="29" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>195</v>
+      </c>
+      <c r="F29">
+        <v>2050</v>
+      </c>
+      <c r="G29" s="35">
+        <v>4.809072736236774E-3</v>
+      </c>
+      <c r="H29">
+        <v>4.809072736236774E-3</v>
+      </c>
+      <c r="I29" t="s">
+        <v>174</v>
+      </c>
+      <c r="J29" t="s">
+        <v>174</v>
+      </c>
+      <c r="K29" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="30" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>195</v>
+      </c>
+      <c r="F30">
+        <v>2050</v>
+      </c>
+      <c r="G30" s="35">
+        <v>4.809072736236774E-3</v>
+      </c>
+      <c r="H30">
+        <v>4.809072736236774E-3</v>
+      </c>
+      <c r="I30" t="s">
+        <v>176</v>
+      </c>
+      <c r="J30" t="s">
+        <v>176</v>
+      </c>
+      <c r="K30" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="31" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>195</v>
+      </c>
+      <c r="F31">
+        <v>2050</v>
+      </c>
+      <c r="G31" s="35">
+        <v>8.1275680236143433E-4</v>
+      </c>
+      <c r="H31">
+        <v>8.1275680236143433E-4</v>
+      </c>
+      <c r="I31" t="s">
+        <v>178</v>
+      </c>
+      <c r="J31" t="s">
+        <v>178</v>
+      </c>
+      <c r="K31" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="32" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>195</v>
+      </c>
+      <c r="F32">
+        <v>2050</v>
+      </c>
+      <c r="G32" s="35">
+        <v>8.1275680236143433E-4</v>
+      </c>
+      <c r="H32">
+        <v>8.1275680236143433E-4</v>
+      </c>
+      <c r="I32" t="s">
+        <v>180</v>
+      </c>
+      <c r="J32" t="s">
+        <v>180</v>
+      </c>
+      <c r="K32" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="33" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>195</v>
+      </c>
+      <c r="F33">
+        <v>2050</v>
+      </c>
+      <c r="G33" s="35">
+        <v>8.1275680236143433E-4</v>
+      </c>
+      <c r="H33">
+        <v>8.1275680236143433E-4</v>
+      </c>
+      <c r="I33" t="s">
+        <v>182</v>
+      </c>
+      <c r="J33" t="s">
+        <v>182</v>
+      </c>
+      <c r="K33" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="34" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>195</v>
+      </c>
+      <c r="F34">
+        <v>2050</v>
+      </c>
+      <c r="G34" s="35">
+        <v>1.2671242344959102E-3</v>
+      </c>
+      <c r="H34">
+        <v>1.2671242344959102E-3</v>
+      </c>
+      <c r="I34" t="s">
+        <v>184</v>
+      </c>
+      <c r="J34" t="s">
+        <v>184</v>
+      </c>
+      <c r="K34" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="35" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>195</v>
+      </c>
+      <c r="F35">
+        <v>2050</v>
+      </c>
+      <c r="G35" s="35">
+        <v>1.2671242344959102E-3</v>
+      </c>
+      <c r="H35">
+        <v>1.2671242344959102E-3</v>
+      </c>
+      <c r="I35" t="s">
+        <v>186</v>
+      </c>
+      <c r="J35" t="s">
+        <v>186</v>
+      </c>
+      <c r="K35" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="36" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>195</v>
+      </c>
+      <c r="F36">
+        <v>2050</v>
+      </c>
+      <c r="G36" s="35">
+        <v>1.2671242344959102E-3</v>
+      </c>
+      <c r="H36">
+        <v>1.2671242344959102E-3</v>
+      </c>
+      <c r="I36" t="s">
+        <v>188</v>
+      </c>
+      <c r="J36" t="s">
+        <v>188</v>
+      </c>
+      <c r="K36" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="37" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>195</v>
+      </c>
+      <c r="F37">
+        <v>2050</v>
+      </c>
+      <c r="G37" s="35">
+        <v>4.4902665035151208E-3</v>
+      </c>
+      <c r="H37">
+        <v>4.4902665035151208E-3</v>
+      </c>
+      <c r="I37" t="s">
+        <v>160</v>
+      </c>
+      <c r="J37" t="s">
+        <v>160</v>
+      </c>
+      <c r="K37" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="38" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>195</v>
+      </c>
+      <c r="F38">
+        <v>2050</v>
+      </c>
+      <c r="G38" s="35">
+        <v>4.4902665035151208E-3</v>
+      </c>
+      <c r="H38">
+        <v>4.4902665035151208E-3</v>
+      </c>
+      <c r="I38" t="s">
+        <v>162</v>
+      </c>
+      <c r="J38" t="s">
+        <v>162</v>
+      </c>
+      <c r="K38" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="39" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
+        <v>195</v>
+      </c>
+      <c r="F39">
+        <v>2050</v>
+      </c>
+      <c r="G39" s="35">
+        <v>4.4902665035151208E-3</v>
+      </c>
+      <c r="H39">
+        <v>4.4902665035151208E-3</v>
+      </c>
+      <c r="I39" t="s">
+        <v>164</v>
+      </c>
+      <c r="J39" t="s">
+        <v>164</v>
+      </c>
+      <c r="K39" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="40" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>195</v>
+      </c>
+      <c r="F40">
+        <v>2050</v>
+      </c>
+      <c r="G40" s="35">
+        <v>8.0094708934328203E-5</v>
+      </c>
+      <c r="H40">
+        <v>8.0094708934328203E-5</v>
+      </c>
+      <c r="I40" t="s">
+        <v>166</v>
+      </c>
+      <c r="J40" t="s">
+        <v>166</v>
+      </c>
+      <c r="K40" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="41" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E41" t="s">
+        <v>195</v>
+      </c>
+      <c r="F41">
+        <v>2050</v>
+      </c>
+      <c r="G41" s="35">
+        <v>8.0094708934328203E-5</v>
+      </c>
+      <c r="H41">
+        <v>8.0094708934328203E-5</v>
+      </c>
+      <c r="I41" t="s">
+        <v>168</v>
+      </c>
+      <c r="J41" t="s">
+        <v>168</v>
+      </c>
+      <c r="K41" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="42" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
+        <v>195</v>
+      </c>
+      <c r="F42">
+        <v>2050</v>
+      </c>
+      <c r="G42" s="35">
+        <v>8.0094708934328203E-5</v>
+      </c>
+      <c r="H42">
+        <v>8.0094708934328203E-5</v>
+      </c>
+      <c r="I42" t="s">
+        <v>170</v>
+      </c>
+      <c r="J42" t="s">
+        <v>170</v>
+      </c>
+      <c r="K42" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="43" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E43" t="s">
+        <v>195</v>
+      </c>
+      <c r="F43">
+        <v>2050</v>
+      </c>
+      <c r="G43" s="35">
+        <v>2.379710566339819E-3</v>
+      </c>
+      <c r="H43">
+        <v>2.379710566339819E-3</v>
+      </c>
+      <c r="I43" t="s">
+        <v>172</v>
+      </c>
+      <c r="J43" t="s">
+        <v>172</v>
+      </c>
+      <c r="K43" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="44" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>195</v>
+      </c>
+      <c r="F44">
+        <v>2050</v>
+      </c>
+      <c r="G44" s="35">
+        <v>2.379710566339819E-3</v>
+      </c>
+      <c r="H44">
+        <v>2.379710566339819E-3</v>
+      </c>
+      <c r="I44" t="s">
+        <v>174</v>
+      </c>
+      <c r="J44" t="s">
+        <v>174</v>
+      </c>
+      <c r="K44" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="45" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
+        <v>195</v>
+      </c>
+      <c r="F45">
+        <v>2050</v>
+      </c>
+      <c r="G45" s="35">
+        <v>2.379710566339819E-3</v>
+      </c>
+      <c r="H45">
+        <v>2.379710566339819E-3</v>
+      </c>
+      <c r="I45" t="s">
+        <v>176</v>
+      </c>
+      <c r="J45" t="s">
+        <v>176</v>
+      </c>
+      <c r="K45" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="46" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
+        <v>195</v>
+      </c>
+      <c r="F46">
+        <v>2050</v>
+      </c>
+      <c r="G46" s="35">
+        <v>4.0218271931515297E-4</v>
+      </c>
+      <c r="H46">
+        <v>4.0218271931515297E-4</v>
+      </c>
+      <c r="I46" t="s">
+        <v>178</v>
+      </c>
+      <c r="J46" t="s">
+        <v>178</v>
+      </c>
+      <c r="K46" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="47" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E47" t="s">
+        <v>195</v>
+      </c>
+      <c r="F47">
+        <v>2050</v>
+      </c>
+      <c r="G47" s="35">
+        <v>4.0218271931515297E-4</v>
+      </c>
+      <c r="H47">
+        <v>4.0218271931515297E-4</v>
+      </c>
+      <c r="I47" t="s">
+        <v>180</v>
+      </c>
+      <c r="J47" t="s">
+        <v>180</v>
+      </c>
+      <c r="K47" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="48" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E48" t="s">
+        <v>195</v>
+      </c>
+      <c r="F48">
+        <v>2050</v>
+      </c>
+      <c r="G48" s="35">
+        <v>4.0218271931515297E-4</v>
+      </c>
+      <c r="H48">
+        <v>4.0218271931515297E-4</v>
+      </c>
+      <c r="I48" t="s">
+        <v>182</v>
+      </c>
+      <c r="J48" t="s">
+        <v>182</v>
+      </c>
+      <c r="K48" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="49" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E49" t="s">
+        <v>195</v>
+      </c>
+      <c r="F49">
+        <v>2050</v>
+      </c>
+      <c r="G49" s="35">
+        <v>6.2702086141761969E-4</v>
+      </c>
+      <c r="H49">
+        <v>6.2702086141761969E-4</v>
+      </c>
+      <c r="I49" t="s">
+        <v>184</v>
+      </c>
+      <c r="J49" t="s">
+        <v>184</v>
+      </c>
+      <c r="K49" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="50" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E50" t="s">
+        <v>195</v>
+      </c>
+      <c r="F50">
+        <v>2050</v>
+      </c>
+      <c r="G50" s="35">
+        <v>6.2702086141761969E-4</v>
+      </c>
+      <c r="H50">
+        <v>6.2702086141761969E-4</v>
+      </c>
+      <c r="I50" t="s">
+        <v>186</v>
+      </c>
+      <c r="J50" t="s">
+        <v>186</v>
+      </c>
+      <c r="K50" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="51" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E51" t="s">
+        <v>195</v>
+      </c>
+      <c r="F51">
+        <v>2050</v>
+      </c>
+      <c r="G51" s="35">
+        <v>6.2702086141761969E-4</v>
+      </c>
+      <c r="H51">
+        <v>6.2702086141761969E-4</v>
+      </c>
+      <c r="I51" t="s">
+        <v>188</v>
+      </c>
+      <c r="J51" t="s">
+        <v>188</v>
+      </c>
+      <c r="K51" t="s">
+        <v>198</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Out-comment input of cooling intensity for existing stock
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_Demands_LED.xlsx
+++ b/SuppXLS/Scen_SYS_Demands_LED.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3936600B-22EE-4D29-AF31-DFC1182F110D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{385821FF-365E-4EB6-B441-60E0C7308991}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="201">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -702,6 +702,9 @@
   </si>
   <si>
     <t>*,-*N*</t>
+  </si>
+  <si>
+    <t>*</t>
   </si>
 </sst>
 </file>
@@ -9470,8 +9473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1E982DE-1A8D-4D0C-9CD3-51B0DFFDA372}">
   <dimension ref="C4:N51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9619,7 +9622,9 @@
       <c r="L9" s="32"/>
     </row>
     <row r="10" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C10" s="32"/>
+      <c r="C10" s="32" t="s">
+        <v>200</v>
+      </c>
       <c r="D10" s="32"/>
       <c r="E10" t="s">
         <v>195</v>
@@ -9645,7 +9650,9 @@
       <c r="L10" s="32"/>
     </row>
     <row r="11" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C11" s="32"/>
+      <c r="C11" s="32" t="s">
+        <v>200</v>
+      </c>
       <c r="D11" s="32"/>
       <c r="E11" t="s">
         <v>195</v>
@@ -9671,7 +9678,9 @@
       <c r="L11" s="32"/>
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C12" s="32"/>
+      <c r="C12" s="32" t="s">
+        <v>200</v>
+      </c>
       <c r="D12" s="32"/>
       <c r="E12" t="s">
         <v>195</v>
@@ -10000,6 +10009,9 @@
       </c>
     </row>
     <row r="25" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>200</v>
+      </c>
       <c r="E25" t="s">
         <v>195</v>
       </c>
@@ -10023,6 +10035,9 @@
       </c>
     </row>
     <row r="26" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>200</v>
+      </c>
       <c r="E26" t="s">
         <v>195</v>
       </c>
@@ -10046,6 +10061,9 @@
       </c>
     </row>
     <row r="27" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>200</v>
+      </c>
       <c r="E27" t="s">
         <v>195</v>
       </c>

</xml_diff>

<commit_message>
Change fuel tourism demand to Zero in 2030
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_Demands_LED.xlsx
+++ b/SuppXLS/Scen_SYS_Demands_LED.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{385821FF-365E-4EB6-B441-60E0C7308991}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{447C6241-6F42-4E9F-BB06-F66179337899}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BY-Demands" sheetId="5" r:id="rId1"/>
@@ -1080,7 +1080,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>19050</xdr:colOff>
+          <xdr:colOff>22860</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -1395,25 +1395,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0226CF39-0357-4B21-823B-1B3093B14EE8}">
   <dimension ref="C4:AK65"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5:J65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="9.140625" style="4"/>
-    <col min="7" max="7" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="4"/>
-    <col min="9" max="9" width="11.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="6" width="9.109375" style="4"/>
+    <col min="7" max="7" width="10.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.109375" style="4"/>
+    <col min="9" max="9" width="11.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:37" x14ac:dyDescent="0.2">
+    <row r="4" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C4" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="3:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C5" s="5" t="s">
         <v>89</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="6" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C6" s="4" t="s">
         <v>92</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>0.20769618859639599</v>
       </c>
     </row>
-    <row r="7" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C7" s="4" t="s">
         <v>92</v>
       </c>
@@ -1746,7 +1746,7 @@
         <v>0.47664625412085698</v>
       </c>
     </row>
-    <row r="8" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C8" s="4" t="s">
         <v>92</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>0.42809298937083901</v>
       </c>
     </row>
-    <row r="9" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C9" s="4" t="s">
         <v>92</v>
       </c>
@@ -1944,7 +1944,7 @@
         <v>0.154582741264056</v>
       </c>
     </row>
-    <row r="10" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C10" s="4" t="s">
         <v>92</v>
       </c>
@@ -2043,7 +2043,7 @@
         <v>9.95787628254481E-2</v>
       </c>
     </row>
-    <row r="11" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C11" s="4" t="s">
         <v>92</v>
       </c>
@@ -2142,7 +2142,7 @@
         <v>4.5290536808279797E-2</v>
       </c>
     </row>
-    <row r="12" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C12" s="4" t="s">
         <v>92</v>
       </c>
@@ -2241,7 +2241,7 @@
         <v>0.28082969344526898</v>
       </c>
     </row>
-    <row r="13" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C13" s="4" t="s">
         <v>92</v>
       </c>
@@ -2340,7 +2340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C14" s="4" t="s">
         <v>92</v>
       </c>
@@ -2439,7 +2439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C15" s="4" t="s">
         <v>92</v>
       </c>
@@ -2488,7 +2488,7 @@
       <c r="AJ15" s="24"/>
       <c r="AK15" s="24"/>
     </row>
-    <row r="16" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C16" s="4" t="s">
         <v>92</v>
       </c>
@@ -2537,7 +2537,7 @@
       <c r="AJ16" s="24"/>
       <c r="AK16" s="24"/>
     </row>
-    <row r="17" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C17" s="4" t="s">
         <v>92</v>
       </c>
@@ -2586,7 +2586,7 @@
       <c r="AJ17" s="24"/>
       <c r="AK17" s="24"/>
     </row>
-    <row r="18" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C18" s="4" t="s">
         <v>92</v>
       </c>
@@ -2635,7 +2635,7 @@
       <c r="AJ18" s="24"/>
       <c r="AK18" s="24"/>
     </row>
-    <row r="19" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C19" s="4" t="s">
         <v>92</v>
       </c>
@@ -2684,7 +2684,7 @@
       <c r="AJ19" s="24"/>
       <c r="AK19" s="24"/>
     </row>
-    <row r="20" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C20" s="4" t="s">
         <v>92</v>
       </c>
@@ -2733,7 +2733,7 @@
       <c r="AJ20" s="24"/>
       <c r="AK20" s="24"/>
     </row>
-    <row r="21" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C21" s="4" t="s">
         <v>92</v>
       </c>
@@ -2782,7 +2782,7 @@
       <c r="AJ21" s="24"/>
       <c r="AK21" s="24"/>
     </row>
-    <row r="22" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C22" s="4" t="s">
         <v>92</v>
       </c>
@@ -2831,7 +2831,7 @@
       <c r="AJ22" s="24"/>
       <c r="AK22" s="24"/>
     </row>
-    <row r="23" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C23" s="4" t="s">
         <v>92</v>
       </c>
@@ -2880,7 +2880,7 @@
       <c r="AJ23" s="24"/>
       <c r="AK23" s="24"/>
     </row>
-    <row r="24" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C24" s="4" t="s">
         <v>92</v>
       </c>
@@ -2929,7 +2929,7 @@
       <c r="AJ24" s="24"/>
       <c r="AK24" s="24"/>
     </row>
-    <row r="25" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C25" s="4" t="s">
         <v>92</v>
       </c>
@@ -2978,7 +2978,7 @@
       <c r="AJ25" s="24"/>
       <c r="AK25" s="24"/>
     </row>
-    <row r="26" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C26" s="4" t="s">
         <v>92</v>
       </c>
@@ -3027,7 +3027,7 @@
       <c r="AJ26" s="24"/>
       <c r="AK26" s="24"/>
     </row>
-    <row r="27" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C27" s="4" t="s">
         <v>92</v>
       </c>
@@ -3076,7 +3076,7 @@
       <c r="AJ27" s="24"/>
       <c r="AK27" s="24"/>
     </row>
-    <row r="28" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C28" s="4" t="s">
         <v>92</v>
       </c>
@@ -3125,7 +3125,7 @@
       <c r="AJ28" s="24"/>
       <c r="AK28" s="24"/>
     </row>
-    <row r="29" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C29" s="4" t="s">
         <v>92</v>
       </c>
@@ -3174,7 +3174,7 @@
       <c r="AJ29" s="24"/>
       <c r="AK29" s="24"/>
     </row>
-    <row r="30" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C30" s="4" t="s">
         <v>92</v>
       </c>
@@ -3223,7 +3223,7 @@
       <c r="AJ30" s="24"/>
       <c r="AK30" s="24"/>
     </row>
-    <row r="31" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C31" s="4" t="s">
         <v>92</v>
       </c>
@@ -3272,7 +3272,7 @@
       <c r="AJ31" s="24"/>
       <c r="AK31" s="24"/>
     </row>
-    <row r="32" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C32" s="4" t="s">
         <v>92</v>
       </c>
@@ -3321,7 +3321,7 @@
       <c r="AJ32" s="24"/>
       <c r="AK32" s="24"/>
     </row>
-    <row r="33" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C33" s="4" t="s">
         <v>92</v>
       </c>
@@ -3370,7 +3370,7 @@
       <c r="AJ33" s="24"/>
       <c r="AK33" s="24"/>
     </row>
-    <row r="34" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C34" s="4" t="s">
         <v>92</v>
       </c>
@@ -3419,7 +3419,7 @@
       <c r="AJ34" s="24"/>
       <c r="AK34" s="24"/>
     </row>
-    <row r="35" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C35" s="4" t="s">
         <v>92</v>
       </c>
@@ -3468,7 +3468,7 @@
       <c r="AJ35" s="24"/>
       <c r="AK35" s="24"/>
     </row>
-    <row r="36" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C36" s="4" t="s">
         <v>92</v>
       </c>
@@ -3513,7 +3513,7 @@
       <c r="AJ36" s="24"/>
       <c r="AK36" s="24"/>
     </row>
-    <row r="37" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C37" s="4" t="s">
         <v>92</v>
       </c>
@@ -3562,7 +3562,7 @@
       <c r="AJ37" s="24"/>
       <c r="AK37" s="24"/>
     </row>
-    <row r="38" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C38" s="4" t="s">
         <v>92</v>
       </c>
@@ -3611,7 +3611,7 @@
       <c r="AJ38" s="24"/>
       <c r="AK38" s="24"/>
     </row>
-    <row r="39" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C39" s="4" t="s">
         <v>92</v>
       </c>
@@ -3660,7 +3660,7 @@
       <c r="AJ39" s="24"/>
       <c r="AK39" s="24"/>
     </row>
-    <row r="40" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C40" s="4" t="s">
         <v>92</v>
       </c>
@@ -3709,7 +3709,7 @@
       <c r="AJ40" s="24"/>
       <c r="AK40" s="24"/>
     </row>
-    <row r="41" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C41" s="4" t="s">
         <v>92</v>
       </c>
@@ -3758,7 +3758,7 @@
       <c r="AJ41" s="24"/>
       <c r="AK41" s="24"/>
     </row>
-    <row r="42" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C42" s="4" t="s">
         <v>92</v>
       </c>
@@ -3807,7 +3807,7 @@
       <c r="AJ42" s="24"/>
       <c r="AK42" s="24"/>
     </row>
-    <row r="43" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C43" s="4" t="s">
         <v>92</v>
       </c>
@@ -3856,7 +3856,7 @@
       <c r="AJ43" s="24"/>
       <c r="AK43" s="24"/>
     </row>
-    <row r="44" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C44" s="4" t="s">
         <v>92</v>
       </c>
@@ -3905,7 +3905,7 @@
       <c r="AJ44" s="24"/>
       <c r="AK44" s="24"/>
     </row>
-    <row r="45" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C45" s="4" t="s">
         <v>92</v>
       </c>
@@ -3954,7 +3954,7 @@
       <c r="AJ45" s="24"/>
       <c r="AK45" s="24"/>
     </row>
-    <row r="46" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C46" s="4" t="s">
         <v>92</v>
       </c>
@@ -4003,7 +4003,7 @@
       <c r="AJ46" s="24"/>
       <c r="AK46" s="24"/>
     </row>
-    <row r="47" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C47" s="4" t="s">
         <v>92</v>
       </c>
@@ -4052,7 +4052,7 @@
       <c r="AJ47" s="24"/>
       <c r="AK47" s="24"/>
     </row>
-    <row r="48" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C48" s="4" t="s">
         <v>92</v>
       </c>
@@ -4101,7 +4101,7 @@
       <c r="AJ48" s="24"/>
       <c r="AK48" s="24"/>
     </row>
-    <row r="49" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C49" s="4" t="s">
         <v>92</v>
       </c>
@@ -4150,7 +4150,7 @@
       <c r="AJ49" s="24"/>
       <c r="AK49" s="24"/>
     </row>
-    <row r="50" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C50" s="4" t="s">
         <v>92</v>
       </c>
@@ -4199,7 +4199,7 @@
       <c r="AJ50" s="24"/>
       <c r="AK50" s="24"/>
     </row>
-    <row r="51" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C51" s="4" t="s">
         <v>92</v>
       </c>
@@ -4244,7 +4244,7 @@
       <c r="AJ51" s="24"/>
       <c r="AK51" s="24"/>
     </row>
-    <row r="52" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C52" s="4" t="s">
         <v>92</v>
       </c>
@@ -4289,7 +4289,7 @@
       <c r="AJ52" s="24"/>
       <c r="AK52" s="24"/>
     </row>
-    <row r="53" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C53" s="4" t="s">
         <v>92</v>
       </c>
@@ -4334,7 +4334,7 @@
       <c r="AJ53" s="24"/>
       <c r="AK53" s="24"/>
     </row>
-    <row r="54" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C54" s="4" t="s">
         <v>92</v>
       </c>
@@ -4379,7 +4379,7 @@
       <c r="AJ54" s="24"/>
       <c r="AK54" s="24"/>
     </row>
-    <row r="55" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C55" s="4" t="s">
         <v>92</v>
       </c>
@@ -4424,7 +4424,7 @@
       <c r="AJ55" s="24"/>
       <c r="AK55" s="24"/>
     </row>
-    <row r="56" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C56" s="4" t="s">
         <v>92</v>
       </c>
@@ -4469,7 +4469,7 @@
       <c r="AJ56" s="24"/>
       <c r="AK56" s="24"/>
     </row>
-    <row r="57" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C57" s="4" t="s">
         <v>92</v>
       </c>
@@ -4514,7 +4514,7 @@
       <c r="AJ57" s="24"/>
       <c r="AK57" s="24"/>
     </row>
-    <row r="58" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C58" s="4" t="s">
         <v>92</v>
       </c>
@@ -4559,7 +4559,7 @@
       <c r="AJ58" s="24"/>
       <c r="AK58" s="24"/>
     </row>
-    <row r="59" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C59" s="4" t="s">
         <v>92</v>
       </c>
@@ -4604,7 +4604,7 @@
       <c r="AJ59" s="24"/>
       <c r="AK59" s="24"/>
     </row>
-    <row r="60" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C60" s="4" t="s">
         <v>92</v>
       </c>
@@ -4649,7 +4649,7 @@
       <c r="AJ60" s="24"/>
       <c r="AK60" s="24"/>
     </row>
-    <row r="61" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C61" s="4" t="s">
         <v>92</v>
       </c>
@@ -4694,7 +4694,7 @@
       <c r="AJ61" s="24"/>
       <c r="AK61" s="24"/>
     </row>
-    <row r="62" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C62" s="4" t="s">
         <v>92</v>
       </c>
@@ -4739,7 +4739,7 @@
       <c r="AJ62" s="24"/>
       <c r="AK62" s="24"/>
     </row>
-    <row r="63" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C63" s="4" t="s">
         <v>92</v>
       </c>
@@ -4784,7 +4784,7 @@
       <c r="AJ63" s="24"/>
       <c r="AK63" s="24"/>
     </row>
-    <row r="64" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C64" s="4" t="s">
         <v>92</v>
       </c>
@@ -4829,7 +4829,7 @@
       <c r="AJ64" s="24"/>
       <c r="AK64" s="24"/>
     </row>
-    <row r="65" spans="3:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C65" s="4" t="s">
         <v>92</v>
       </c>
@@ -4885,22 +4885,22 @@
   <dimension ref="B2:AF21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="G12" sqref="G12:AF12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="4"/>
-    <col min="4" max="4" width="11.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="3" width="9.109375" style="4"/>
+    <col min="4" max="4" width="11.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="2:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:32" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="14" t="s">
         <v>91</v>
       </c>
@@ -5021,7 +5021,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="4" spans="2:32" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:32" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D4" s="4" t="s">
         <v>85</v>
       </c>
@@ -5137,7 +5137,7 @@
         <v>0.15354445783325901</v>
       </c>
     </row>
-    <row r="5" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:32" x14ac:dyDescent="0.25">
       <c r="D5" s="4" t="s">
         <v>85</v>
       </c>
@@ -5253,7 +5253,7 @@
         <v>0.2713201852314594</v>
       </c>
     </row>
-    <row r="6" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:32" x14ac:dyDescent="0.25">
       <c r="D6" s="4" t="s">
         <v>85</v>
       </c>
@@ -5369,7 +5369,7 @@
         <v>0.35260315962707711</v>
       </c>
     </row>
-    <row r="7" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:32" x14ac:dyDescent="0.25">
       <c r="D7" s="4" t="s">
         <v>85</v>
       </c>
@@ -5485,7 +5485,7 @@
         <v>0.46884077905903881</v>
       </c>
     </row>
-    <row r="8" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:32" x14ac:dyDescent="0.25">
       <c r="D8" s="4" t="s">
         <v>85</v>
       </c>
@@ -5601,7 +5601,7 @@
         <v>0.31412261464919838</v>
       </c>
     </row>
-    <row r="9" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:32" x14ac:dyDescent="0.25">
       <c r="D9" s="4" t="s">
         <v>85</v>
       </c>
@@ -5717,7 +5717,7 @@
         <v>0.41709875548708081</v>
       </c>
     </row>
-    <row r="10" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:32" x14ac:dyDescent="0.25">
       <c r="D10" s="4" t="s">
         <v>85</v>
       </c>
@@ -5833,7 +5833,7 @@
         <v>0.15629751581539669</v>
       </c>
     </row>
-    <row r="11" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:32" x14ac:dyDescent="0.25">
       <c r="D11" s="4" t="s">
         <v>85</v>
       </c>
@@ -5949,7 +5949,7 @@
         <v>0.12881123700615976</v>
       </c>
     </row>
-    <row r="12" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:32" x14ac:dyDescent="0.25">
       <c r="D12" s="4" t="s">
         <v>85</v>
       </c>
@@ -5962,110 +5962,110 @@
       </c>
       <c r="G12" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.13064779508364899</v>
+        <v>0.11877072280331726</v>
       </c>
       <c r="H12" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>3.0919251481787136</v>
+        <v>2.8108410437988307</v>
       </c>
       <c r="I12" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.51060312297639665</v>
+        <v>0.46418465725126973</v>
       </c>
       <c r="J12" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.22771801450398094</v>
+        <v>0.20701637682180085</v>
       </c>
       <c r="K12" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.1943630348521006</v>
+        <v>0.17669366804736417</v>
       </c>
       <c r="L12" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>9.3795533767547012E-2</v>
+        <v>8.5268667061406372E-2</v>
       </c>
       <c r="M12" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.29576354987636128</v>
+        <v>0.26887595443305573</v>
       </c>
       <c r="N12" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.4475877985016371</v>
+        <v>0.40689799863785192</v>
       </c>
       <c r="O12" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.1789052334805798</v>
+        <v>0.16264112134598166</v>
       </c>
       <c r="P12" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.20370977252820086</v>
+        <v>0.18519070229836443</v>
       </c>
       <c r="Q12" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.3435826806631439</v>
+        <v>0.31234789151194903</v>
       </c>
       <c r="R12" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.32683749411207558</v>
+        <v>0.29712499464734149</v>
       </c>
       <c r="S12" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.27266175557601846</v>
+        <v>0.2478743232509259</v>
       </c>
       <c r="T12" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.2457757890372787</v>
+        <v>1.1325234445793442</v>
       </c>
       <c r="U12" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.33895865011628784</v>
+        <v>0.30814422737844349</v>
       </c>
       <c r="V12" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.44725505188660325</v>
+        <v>0.4065955017150939</v>
       </c>
       <c r="W12" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.3661429011624644</v>
+        <v>0.33285718287496763</v>
       </c>
       <c r="X12" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.26660117757391238</v>
+        <v>0.2423647068853749</v>
       </c>
       <c r="Y12" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.5921925929827917</v>
+        <v>0.53835690271162884</v>
       </c>
       <c r="Z12" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>7.3534707118324452E-2</v>
+        <v>6.6849733743931328E-2</v>
       </c>
       <c r="AA12" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.29948801716050255</v>
+        <v>0.27226183378227509</v>
       </c>
       <c r="AB12" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.14811584497082575</v>
+        <v>0.13465076815529611</v>
       </c>
       <c r="AC12" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.15038999597426655</v>
+        <v>0.13671817815842413</v>
       </c>
       <c r="AD12" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.17480900790929571</v>
+        <v>0.15891727991754154</v>
       </c>
       <c r="AE12" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.36531447683124091</v>
+        <v>0.33210406984658275</v>
       </c>
       <c r="AF12" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.14086885317580392</v>
-      </c>
-    </row>
-    <row r="13" spans="2:32" x14ac:dyDescent="0.2">
+        <v>0.12806259379618537</v>
+      </c>
+    </row>
+    <row r="13" spans="2:32" x14ac:dyDescent="0.25">
       <c r="D13" s="4" t="s">
         <v>85</v>
       </c>
@@ -6078,110 +6078,110 @@
       </c>
       <c r="G13" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>9.2353600579585193E-2</v>
+        <v>0</v>
       </c>
       <c r="H13" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>2.18565051154552</v>
+        <v>0</v>
       </c>
       <c r="I13" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.36094016622216002</v>
+        <v>0</v>
       </c>
       <c r="J13" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.160971553655473</v>
+        <v>0</v>
       </c>
       <c r="K13" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.13739325701343899</v>
+        <v>0</v>
       </c>
       <c r="L13" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>6.6303111018221506E-2</v>
+        <v>0</v>
       </c>
       <c r="M13" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.20907225210952099</v>
+        <v>0</v>
       </c>
       <c r="N13" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.31639527280693802</v>
+        <v>0</v>
       </c>
       <c r="O13" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.126466294083908</v>
+        <v>0</v>
       </c>
       <c r="P13" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.14400037102947</v>
+        <v>0</v>
       </c>
       <c r="Q13" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.24287511041201201</v>
+        <v>0</v>
       </c>
       <c r="R13" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.23103810796296301</v>
+        <v>0</v>
       </c>
       <c r="S13" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.19274182814699201</v>
+        <v>0</v>
       </c>
       <c r="T13" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.880626263602864</v>
+        <v>0</v>
       </c>
       <c r="U13" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.239606430141375</v>
+        <v>0</v>
       </c>
       <c r="V13" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.31616005760135901</v>
+        <v>0</v>
       </c>
       <c r="W13" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.25882270135028701</v>
+        <v>0</v>
       </c>
       <c r="X13" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.18845766705778599</v>
+        <v>0</v>
       </c>
       <c r="Y13" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.418614934630201</v>
+        <v>0</v>
       </c>
       <c r="Z13" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>5.1980938259190403E-2</v>
+        <v>0</v>
       </c>
       <c r="AA13" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.21170504023817699</v>
+        <v>0</v>
       </c>
       <c r="AB13" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.10470158778558201</v>
+        <v>0</v>
       </c>
       <c r="AC13" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.106309162052679</v>
+        <v>0</v>
       </c>
       <c r="AD13" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.12357071379453501</v>
+        <v>0</v>
       </c>
       <c r="AE13" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.25823709659708599</v>
+        <v>0</v>
       </c>
       <c r="AF13" s="15">
         <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>9.95787628254481E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="2:32" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:32" x14ac:dyDescent="0.25">
       <c r="D14" s="4" t="s">
         <v>85</v>
       </c>
@@ -6297,7 +6297,7 @@
         <v>5.6842758875006463E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:32" x14ac:dyDescent="0.25">
       <c r="D15" s="4" t="s">
         <v>85</v>
       </c>
@@ -6413,7 +6413,7 @@
         <v>4.5290536808279797E-2</v>
       </c>
     </row>
-    <row r="16" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:32" x14ac:dyDescent="0.25">
       <c r="D16" s="4" t="s">
         <v>85</v>
       </c>
@@ -6529,7 +6529,7 @@
         <v>0.17505912318297531</v>
       </c>
     </row>
-    <row r="17" spans="4:32" x14ac:dyDescent="0.2">
+    <row r="17" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D17" s="4" t="s">
         <v>85</v>
       </c>
@@ -6645,7 +6645,7 @@
         <v>0.28082969344526898</v>
       </c>
     </row>
-    <row r="18" spans="4:32" x14ac:dyDescent="0.2">
+    <row r="18" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D18" s="4" t="s">
         <v>85</v>
       </c>
@@ -6761,7 +6761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="4:32" x14ac:dyDescent="0.2">
+    <row r="19" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D19" s="4" t="s">
         <v>85</v>
       </c>
@@ -6877,7 +6877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="4:32" x14ac:dyDescent="0.2">
+    <row r="20" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D20" s="4" t="s">
         <v>85</v>
       </c>
@@ -6993,7 +6993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="4:32" x14ac:dyDescent="0.2">
+    <row r="21" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D21" s="4" t="s">
         <v>85</v>
       </c>
@@ -7122,40 +7122,40 @@
       <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="3.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="5.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.5703125" style="4" customWidth="1"/>
-    <col min="25" max="25" width="6.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="3.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.5546875" style="4" customWidth="1"/>
+    <col min="25" max="25" width="6.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.109375" style="4" bestFit="1" customWidth="1"/>
     <col min="27" max="28" width="6" style="4" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="9.140625" style="4"/>
+    <col min="29" max="29" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:30" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" ht="14.4" x14ac:dyDescent="0.25">
       <c r="C3" s="21" t="str">
         <f t="array" ref="C3">INDEX(C5:C7,$A$4)</f>
         <v>IE</v>
@@ -7269,12 +7269,12 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>159</v>
       </c>
@@ -7389,7 +7389,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>158</v>
       </c>
@@ -7506,7 +7506,7 @@
         <v>*IE-MN</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>157</v>
       </c>
@@ -7623,7 +7623,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
         <v>156</v>
       </c>
@@ -7631,7 +7631,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>102</v>
       </c>
@@ -7639,7 +7639,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>125</v>
       </c>
@@ -7647,7 +7647,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>114</v>
       </c>
@@ -7655,7 +7655,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>115</v>
       </c>
@@ -7663,7 +7663,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>126</v>
       </c>
@@ -7671,7 +7671,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>103</v>
       </c>
@@ -7679,7 +7679,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>120</v>
       </c>
@@ -7687,7 +7687,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
         <v>116</v>
       </c>
@@ -7695,7 +7695,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
         <v>104</v>
       </c>
@@ -7703,7 +7703,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
         <v>105</v>
       </c>
@@ -7711,7 +7711,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
         <v>106</v>
       </c>
@@ -7719,7 +7719,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
         <v>121</v>
       </c>
@@ -7727,7 +7727,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
         <v>117</v>
       </c>
@@ -7735,7 +7735,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
         <v>107</v>
       </c>
@@ -7743,7 +7743,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
         <v>108</v>
       </c>
@@ -7751,7 +7751,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
         <v>122</v>
       </c>
@@ -7759,7 +7759,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
         <v>109</v>
       </c>
@@ -7767,7 +7767,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
         <v>127</v>
       </c>
@@ -7775,7 +7775,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
         <v>110</v>
       </c>
@@ -7783,7 +7783,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
         <v>123</v>
       </c>
@@ -7791,7 +7791,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
         <v>124</v>
       </c>
@@ -7799,7 +7799,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
         <v>118</v>
       </c>
@@ -7807,7 +7807,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
         <v>119</v>
       </c>
@@ -7815,7 +7815,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
         <v>111</v>
       </c>
@@ -7823,7 +7823,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
         <v>112</v>
       </c>
@@ -7831,7 +7831,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
         <v>113</v>
       </c>
@@ -7839,7 +7839,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A37" s="17" t="s">
         <v>128</v>
       </c>
@@ -7865,7 +7865,7 @@
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>19050</xdr:colOff>
+                    <xdr:colOff>22860</xdr:colOff>
                     <xdr:row>3</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -7884,23 +7884,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:Q57"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="53.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.85546875" customWidth="1"/>
-    <col min="11" max="12" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="53.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.88671875" customWidth="1"/>
+    <col min="11" max="12" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
         <v>190</v>
       </c>
@@ -7908,7 +7908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C2" s="14" t="s">
         <v>1</v>
       </c>
@@ -7937,7 +7937,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="3" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:15" x14ac:dyDescent="0.3">
       <c r="D3" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -7966,7 +7966,7 @@
       </c>
       <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:15" x14ac:dyDescent="0.3">
       <c r="D4" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -7995,7 +7995,7 @@
       </c>
       <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:15" x14ac:dyDescent="0.3">
       <c r="D5" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8024,7 +8024,7 @@
       </c>
       <c r="O5" s="2"/>
     </row>
-    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:15" x14ac:dyDescent="0.3">
       <c r="D6" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8053,7 +8053,7 @@
       </c>
       <c r="O6" s="2"/>
     </row>
-    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:15" x14ac:dyDescent="0.3">
       <c r="D7" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8082,7 +8082,7 @@
       </c>
       <c r="O7" s="2"/>
     </row>
-    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:15" x14ac:dyDescent="0.3">
       <c r="D8" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8111,7 +8111,7 @@
       </c>
       <c r="O8" s="2"/>
     </row>
-    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:15" x14ac:dyDescent="0.3">
       <c r="D9" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8140,7 +8140,7 @@
       </c>
       <c r="O9" s="2"/>
     </row>
-    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:15" x14ac:dyDescent="0.3">
       <c r="D10" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8169,7 +8169,7 @@
       </c>
       <c r="O10" s="2"/>
     </row>
-    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:15" x14ac:dyDescent="0.3">
       <c r="D11" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8198,7 +8198,7 @@
       </c>
       <c r="O11" s="2"/>
     </row>
-    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:15" x14ac:dyDescent="0.3">
       <c r="D12" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8227,7 +8227,7 @@
       </c>
       <c r="O12" s="2"/>
     </row>
-    <row r="13" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:15" x14ac:dyDescent="0.3">
       <c r="D13" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8256,7 +8256,7 @@
       </c>
       <c r="O13" s="2"/>
     </row>
-    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:15" x14ac:dyDescent="0.3">
       <c r="D14" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8285,7 +8285,7 @@
       </c>
       <c r="O14" s="2"/>
     </row>
-    <row r="15" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:15" x14ac:dyDescent="0.3">
       <c r="D15" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8314,7 +8314,7 @@
       </c>
       <c r="O15" s="2"/>
     </row>
-    <row r="16" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:15" x14ac:dyDescent="0.3">
       <c r="D16" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8343,7 +8343,7 @@
       </c>
       <c r="O16" s="2"/>
     </row>
-    <row r="17" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D17" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -8372,7 +8372,7 @@
       </c>
       <c r="O17" s="2"/>
     </row>
-    <row r="18" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D18" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -8401,7 +8401,7 @@
       </c>
       <c r="O18" s="2"/>
     </row>
-    <row r="19" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -8430,7 +8430,7 @@
       </c>
       <c r="O19" s="2"/>
     </row>
-    <row r="20" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D20" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -8459,7 +8459,7 @@
       </c>
       <c r="O20" s="2"/>
     </row>
-    <row r="21" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D21" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -8481,15 +8481,14 @@
         <v>10.927548</v>
       </c>
       <c r="J21">
-        <v>10.927548</v>
+        <v>9.9341345454545458</v>
       </c>
       <c r="K21">
-        <f>H21</f>
-        <v>7.7245727925227703</v>
+        <v>0</v>
       </c>
       <c r="O21" s="2"/>
     </row>
-    <row r="22" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D22" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -8514,12 +8513,12 @@
         <v>4.4094344637268001</v>
       </c>
       <c r="K22">
-        <f t="shared" ref="K22:K25" si="0">H22</f>
+        <f>H22</f>
         <v>3.5132998087277199</v>
       </c>
       <c r="O22" s="2"/>
     </row>
-    <row r="23" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D23" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -8544,12 +8543,12 @@
         <v>13.57977245</v>
       </c>
       <c r="K23">
-        <f t="shared" si="0"/>
+        <f>H23</f>
         <v>21.784659175997099</v>
       </c>
       <c r="O23" s="2"/>
     </row>
-    <row r="24" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D24" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -8574,12 +8573,12 @@
         <v>0.23</v>
       </c>
       <c r="K24">
-        <f t="shared" si="0"/>
+        <f>H24</f>
         <v>0.23349320028657899</v>
       </c>
       <c r="O24" s="2"/>
     </row>
-    <row r="25" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D25" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -8604,12 +8603,12 @@
         <v>46.814427170000002</v>
       </c>
       <c r="K25">
-        <f t="shared" si="0"/>
+        <f>H25</f>
         <v>45.935836654432002</v>
       </c>
       <c r="O25" s="2"/>
     </row>
-    <row r="26" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D26" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8638,7 +8637,7 @@
       </c>
       <c r="O26" s="2"/>
     </row>
-    <row r="27" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D27" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8667,7 +8666,7 @@
       </c>
       <c r="O27" s="2"/>
     </row>
-    <row r="28" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D28" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8696,7 +8695,7 @@
       </c>
       <c r="O28" s="2"/>
     </row>
-    <row r="29" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D29" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8721,15 +8720,15 @@
       </c>
       <c r="O29" s="2"/>
       <c r="P29" t="str">
-        <f t="shared" ref="P29:P39" si="1">IF(P66&lt;&gt;"",P66*$H29,"")</f>
+        <f t="shared" ref="P29:P39" si="0">IF(P66&lt;&gt;"",P66*$H29,"")</f>
         <v/>
       </c>
       <c r="Q29" t="str">
-        <f t="shared" ref="Q29" si="2">IF(Q66&lt;&gt;"",Q66*$H29,"")</f>
+        <f t="shared" ref="Q29" si="1">IF(Q66&lt;&gt;"",Q66*$H29,"")</f>
         <v/>
       </c>
     </row>
-    <row r="30" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D30" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8754,15 +8753,15 @@
       </c>
       <c r="O30" s="2"/>
       <c r="P30" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="Q30" t="str">
-        <f t="shared" ref="Q30:Q39" si="3">IF(Q67&lt;&gt;"",Q67*$H30,"")</f>
+        <f t="shared" ref="Q30:Q39" si="2">IF(Q67&lt;&gt;"",Q67*$H30,"")</f>
         <v/>
       </c>
     </row>
-    <row r="31" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D31" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8787,15 +8786,15 @@
       </c>
       <c r="O31" s="2"/>
       <c r="P31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="Q31" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="32" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D32" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8820,15 +8819,15 @@
       </c>
       <c r="O32" s="2"/>
       <c r="P32" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="Q32" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="33" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D33" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8853,15 +8852,15 @@
       </c>
       <c r="O33" s="2"/>
       <c r="P33" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="Q33" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="34" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D34" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8886,15 +8885,15 @@
       </c>
       <c r="O34" s="2"/>
       <c r="P34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="Q34" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="35" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D35" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8919,15 +8918,15 @@
       </c>
       <c r="O35" s="2"/>
       <c r="P35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="Q35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="36" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D36" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8952,15 +8951,15 @@
       </c>
       <c r="O36" s="2"/>
       <c r="P36" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="Q36" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="37" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D37" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8985,15 +8984,15 @@
       </c>
       <c r="O37" s="2"/>
       <c r="P37" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="Q37" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="38" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D38" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9018,15 +9017,15 @@
       </c>
       <c r="O38" s="2"/>
       <c r="P38" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="Q38" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="39" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D39" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9051,15 +9050,15 @@
       </c>
       <c r="O39" s="2"/>
       <c r="P39" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="Q39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="40" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D40" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9083,7 +9082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D41" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9104,7 +9103,7 @@
         <v>32.865000000000002</v>
       </c>
     </row>
-    <row r="43" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D43" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9128,7 +9127,7 @@
         <v>10.047893325490021</v>
       </c>
     </row>
-    <row r="44" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D44" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9152,7 +9151,7 @@
         <v>16.878788423834521</v>
       </c>
     </row>
-    <row r="45" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D45" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9176,7 +9175,7 @@
         <v>14.214862498864701</v>
       </c>
     </row>
-    <row r="46" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D46" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9200,7 +9199,7 @@
         <v>0.179228357755223</v>
       </c>
     </row>
-    <row r="47" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D47" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9224,7 +9223,7 @@
         <v>0.30107381041032272</v>
       </c>
     </row>
-    <row r="48" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D48" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9248,7 +9247,7 @@
         <v>0.2535562807901901</v>
       </c>
     </row>
-    <row r="49" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D49" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9272,7 +9271,7 @@
         <v>5.3250910380053398</v>
       </c>
     </row>
-    <row r="50" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D50" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9296,7 +9295,7 @@
         <v>8.9452666401358414</v>
       </c>
     </row>
-    <row r="51" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D51" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9320,7 +9319,7 @@
         <v>7.5334634283143167</v>
       </c>
     </row>
-    <row r="52" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D52" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9344,7 +9343,7 @@
         <v>0.89996641800005883</v>
       </c>
     </row>
-    <row r="53" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D53" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9368,7 +9367,7 @@
         <v>1.5117937925797396</v>
       </c>
     </row>
-    <row r="54" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D54" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9392,7 +9391,7 @@
         <v>1.2731921479513455</v>
       </c>
     </row>
-    <row r="55" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D55" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9416,7 +9415,7 @@
         <v>1.4030879288454441</v>
       </c>
     </row>
-    <row r="56" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D56" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9440,7 +9439,7 @@
         <v>2.3569541916751464</v>
       </c>
     </row>
-    <row r="57" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D57" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9473,19 +9472,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1E982DE-1A8D-4D0C-9CD3-51B0DFFDA372}">
   <dimension ref="C4:N51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="14.7109375" customWidth="1"/>
-    <col min="14" max="14" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="14.6640625" customWidth="1"/>
+    <col min="14" max="14" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C4" s="28" t="s">
         <v>191</v>
       </c>
@@ -9493,7 +9492,7 @@
       <c r="J4" s="29"/>
       <c r="K4" s="29"/>
     </row>
-    <row r="5" spans="3:14" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:14" ht="26.4" x14ac:dyDescent="0.3">
       <c r="C5" s="30" t="s">
         <v>91</v>
       </c>
@@ -9526,7 +9525,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="6" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C6" s="31" t="s">
         <v>194</v>
       </c>
@@ -9543,7 +9542,7 @@
       <c r="L6" s="31"/>
       <c r="N6" s="33"/>
     </row>
-    <row r="7" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C7" s="32"/>
       <c r="D7" s="32"/>
       <c r="E7" t="s">
@@ -9569,7 +9568,7 @@
       </c>
       <c r="L7" s="32"/>
     </row>
-    <row r="8" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C8" s="32"/>
       <c r="D8" s="32"/>
       <c r="E8" t="s">
@@ -9595,7 +9594,7 @@
       </c>
       <c r="L8" s="32"/>
     </row>
-    <row r="9" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C9" s="32"/>
       <c r="D9" s="32"/>
       <c r="E9" t="s">
@@ -9621,7 +9620,7 @@
       </c>
       <c r="L9" s="32"/>
     </row>
-    <row r="10" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C10" s="32" t="s">
         <v>200</v>
       </c>
@@ -9649,7 +9648,7 @@
       </c>
       <c r="L10" s="32"/>
     </row>
-    <row r="11" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C11" s="32" t="s">
         <v>200</v>
       </c>
@@ -9677,7 +9676,7 @@
       </c>
       <c r="L11" s="32"/>
     </row>
-    <row r="12" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C12" s="32" t="s">
         <v>200</v>
       </c>
@@ -9705,7 +9704,7 @@
       </c>
       <c r="L12" s="32"/>
     </row>
-    <row r="13" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C13" s="32"/>
       <c r="D13" s="32"/>
       <c r="E13" t="s">
@@ -9731,7 +9730,7 @@
       </c>
       <c r="L13" s="32"/>
     </row>
-    <row r="14" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C14" s="32"/>
       <c r="D14" s="32"/>
       <c r="E14" t="s">
@@ -9757,7 +9756,7 @@
       </c>
       <c r="L14" s="32"/>
     </row>
-    <row r="15" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C15" s="32"/>
       <c r="D15" s="32"/>
       <c r="E15" t="s">
@@ -9783,7 +9782,7 @@
       </c>
       <c r="L15" s="32"/>
     </row>
-    <row r="16" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C16" s="32"/>
       <c r="D16" s="32"/>
       <c r="E16" t="s">
@@ -9809,7 +9808,7 @@
       </c>
       <c r="L16" s="32"/>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C17" s="32"/>
       <c r="D17" s="32"/>
       <c r="E17" t="s">
@@ -9835,7 +9834,7 @@
       </c>
       <c r="L17" s="32"/>
     </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C18" s="32"/>
       <c r="D18" s="32"/>
       <c r="E18" t="s">
@@ -9861,7 +9860,7 @@
       </c>
       <c r="L18" s="32"/>
     </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C19" s="32"/>
       <c r="D19" s="32"/>
       <c r="E19" t="s">
@@ -9887,7 +9886,7 @@
       </c>
       <c r="L19" s="32"/>
     </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C20" s="32"/>
       <c r="D20" s="32"/>
       <c r="E20" t="s">
@@ -9913,7 +9912,7 @@
       </c>
       <c r="L20" s="32"/>
     </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C21" s="32"/>
       <c r="D21" s="32"/>
       <c r="E21" t="s">
@@ -9939,7 +9938,7 @@
       </c>
       <c r="L21" s="32"/>
     </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:12" x14ac:dyDescent="0.3">
       <c r="E22" t="s">
         <v>195</v>
       </c>
@@ -9962,7 +9961,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:12" x14ac:dyDescent="0.3">
       <c r="E23" t="s">
         <v>195</v>
       </c>
@@ -9985,7 +9984,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:12" x14ac:dyDescent="0.3">
       <c r="E24" t="s">
         <v>195</v>
       </c>
@@ -10008,7 +10007,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="25" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
         <v>200</v>
       </c>
@@ -10034,7 +10033,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="26" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
         <v>200</v>
       </c>
@@ -10060,7 +10059,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="27" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
         <v>200</v>
       </c>
@@ -10086,7 +10085,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="28" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:12" x14ac:dyDescent="0.3">
       <c r="E28" t="s">
         <v>195</v>
       </c>
@@ -10109,7 +10108,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="29" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:12" x14ac:dyDescent="0.3">
       <c r="E29" t="s">
         <v>195</v>
       </c>
@@ -10132,7 +10131,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="30" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:12" x14ac:dyDescent="0.3">
       <c r="E30" t="s">
         <v>195</v>
       </c>
@@ -10155,7 +10154,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="31" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:12" x14ac:dyDescent="0.3">
       <c r="E31" t="s">
         <v>195</v>
       </c>
@@ -10178,7 +10177,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="32" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:12" x14ac:dyDescent="0.3">
       <c r="E32" t="s">
         <v>195</v>
       </c>
@@ -10201,7 +10200,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="33" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E33" t="s">
         <v>195</v>
       </c>
@@ -10224,7 +10223,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="34" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E34" t="s">
         <v>195</v>
       </c>
@@ -10247,7 +10246,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="35" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E35" t="s">
         <v>195</v>
       </c>
@@ -10270,7 +10269,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="36" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E36" t="s">
         <v>195</v>
       </c>
@@ -10293,7 +10292,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="37" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E37" t="s">
         <v>195</v>
       </c>
@@ -10316,7 +10315,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="38" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E38" t="s">
         <v>195</v>
       </c>
@@ -10339,7 +10338,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="39" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E39" t="s">
         <v>195</v>
       </c>
@@ -10362,7 +10361,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="40" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E40" t="s">
         <v>195</v>
       </c>
@@ -10385,7 +10384,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="41" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E41" t="s">
         <v>195</v>
       </c>
@@ -10408,7 +10407,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="42" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E42" t="s">
         <v>195</v>
       </c>
@@ -10431,7 +10430,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="43" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E43" t="s">
         <v>195</v>
       </c>
@@ -10454,7 +10453,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="44" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E44" t="s">
         <v>195</v>
       </c>
@@ -10477,7 +10476,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="45" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E45" t="s">
         <v>195</v>
       </c>
@@ -10500,7 +10499,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="46" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E46" t="s">
         <v>195</v>
       </c>
@@ -10523,7 +10522,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="47" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E47" t="s">
         <v>195</v>
       </c>
@@ -10546,7 +10545,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="48" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E48" t="s">
         <v>195</v>
       </c>
@@ -10569,7 +10568,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="49" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E49" t="s">
         <v>195</v>
       </c>
@@ -10592,7 +10591,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="50" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E50" t="s">
         <v>195</v>
       </c>
@@ -10615,7 +10614,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="51" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E51" t="s">
         <v>195</v>
       </c>

</xml_diff>

<commit_message>
Add value for energy demand in 2030
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_Demands_LED.xlsx
+++ b/SuppXLS/Scen_SYS_Demands_LED.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{447C6241-6F42-4E9F-BB06-F66179337899}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C69F530E-E3CE-485A-943C-5B1B3FC47B5F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5033,107 +5033,107 @@
         <v>2020</v>
       </c>
       <c r="G4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.14102260336618419</v>
       </c>
       <c r="H4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>2.8193762108637852</v>
       </c>
       <c r="I4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.51996369762144268</v>
       </c>
       <c r="J4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.2412295956815371</v>
       </c>
       <c r="K4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.19018531303154435</v>
       </c>
       <c r="L4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>9.5561633661176384E-2</v>
       </c>
       <c r="M4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.27402416687719383</v>
       </c>
       <c r="N4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.45105079601868803</v>
       </c>
       <c r="O4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.18671376666095213</v>
       </c>
       <c r="P4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.21163803569729758</v>
       </c>
       <c r="Q4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.36834282959899767</v>
       </c>
       <c r="R4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.32581863140183054</v>
       </c>
       <c r="S4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.28676020471389613</v>
       </c>
       <c r="T4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>1.2126707484972317</v>
       </c>
       <c r="U4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.37129140482878509</v>
       </c>
       <c r="V4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.44273492088669852</v>
       </c>
       <c r="W4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.40362820139863753</v>
       </c>
       <c r="X4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.26802209006972721</v>
       </c>
       <c r="Y4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.59904734864666986</v>
       </c>
       <c r="Z4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>7.6883209959732524E-2</v>
       </c>
       <c r="AA4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.32081898120752922</v>
       </c>
       <c r="AB4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.1678236258531208</v>
       </c>
       <c r="AC4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.14796147778469043</v>
       </c>
       <c r="AD4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.16503614500140071</v>
       </c>
       <c r="AE4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.32014165283799628</v>
       </c>
       <c r="AF4" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E4,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F4,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E4,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.15354445783325901</v>
       </c>
     </row>
@@ -5149,107 +5149,107 @@
         <v>2050</v>
       </c>
       <c r="G5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.24919348706604891</v>
       </c>
       <c r="H5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>4.9819686530101315</v>
       </c>
       <c r="I5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.91879999280394731</v>
       </c>
       <c r="J5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.42626389455684793</v>
       </c>
       <c r="K5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.33606627740388867</v>
       </c>
       <c r="L5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.16886184308995011</v>
       </c>
       <c r="M5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.48421342433443482</v>
       </c>
       <c r="N5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.797027696417964</v>
       </c>
       <c r="O5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.32993189380189941</v>
       </c>
       <c r="P5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.37397423428835075</v>
       </c>
       <c r="Q5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.65087888007008443</v>
       </c>
       <c r="R5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.57573664768678368</v>
       </c>
       <c r="S5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.50671859445735434</v>
       </c>
       <c r="T5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>2.1428455103494626</v>
       </c>
       <c r="U5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.65608914938754559</v>
       </c>
       <c r="V5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.78233315899855904</v>
       </c>
       <c r="W5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.7132297701493322</v>
       </c>
       <c r="X5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.47360747597162428</v>
       </c>
       <c r="Y5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>1.0585444755924167</v>
       </c>
       <c r="Z5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.13585620127114331</v>
       </c>
       <c r="AA5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.56690203368669112</v>
       </c>
       <c r="AB5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.29655213802722385</v>
       </c>
       <c r="AC5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.26145480029802121</v>
       </c>
       <c r="AD5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.29162652995454996</v>
       </c>
       <c r="AE5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.56570516301302765</v>
       </c>
       <c r="AF5" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E5,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F5,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E5,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.2713201852314594</v>
       </c>
     </row>
@@ -5265,107 +5265,107 @@
         <v>2020</v>
       </c>
       <c r="G6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.32193664473309486</v>
       </c>
       <c r="H6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>5.637813854608976</v>
       </c>
       <c r="I6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>1.1480382927336128</v>
       </c>
       <c r="J6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.54522568908947855</v>
       </c>
       <c r="K6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.41020881320348074</v>
       </c>
       <c r="L6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.21133746790128183</v>
       </c>
       <c r="M6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.56924850267004323</v>
       </c>
       <c r="N6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.98828046988197249</v>
       </c>
       <c r="O6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.41882409160736161</v>
       </c>
       <c r="P6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.47278848560105868</v>
       </c>
       <c r="Q6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.83850274795415447</v>
       </c>
       <c r="R6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.71154373932557857</v>
       </c>
       <c r="S6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.64533477367968184</v>
       </c>
       <c r="T6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>2.6080003354214218</v>
       </c>
       <c r="U6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.8535978085319772</v>
       </c>
       <c r="V6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.96137078018953437</v>
       </c>
       <c r="W6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.932415749736074</v>
       </c>
       <c r="X6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.58823966562202801</v>
       </c>
       <c r="Y6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>1.3170332096303565</v>
       </c>
       <c r="Z6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.17261327906182664</v>
       </c>
       <c r="AA6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.72941378774211518</v>
       </c>
       <c r="AB6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.39273887171064176</v>
       </c>
       <c r="AC6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.32039449419408184</v>
       </c>
       <c r="AD6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.34813170258514758</v>
       </c>
       <c r="AE6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.64114085295794276</v>
       </c>
       <c r="AF6" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E6,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.35260315962707711</v>
       </c>
     </row>
@@ -5381,107 +5381,107 @@
         <v>2050</v>
       </c>
       <c r="G7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.42806487464250859</v>
       </c>
       <c r="H7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>7.4963509759251048</v>
       </c>
       <c r="I7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>1.5264955881963764</v>
       </c>
       <c r="J7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.72496241130132655</v>
       </c>
       <c r="K7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.54543646109867361</v>
       </c>
       <c r="L7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.2810060556462261</v>
       </c>
       <c r="M7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.75690448081146366</v>
       </c>
       <c r="N7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>1.3140726983795172</v>
       </c>
       <c r="O7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.55689181459850601</v>
       </c>
       <c r="P7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.62864587530576854</v>
       </c>
       <c r="Q7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>1.1149199060205524</v>
       </c>
       <c r="R7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.94610814444434155</v>
       </c>
       <c r="S7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.85807302000885533</v>
       </c>
       <c r="T7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>3.4677423490430845</v>
       </c>
       <c r="U7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>1.134991138418852</v>
       </c>
       <c r="V7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>1.2782920777719677</v>
       </c>
       <c r="W7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>1.2397918582905652</v>
       </c>
       <c r="X7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.78215618769651429</v>
       </c>
       <c r="Y7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>1.7512006321860119</v>
       </c>
       <c r="Z7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.22951621964157642</v>
       </c>
       <c r="AA7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.96986915506685767</v>
       </c>
       <c r="AB7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.52220745490292342</v>
       </c>
       <c r="AC7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.42601434548417128</v>
       </c>
       <c r="AD7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.46289528099462979</v>
       </c>
       <c r="AE7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.85249654967724642</v>
       </c>
       <c r="AF7" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E7,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F7,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E7,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.46884077905903881</v>
       </c>
     </row>
@@ -5497,107 +5497,107 @@
         <v>2020</v>
       </c>
       <c r="G8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.27435547637321495</v>
       </c>
       <c r="H8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>4.8874675973215007</v>
       </c>
       <c r="I8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.98750716185845822</v>
       </c>
       <c r="J8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.47552429060912443</v>
       </c>
       <c r="K8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.35331078909799174</v>
       </c>
       <c r="L8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.18192405921838437</v>
       </c>
       <c r="M8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.49433293928500699</v>
       </c>
       <c r="N8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.84062004677085977</v>
       </c>
       <c r="O8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.36232197941731037</v>
       </c>
       <c r="P8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.40153594290187117</v>
       </c>
       <c r="Q8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.71368599033539704</v>
       </c>
       <c r="R8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.61113233633908892</v>
       </c>
       <c r="S8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.54794246709160832</v>
       </c>
       <c r="T8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>2.2342931214267647</v>
       </c>
       <c r="U8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.74304638421703217</v>
       </c>
       <c r="V8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.82312954869858934</v>
       </c>
       <c r="W8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.79632066689536773</v>
       </c>
       <c r="X8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.5014811864865022</v>
       </c>
       <c r="Y8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>1.1393573908292929</v>
       </c>
       <c r="Z8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.14698615350023855</v>
       </c>
       <c r="AA8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.63179454507028443</v>
       </c>
       <c r="AB8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.33116307912916793</v>
       </c>
       <c r="AC8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.27602684102814479</v>
       </c>
       <c r="AD8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.2952095661319819</v>
       </c>
       <c r="AE8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.54379756531765255</v>
       </c>
       <c r="AF8" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E8,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F8,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E8,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.31412261464919838</v>
       </c>
     </row>
@@ -5613,107 +5613,107 @@
         <v>2050</v>
       </c>
       <c r="G9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.36429509503519336</v>
       </c>
       <c r="H9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>6.4896844647839922</v>
       </c>
       <c r="I9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>1.3112332224336185</v>
       </c>
       <c r="J9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.63141136794128272</v>
       </c>
       <c r="K9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.46913365533234114</v>
       </c>
       <c r="L9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.24156267379184618</v>
       </c>
       <c r="M9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.65638589568697026</v>
       </c>
       <c r="N9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>1.1161933556970411</v>
       </c>
       <c r="O9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.48109890741023575</v>
       </c>
       <c r="P9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.53316805049116955</v>
       </c>
       <c r="Q9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.94764758885601152</v>
       </c>
       <c r="R9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.81147464409594539</v>
       </c>
       <c r="S9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.72756977830985914</v>
       </c>
       <c r="T9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>2.9667424021068545</v>
       </c>
       <c r="U9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.98663295055089162</v>
       </c>
       <c r="V9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>1.0929690966383923</v>
       </c>
       <c r="W9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>1.0573716874909749</v>
       </c>
       <c r="X9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.66587749187461598</v>
       </c>
       <c r="Y9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>1.5128632183983965</v>
       </c>
       <c r="Z9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.19517137206835286</v>
       </c>
       <c r="AA9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.83891036869992042</v>
       </c>
       <c r="AB9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.43972545027457505</v>
       </c>
       <c r="AC9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.36651436892706152</v>
       </c>
       <c r="AD9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.39198560338942773</v>
       </c>
       <c r="AE9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.7220660886966046</v>
       </c>
       <c r="AF9" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E9,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F9,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E9,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.41709875548708081</v>
       </c>
     </row>
@@ -5729,107 +5729,107 @@
         <v>2020</v>
       </c>
       <c r="G10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.17991488188042462</v>
       </c>
       <c r="H10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>2.6871723541686299</v>
       </c>
       <c r="I10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.48763398226070803</v>
       </c>
       <c r="J10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.3135901348759621</v>
       </c>
       <c r="K10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.22335515894815736</v>
       </c>
       <c r="L10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.10778652622510916</v>
       </c>
       <c r="M10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.2824588239748011</v>
       </c>
       <c r="N10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.43704621254646414</v>
       </c>
       <c r="O10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.20559159765702764</v>
       </c>
       <c r="P10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.23409610092244049</v>
       </c>
       <c r="Q10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.47314719217489071</v>
       </c>
       <c r="R10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.31213492756751032</v>
       </c>
       <c r="S10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.30715715583422787</v>
       </c>
       <c r="T10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>1.643458450750628</v>
       </c>
       <c r="U10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.44716269403431846</v>
       </c>
       <c r="V10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.50383886577623815</v>
       </c>
       <c r="W10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.41246493081645397</v>
       </c>
       <c r="X10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.38312416759737483</v>
       </c>
       <c r="Y10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.61177286314532875</v>
       </c>
       <c r="Z10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>8.1588596696128737E-2</v>
       </c>
       <c r="AA10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.34456408847334713</v>
       </c>
       <c r="AB10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.15301315083761008</v>
       </c>
       <c r="AC10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.16686146187994025</v>
       </c>
       <c r="AD10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.1939549663563945</v>
       </c>
       <c r="AE10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.40532554878448751</v>
       </c>
       <c r="AF10" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E10,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F10,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E10,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.15629751581539669</v>
       </c>
     </row>
@@ -5845,107 +5845,107 @@
         <v>2050</v>
       </c>
       <c r="G11" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.14827528364690531</v>
       </c>
       <c r="H11" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>2.2146097024218854</v>
       </c>
       <c r="I11" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.40187930136669486</v>
       </c>
       <c r="J11" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.2584425796889217</v>
       </c>
       <c r="K11" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.18407620982153458</v>
       </c>
       <c r="L11" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>8.8831327249319483E-2</v>
       </c>
       <c r="M11" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.23278598082436783</v>
       </c>
       <c r="N11" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.36018783135017274</v>
       </c>
       <c r="O11" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.16943652542470969</v>
       </c>
       <c r="P11" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.19292826364402085</v>
       </c>
       <c r="Q11" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.38994013943269012</v>
       </c>
       <c r="R11" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.25724328325401569</v>
       </c>
       <c r="S11" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.25314089601418438</v>
       </c>
       <c r="T11" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>1.3544419750052186</v>
       </c>
       <c r="U11" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.36852524149902982</v>
       </c>
       <c r="V11" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.41523441504387931</v>
       </c>
       <c r="W11" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.33992938200553119</v>
       </c>
       <c r="X11" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.31574844742549418</v>
       </c>
       <c r="Y11" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.50418727935269625</v>
       </c>
       <c r="Z11" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>6.7240531694936503E-2</v>
       </c>
       <c r="AA11" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.28396949390144766</v>
       </c>
       <c r="AB11" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.12610445620186289</v>
       </c>
       <c r="AC11" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.1375174211904778</v>
       </c>
       <c r="AD11" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.15984629704136455</v>
       </c>
       <c r="AE11" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.33404552245600816</v>
       </c>
       <c r="AF11" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E11,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F11,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E11,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.12881123700615976</v>
       </c>
     </row>
@@ -5961,107 +5961,107 @@
         <v>2020</v>
       </c>
       <c r="G12" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.11877072280331726</v>
       </c>
       <c r="H12" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>2.8108410437988307</v>
       </c>
       <c r="I12" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.46418465725126973</v>
       </c>
       <c r="J12" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.20701637682180085</v>
       </c>
       <c r="K12" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.17669366804736417</v>
       </c>
       <c r="L12" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>8.5268667061406372E-2</v>
       </c>
       <c r="M12" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.26887595443305573</v>
       </c>
       <c r="N12" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.40689799863785192</v>
       </c>
       <c r="O12" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.16264112134598166</v>
       </c>
       <c r="P12" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.18519070229836443</v>
       </c>
       <c r="Q12" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.31234789151194903</v>
       </c>
       <c r="R12" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.29712499464734149</v>
       </c>
       <c r="S12" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.2478743232509259</v>
       </c>
       <c r="T12" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>1.1325234445793442</v>
       </c>
       <c r="U12" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.30814422737844349</v>
       </c>
       <c r="V12" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.4065955017150939</v>
       </c>
       <c r="W12" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.33285718287496763</v>
       </c>
       <c r="X12" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.2423647068853749</v>
       </c>
       <c r="Y12" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.53835690271162884</v>
       </c>
       <c r="Z12" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>6.6849733743931328E-2</v>
       </c>
       <c r="AA12" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.27226183378227509</v>
       </c>
       <c r="AB12" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.13465076815529611</v>
       </c>
       <c r="AC12" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.13671817815842413</v>
       </c>
       <c r="AD12" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.15891727991754154</v>
       </c>
       <c r="AE12" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.33210406984658275</v>
       </c>
       <c r="AF12" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E12,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.12806259379618537</v>
       </c>
     </row>
@@ -6077,107 +6077,107 @@
         <v>2050</v>
       </c>
       <c r="G13" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="H13" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="I13" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="J13" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="K13" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="L13" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="M13" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="N13" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="O13" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="P13" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="Q13" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="R13" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="S13" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="T13" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="U13" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="V13" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="W13" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="X13" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="Y13" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="Z13" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AA13" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AB13" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AC13" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AD13" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AE13" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AF13" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E13,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F13,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E13,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
     </row>
@@ -6193,107 +6193,107 @@
         <v>2020</v>
       </c>
       <c r="G14" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>5.2718404005341085E-2</v>
       </c>
       <c r="H14" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>1.2476395718090449</v>
       </c>
       <c r="I14" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.20603624964526826</v>
       </c>
       <c r="J14" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>9.1887737410560083E-2</v>
       </c>
       <c r="K14" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>7.8428487740468913E-2</v>
       </c>
       <c r="L14" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>3.7847947145898689E-2</v>
       </c>
       <c r="M14" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.11934516233092786</v>
       </c>
       <c r="N14" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.18060859254580502</v>
       </c>
       <c r="O14" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>7.2191026042654344E-2</v>
       </c>
       <c r="P14" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>8.2200040812796554E-2</v>
       </c>
       <c r="Q14" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.13864092047508789</v>
       </c>
       <c r="R14" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.13188397896544479</v>
       </c>
       <c r="S14" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.11002323137607345</v>
       </c>
       <c r="T14" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.502689779835093</v>
       </c>
       <c r="U14" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.13677505270176574</v>
       </c>
       <c r="V14" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.18047432414524345</v>
       </c>
       <c r="W14" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.14774431803316512</v>
       </c>
       <c r="X14" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.1075776945079131</v>
       </c>
       <c r="Y14" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.23895886146297882</v>
       </c>
       <c r="Z14" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>2.9672390535149896E-2</v>
       </c>
       <c r="AA14" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.12084804242824863</v>
       </c>
       <c r="AB14" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>5.9767032040341748E-2</v>
       </c>
       <c r="AC14" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>6.0684687109007783E-2</v>
       </c>
       <c r="AD14" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>7.0538135732292298E-2</v>
       </c>
       <c r="AE14" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.14741003601521568</v>
       </c>
       <c r="AF14" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E14,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F14,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E14,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>5.6842758875006463E-2</v>
       </c>
     </row>
@@ -6309,107 +6309,107 @@
         <v>2050</v>
       </c>
       <c r="G15" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>4.2004379525771102E-2</v>
       </c>
       <c r="H15" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.99408028513777102</v>
       </c>
       <c r="I15" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.16416325549782501</v>
       </c>
       <c r="J15" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>7.3213282321037701E-2</v>
       </c>
       <c r="K15" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>6.2489372105217399E-2</v>
       </c>
       <c r="L15" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>3.0156063450376601E-2</v>
       </c>
       <c r="M15" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>9.5090501840783506E-2</v>
       </c>
       <c r="N15" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.143903291650118</v>
       </c>
       <c r="O15" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>5.75195572298293E-2</v>
       </c>
       <c r="P15" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>6.5494427922832596E-2</v>
       </c>
       <c r="Q15" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.110464759912835</v>
       </c>
       <c r="R15" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.105081039730871</v>
       </c>
       <c r="S15" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>8.7663078095158206E-2</v>
       </c>
       <c r="T15" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.40052753292342302</v>
       </c>
       <c r="U15" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.108978094685117</v>
       </c>
       <c r="V15" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.14379631077765201</v>
       </c>
       <c r="W15" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.117718063066032</v>
       </c>
       <c r="X15" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>8.5714550618035304E-2</v>
       </c>
       <c r="Y15" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.190394965426499</v>
       </c>
       <c r="Z15" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>2.36420350158753E-2</v>
       </c>
       <c r="AA15" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>9.6287949813282703E-2</v>
       </c>
       <c r="AB15" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>4.7620506430678201E-2</v>
       </c>
       <c r="AC15" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>4.8351665359049598E-2</v>
       </c>
       <c r="AD15" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>5.6202585799816303E-2</v>
       </c>
       <c r="AE15" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.117451717583548</v>
       </c>
       <c r="AF15" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E15,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F15,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E15,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>4.5290536808279797E-2</v>
       </c>
     </row>
@@ -6425,107 +6425,107 @@
         <v>2020</v>
       </c>
       <c r="G16" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.16235731275947515</v>
       </c>
       <c r="H16" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>3.8423660957334085</v>
       </c>
       <c r="I16" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.63453157307374231</v>
       </c>
       <c r="J16" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.28298743869437681</v>
       </c>
       <c r="K16" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.24153687414440531</v>
       </c>
       <c r="L16" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.11656064154461539</v>
       </c>
       <c r="M16" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.3675483014419349</v>
       </c>
       <c r="N16" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.55622180337699523</v>
       </c>
       <c r="O16" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.22232731082767995</v>
       </c>
       <c r="P16" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.25315215790168288</v>
       </c>
       <c r="Q16" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.42697361028901426</v>
       </c>
       <c r="R16" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.40616420062123709</v>
       </c>
       <c r="S16" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.3388394721798389</v>
       </c>
       <c r="T16" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>1.5481379481330504</v>
       </c>
       <c r="U16" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.4212272815949526</v>
       </c>
       <c r="V16" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.55580829585310521</v>
       </c>
       <c r="W16" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.45500942040877851</v>
       </c>
       <c r="X16" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.33130793169298151</v>
       </c>
       <c r="Y16" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.73592361793165129</v>
       </c>
       <c r="Z16" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>9.1382311003734881E-2</v>
       </c>
       <c r="AA16" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.37217673393347922</v>
       </c>
       <c r="AB16" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.18406503187570397</v>
       </c>
       <c r="AC16" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.18689114191829229</v>
       </c>
       <c r="AD16" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.21723689061978846</v>
       </c>
       <c r="AE16" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.45397992926309294</v>
       </c>
       <c r="AF16" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E16,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F16,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E16,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.17505912318297531</v>
       </c>
     </row>
@@ -6541,108 +6541,108 @@
         <v>2050</v>
       </c>
       <c r="G17" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.26045346019004401</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
       </c>
       <c r="H17" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>6.1639203553045512</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
       </c>
       <c r="I17" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.0179149987024101</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
       </c>
       <c r="J17" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.45396820349853301</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
       </c>
       <c r="K17" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.38747324382976506</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
       </c>
       <c r="L17" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.18698647998221901</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
       </c>
       <c r="M17" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.58962066611279595</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
       </c>
       <c r="N17" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.89229053413382609</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
       </c>
       <c r="O17" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.35665727903246103</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
       </c>
       <c r="P17" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.40610647195022492</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
       </c>
       <c r="Q17" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.68495069497951599</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
       </c>
       <c r="R17" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.65156825805464502</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
       </c>
       <c r="S17" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.54356598713202597</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
       </c>
       <c r="T17" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>2.4835215524915499</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
       </c>
       <c r="U17" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.67573243947675998</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
       </c>
       <c r="V17" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.89162718572295807</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
       </c>
       <c r="W17" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.72992571723638999</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
       </c>
       <c r="X17" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.53148389642096905</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
       </c>
       <c r="Y17" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.1805680290473299</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
       </c>
       <c r="Z17" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.146595423985277</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
       </c>
       <c r="AA17" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.59704559349789399</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
       </c>
       <c r="AB17" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.29527696435231898</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
       </c>
       <c r="AC17" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.29981060762935702</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
       </c>
       <c r="AD17" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.34849123135384003</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
       </c>
       <c r="AE17" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.72827420843415902</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
       </c>
       <c r="AF17" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.28082969344526898</v>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E17,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F17,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E17,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="4:32" x14ac:dyDescent="0.25">
@@ -6657,107 +6657,107 @@
         <v>2020</v>
       </c>
       <c r="G18" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="H18" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.13395677260860595</v>
       </c>
       <c r="I18" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="J18" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="K18" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="L18" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="M18" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="N18" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="O18" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="P18" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="Q18" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="R18" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="S18" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>4.6779068407982807E-2</v>
       </c>
       <c r="T18" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>4.6352277307537207E-4</v>
       </c>
       <c r="U18" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>4.6529102661710439E-2</v>
       </c>
       <c r="V18" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="W18" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="X18" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="Y18" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="Z18" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AA18" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>9.2704554615074527E-5</v>
       </c>
       <c r="AB18" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AC18" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AD18" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AE18" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AF18" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E18,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
     </row>
@@ -6773,107 +6773,107 @@
         <v>2050</v>
       </c>
       <c r="G19" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="H19" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.13599128494106499</v>
       </c>
       <c r="I19" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="J19" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="K19" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="L19" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="M19" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="N19" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="O19" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="P19" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="Q19" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="R19" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="S19" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>4.7489540821759602E-2</v>
       </c>
       <c r="T19" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>4.7056267691773199E-4</v>
       </c>
       <c r="U19" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>4.7235778638893701E-2</v>
       </c>
       <c r="V19" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="W19" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="X19" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="Y19" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="Z19" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AA19" s="16">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>9.4112535383546506E-5</v>
       </c>
       <c r="AB19" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AC19" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AD19" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AE19" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AF19" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E19,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F19,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E19,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
     </row>
@@ -6889,107 +6889,107 @@
         <v>2020</v>
       </c>
       <c r="G20" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="H20" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>41.184477806263274</v>
       </c>
       <c r="I20" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="J20" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="K20" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="L20" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="M20" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="N20" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="O20" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="P20" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="Q20" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="R20" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="S20" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>2.4385793540260186</v>
       </c>
       <c r="T20" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>2.2547565653239303</v>
       </c>
       <c r="U20" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.24571396736982151</v>
       </c>
       <c r="V20" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="W20" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="X20" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="Y20" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="Z20" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AA20" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.70149337318584271</v>
       </c>
       <c r="AB20" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AC20" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AD20" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AE20" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AF20" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
     </row>
@@ -7005,107 +7005,107 @@
         <v>2050</v>
       </c>
       <c r="G21" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="H21" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>40.411547456014503</v>
       </c>
       <c r="I21" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="J21" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="K21" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="L21" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="M21" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="N21" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="O21" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="P21" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="Q21" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="R21" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="S21" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>2.3928132767411898</v>
       </c>
       <c r="T21" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>2.2124403851853902</v>
       </c>
       <c r="U21" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.24110252653151398</v>
       </c>
       <c r="V21" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="W21" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="X21" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="Y21" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="Z21" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AA21" s="15">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0.68832808501139198</v>
       </c>
       <c r="AB21" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AC21" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AD21" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AE21" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AF21" s="4">
-        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CN$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
+        <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
         <v>0</v>
       </c>
     </row>
@@ -7882,10 +7882,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C1:Q57"/>
+  <dimension ref="C1:R57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7896,11 +7896,11 @@
     <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="53.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.88671875" customWidth="1"/>
-    <col min="11" max="12" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="15.88671875" customWidth="1"/>
+    <col min="12" max="13" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
         <v>190</v>
       </c>
@@ -7908,7 +7908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="3:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C2" s="14" t="s">
         <v>1</v>
       </c>
@@ -7934,10 +7934,13 @@
         <v>2020</v>
       </c>
       <c r="K2" s="14">
+        <v>2030</v>
+      </c>
+      <c r="L2" s="14">
         <v>2050</v>
       </c>
     </row>
-    <row r="3" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:16" x14ac:dyDescent="0.3">
       <c r="D3" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -7962,11 +7965,15 @@
         <v>2.2653176519999998</v>
       </c>
       <c r="K3">
+        <f>(J3*2/3)+(L3/3)</f>
+        <v>1.9610696723833332</v>
+      </c>
+      <c r="L3">
         <v>1.35257371315</v>
       </c>
-      <c r="O3" s="2"/>
-    </row>
-    <row r="4" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="P3" s="2"/>
+    </row>
+    <row r="4" spans="3:16" x14ac:dyDescent="0.3">
       <c r="D4" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -7991,11 +7998,15 @@
         <v>22.058152969999998</v>
       </c>
       <c r="K4">
+        <f t="shared" ref="K4:K28" si="0">(J4*2/3)+(L4/3)</f>
+        <v>20.371927879499999</v>
+      </c>
+      <c r="L4">
         <v>16.999477698500002</v>
       </c>
-      <c r="O4" s="2"/>
-    </row>
-    <row r="5" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="P4" s="2"/>
+    </row>
+    <row r="5" spans="3:16" x14ac:dyDescent="0.3">
       <c r="D5" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8020,11 +8031,15 @@
         <v>0.82191421200000003</v>
       </c>
       <c r="K5">
+        <f t="shared" si="0"/>
+        <v>1.0520667756000002</v>
+      </c>
+      <c r="L5">
         <v>1.5123719028</v>
       </c>
-      <c r="O5" s="2"/>
-    </row>
-    <row r="6" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="P5" s="2"/>
+    </row>
+    <row r="6" spans="3:16" x14ac:dyDescent="0.3">
       <c r="D6" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8049,11 +8064,15 @@
         <v>5.7840131420000001</v>
       </c>
       <c r="K6">
+        <f t="shared" si="0"/>
+        <v>5.425879528816667</v>
+      </c>
+      <c r="L6">
         <v>4.7096123024500001</v>
       </c>
-      <c r="O6" s="2"/>
-    </row>
-    <row r="7" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="P6" s="2"/>
+    </row>
+    <row r="7" spans="3:16" x14ac:dyDescent="0.3">
       <c r="D7" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8078,11 +8097,15 @@
         <v>1.2574088990000001</v>
       </c>
       <c r="K7">
+        <f t="shared" si="0"/>
+        <v>1.2069042374333334</v>
+      </c>
+      <c r="L7">
         <v>1.1058949143000001</v>
       </c>
-      <c r="O7" s="2"/>
-    </row>
-    <row r="8" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="P7" s="2"/>
+    </row>
+    <row r="8" spans="3:16" x14ac:dyDescent="0.3">
       <c r="D8" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8107,11 +8130,15 @@
         <v>10.12574641</v>
       </c>
       <c r="K8">
+        <f t="shared" si="0"/>
+        <v>9.6351456128333322</v>
+      </c>
+      <c r="L8">
         <v>8.6539440184999989</v>
       </c>
-      <c r="O8" s="2"/>
-    </row>
-    <row r="9" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="P8" s="2"/>
+    </row>
+    <row r="9" spans="3:16" x14ac:dyDescent="0.3">
       <c r="D9" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8136,11 +8163,15 @@
         <v>1.449528948</v>
       </c>
       <c r="K9">
+        <f t="shared" si="0"/>
+        <v>1.4808533143</v>
+      </c>
+      <c r="L9">
         <v>1.5435020469</v>
       </c>
-      <c r="O9" s="2"/>
-    </row>
-    <row r="10" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="P9" s="2"/>
+    </row>
+    <row r="10" spans="3:16" x14ac:dyDescent="0.3">
       <c r="D10" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8165,11 +8196,15 @@
         <v>14.23391084</v>
       </c>
       <c r="K10">
+        <f t="shared" si="0"/>
+        <v>12.450956954125866</v>
+      </c>
+      <c r="L10">
         <v>8.8850491823775997</v>
       </c>
-      <c r="O10" s="2"/>
-    </row>
-    <row r="11" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="P10" s="2"/>
+    </row>
+    <row r="11" spans="3:16" x14ac:dyDescent="0.3">
       <c r="D11" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8194,11 +8229,15 @@
         <v>18.18372415</v>
       </c>
       <c r="K11">
+        <f t="shared" si="0"/>
+        <v>15.988176054166667</v>
+      </c>
+      <c r="L11">
         <v>11.597079862500001</v>
       </c>
-      <c r="O11" s="2"/>
-    </row>
-    <row r="12" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="P11" s="2"/>
+    </row>
+    <row r="12" spans="3:16" x14ac:dyDescent="0.3">
       <c r="D12" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8223,11 +8262,15 @@
         <v>2.2668447500000002</v>
       </c>
       <c r="K12">
+        <f t="shared" si="0"/>
+        <v>1.6954790646166666</v>
+      </c>
+      <c r="L12">
         <v>0.55274769385</v>
       </c>
-      <c r="O12" s="2"/>
-    </row>
-    <row r="13" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="P12" s="2"/>
+    </row>
+    <row r="13" spans="3:16" x14ac:dyDescent="0.3">
       <c r="D13" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8252,11 +8295,15 @@
         <v>7.0076904100000004</v>
       </c>
       <c r="K13">
+        <f t="shared" si="0"/>
+        <v>9.9931567838333351</v>
+      </c>
+      <c r="L13">
         <v>15.964089531500001</v>
       </c>
-      <c r="O13" s="2"/>
-    </row>
-    <row r="14" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="P13" s="2"/>
+    </row>
+    <row r="14" spans="3:16" x14ac:dyDescent="0.3">
       <c r="D14" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8281,11 +8328,15 @@
         <v>0.186509807</v>
       </c>
       <c r="K14">
+        <f t="shared" si="0"/>
+        <v>0.13639114078333334</v>
+      </c>
+      <c r="L14">
         <v>3.6153808350000004E-2</v>
       </c>
-      <c r="O14" s="2"/>
-    </row>
-    <row r="15" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="P14" s="2"/>
+    </row>
+    <row r="15" spans="3:16" x14ac:dyDescent="0.3">
       <c r="D15" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8310,11 +8361,15 @@
         <v>3.4153449619999998</v>
       </c>
       <c r="K15">
+        <f t="shared" si="0"/>
+        <v>3.7348343824833337</v>
+      </c>
+      <c r="L15">
         <v>4.3738132234500009</v>
       </c>
-      <c r="O15" s="2"/>
-    </row>
-    <row r="16" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="P15" s="2"/>
+    </row>
+    <row r="16" spans="3:16" x14ac:dyDescent="0.3">
       <c r="D16" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8339,11 +8394,15 @@
         <v>4.0998448639999996</v>
       </c>
       <c r="K16">
+        <f t="shared" si="0"/>
+        <v>4.1453782241999999</v>
+      </c>
+      <c r="L16">
         <v>4.2364449446000005</v>
       </c>
-      <c r="O16" s="2"/>
-    </row>
-    <row r="17" spans="4:17" x14ac:dyDescent="0.3">
+      <c r="P16" s="2"/>
+    </row>
+    <row r="17" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D17" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -8367,12 +8426,16 @@
       <c r="J17">
         <v>10.76129175</v>
       </c>
-      <c r="K17" s="1">
+      <c r="K17">
+        <f t="shared" si="0"/>
+        <v>13.512761870306244</v>
+      </c>
+      <c r="L17" s="1">
         <v>19.015702110918735</v>
       </c>
-      <c r="O17" s="2"/>
-    </row>
-    <row r="18" spans="4:17" x14ac:dyDescent="0.3">
+      <c r="P17" s="2"/>
+    </row>
+    <row r="18" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D18" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -8396,12 +8459,16 @@
       <c r="J18">
         <v>23.13677727</v>
       </c>
-      <c r="K18" s="1">
+      <c r="K18">
+        <f t="shared" si="0"/>
+        <v>25.67916695820422</v>
+      </c>
+      <c r="L18" s="1">
         <v>30.763946334612658</v>
       </c>
-      <c r="O18" s="2"/>
-    </row>
-    <row r="19" spans="4:17" x14ac:dyDescent="0.3">
+      <c r="P18" s="2"/>
+    </row>
+    <row r="19" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -8425,12 +8492,16 @@
       <c r="J19">
         <v>19.908389740000001</v>
       </c>
-      <c r="K19" s="1">
+      <c r="K19">
+        <f t="shared" si="0"/>
+        <v>22.083855678156205</v>
+      </c>
+      <c r="L19" s="1">
         <v>26.43478755446861</v>
       </c>
-      <c r="O19" s="2"/>
-    </row>
-    <row r="20" spans="4:17" x14ac:dyDescent="0.3">
+      <c r="P19" s="2"/>
+    </row>
+    <row r="20" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D20" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -8454,12 +8525,16 @@
       <c r="J20">
         <v>11.754512350000001</v>
       </c>
-      <c r="K20" s="1">
+      <c r="K20">
+        <f t="shared" si="0"/>
+        <v>11.065467907987845</v>
+      </c>
+      <c r="L20" s="1">
         <v>9.6873790239635298</v>
       </c>
-      <c r="O20" s="2"/>
-    </row>
-    <row r="21" spans="4:17" x14ac:dyDescent="0.3">
+      <c r="P20" s="2"/>
+    </row>
+    <row r="21" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D21" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -8486,9 +8561,12 @@
       <c r="K21">
         <v>0</v>
       </c>
-      <c r="O21" s="2"/>
-    </row>
-    <row r="22" spans="4:17" x14ac:dyDescent="0.3">
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="P21" s="2"/>
+    </row>
+    <row r="22" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D22" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -8513,12 +8591,16 @@
         <v>4.4094344637268001</v>
       </c>
       <c r="K22">
+        <f t="shared" si="0"/>
+        <v>4.1107229120604405</v>
+      </c>
+      <c r="L22">
         <f>H22</f>
         <v>3.5132998087277199</v>
       </c>
-      <c r="O22" s="2"/>
-    </row>
-    <row r="23" spans="4:17" x14ac:dyDescent="0.3">
+      <c r="P22" s="2"/>
+    </row>
+    <row r="23" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D23" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -8543,12 +8625,14 @@
         <v>13.57977245</v>
       </c>
       <c r="K23">
-        <f>H23</f>
-        <v>21.784659175997099</v>
-      </c>
-      <c r="O23" s="2"/>
-    </row>
-    <row r="24" spans="4:17" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="P23" s="2"/>
+    </row>
+    <row r="24" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D24" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -8573,12 +8657,16 @@
         <v>0.23</v>
       </c>
       <c r="K24">
+        <f t="shared" si="0"/>
+        <v>0.23116440009552636</v>
+      </c>
+      <c r="L24">
         <f>H24</f>
         <v>0.23349320028657899</v>
       </c>
-      <c r="O24" s="2"/>
-    </row>
-    <row r="25" spans="4:17" x14ac:dyDescent="0.3">
+      <c r="P24" s="2"/>
+    </row>
+    <row r="25" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D25" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -8603,12 +8691,16 @@
         <v>46.814427170000002</v>
       </c>
       <c r="K25">
+        <f t="shared" si="0"/>
+        <v>46.521563664810671</v>
+      </c>
+      <c r="L25">
         <f>H25</f>
         <v>45.935836654432002</v>
       </c>
-      <c r="O25" s="2"/>
-    </row>
-    <row r="26" spans="4:17" x14ac:dyDescent="0.3">
+      <c r="P25" s="2"/>
+    </row>
+    <row r="26" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D26" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8633,11 +8725,15 @@
         <v>225.3003382</v>
       </c>
       <c r="K26">
+        <f t="shared" si="0"/>
+        <v>397.11688316666664</v>
+      </c>
+      <c r="L26">
         <v>740.74997310000003</v>
       </c>
-      <c r="O26" s="2"/>
-    </row>
-    <row r="27" spans="4:17" x14ac:dyDescent="0.3">
+      <c r="P26" s="2"/>
+    </row>
+    <row r="27" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D27" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8662,11 +8758,15 @@
         <v>788.3008562</v>
       </c>
       <c r="K27">
+        <f t="shared" si="0"/>
+        <v>940.31279246666668</v>
+      </c>
+      <c r="L27">
         <v>1244.336665</v>
       </c>
-      <c r="O27" s="2"/>
-    </row>
-    <row r="28" spans="4:17" x14ac:dyDescent="0.3">
+      <c r="P27" s="2"/>
+    </row>
+    <row r="28" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D28" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8691,11 +8791,15 @@
         <v>739.68368569999996</v>
       </c>
       <c r="K28">
+        <f t="shared" si="0"/>
+        <v>842.43810213333325</v>
+      </c>
+      <c r="L28">
         <v>1047.9469349999999</v>
       </c>
-      <c r="O28" s="2"/>
-    </row>
-    <row r="29" spans="4:17" x14ac:dyDescent="0.3">
+      <c r="P28" s="2"/>
+    </row>
+    <row r="29" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D29" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8715,20 +8819,21 @@
       </c>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
-      <c r="K29">
+      <c r="K29" s="2"/>
+      <c r="L29">
         <v>8.3303707615599745</v>
       </c>
-      <c r="O29" s="2"/>
-      <c r="P29" t="str">
-        <f t="shared" ref="P29:P39" si="0">IF(P66&lt;&gt;"",P66*$H29,"")</f>
+      <c r="P29" s="2"/>
+      <c r="Q29" t="str">
+        <f t="shared" ref="Q29:Q39" si="1">IF(Q66&lt;&gt;"",Q66*$H29,"")</f>
         <v/>
       </c>
-      <c r="Q29" t="str">
-        <f t="shared" ref="Q29" si="1">IF(Q66&lt;&gt;"",Q66*$H29,"")</f>
+      <c r="R29" t="str">
+        <f t="shared" ref="R29" si="2">IF(R66&lt;&gt;"",R66*$H29,"")</f>
         <v/>
       </c>
     </row>
-    <row r="30" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D30" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8748,20 +8853,21 @@
       </c>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
-      <c r="K30">
+      <c r="K30" s="2"/>
+      <c r="L30">
         <v>7.5247845525179748</v>
       </c>
-      <c r="O30" s="2"/>
-      <c r="P30" t="str">
-        <f t="shared" si="0"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="Q30" t="str">
-        <f t="shared" ref="Q30:Q39" si="2">IF(Q67&lt;&gt;"",Q67*$H30,"")</f>
+      <c r="R30" t="str">
+        <f t="shared" ref="R30:R39" si="3">IF(R67&lt;&gt;"",R67*$H30,"")</f>
         <v/>
       </c>
     </row>
-    <row r="31" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D31" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8781,20 +8887,21 @@
       </c>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
-      <c r="K31">
+      <c r="K31" s="2"/>
+      <c r="L31">
         <v>5.7762096629087072</v>
       </c>
-      <c r="O31" s="2"/>
-      <c r="P31" t="str">
-        <f t="shared" si="0"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="Q31" t="str">
-        <f t="shared" si="2"/>
+      <c r="R31" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="32" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D32" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8814,20 +8921,21 @@
       </c>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
-      <c r="K32">
+      <c r="K32" s="2"/>
+      <c r="L32">
         <v>2.8258260553410754</v>
       </c>
-      <c r="O32" s="2"/>
-      <c r="P32" t="str">
-        <f t="shared" si="0"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="Q32" t="str">
-        <f t="shared" si="2"/>
+      <c r="R32" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="33" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D33" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8847,20 +8955,21 @@
       </c>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
-      <c r="K33">
+      <c r="K33" s="2"/>
+      <c r="L33">
         <v>0.86352973225925755</v>
       </c>
-      <c r="O33" s="2"/>
-      <c r="P33" t="str">
-        <f t="shared" si="0"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="Q33" t="str">
-        <f t="shared" si="2"/>
+      <c r="R33" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="34" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D34" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8880,20 +8989,21 @@
       </c>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
-      <c r="K34">
+      <c r="K34" s="2"/>
+      <c r="L34">
         <v>0.80798776317929155</v>
       </c>
-      <c r="O34" s="2"/>
-      <c r="P34" t="str">
-        <f t="shared" si="0"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="Q34" t="str">
-        <f t="shared" si="2"/>
+      <c r="R34" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="35" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D35" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8913,20 +9023,21 @@
       </c>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
-      <c r="K35">
+      <c r="K35" s="2"/>
+      <c r="L35">
         <v>23.587286108700724</v>
       </c>
-      <c r="O35" s="2"/>
-      <c r="P35" t="str">
-        <f t="shared" si="0"/>
+      <c r="P35" s="2"/>
+      <c r="Q35" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="Q35" t="str">
-        <f t="shared" si="2"/>
+      <c r="R35" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="36" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D36" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8946,20 +9057,21 @@
       </c>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
-      <c r="K36">
+      <c r="K36" s="2"/>
+      <c r="L36">
         <v>0.55087144494553486</v>
       </c>
-      <c r="O36" s="2"/>
-      <c r="P36" t="str">
-        <f t="shared" si="0"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="Q36" t="str">
-        <f t="shared" si="2"/>
+      <c r="R36" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="37" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D37" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -8979,20 +9091,21 @@
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
-      <c r="K37">
+      <c r="K37" s="2"/>
+      <c r="L37">
         <v>1.7006066461478033</v>
       </c>
-      <c r="O37" s="2"/>
-      <c r="P37" t="str">
-        <f t="shared" si="0"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="Q37" t="str">
-        <f t="shared" si="2"/>
+      <c r="R37" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="38" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D38" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9012,20 +9125,21 @@
       </c>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
-      <c r="K38">
+      <c r="K38" s="2"/>
+      <c r="L38">
         <v>0.75018311632173929</v>
       </c>
-      <c r="O38" s="2"/>
-      <c r="P38" t="str">
-        <f t="shared" si="0"/>
+      <c r="P38" s="2"/>
+      <c r="Q38" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="Q38" t="str">
-        <f t="shared" si="2"/>
+      <c r="R38" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="39" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D39" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9045,20 +9159,21 @@
       </c>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
-      <c r="K39">
+      <c r="K39" s="2"/>
+      <c r="L39">
         <v>5.3069347641179023</v>
       </c>
-      <c r="O39" s="2"/>
-      <c r="P39" t="str">
-        <f t="shared" si="0"/>
+      <c r="P39" s="2"/>
+      <c r="Q39" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="Q39" t="str">
-        <f t="shared" si="2"/>
+      <c r="R39" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="40" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D40" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9078,11 +9193,12 @@
       </c>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
-      <c r="K40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="4:17" x14ac:dyDescent="0.3">
+      <c r="K40" s="2"/>
+      <c r="L40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D41" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9099,11 +9215,11 @@
       <c r="H41">
         <v>7.8120000000000003</v>
       </c>
-      <c r="K41">
+      <c r="L41">
         <v>32.865000000000002</v>
       </c>
     </row>
-    <row r="43" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D43" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9123,11 +9239,12 @@
       </c>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
-      <c r="K43">
+      <c r="K43" s="2"/>
+      <c r="L43">
         <v>10.047893325490021</v>
       </c>
     </row>
-    <row r="44" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D44" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9147,11 +9264,12 @@
       </c>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
-      <c r="K44">
+      <c r="K44" s="2"/>
+      <c r="L44">
         <v>16.878788423834521</v>
       </c>
     </row>
-    <row r="45" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D45" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9171,11 +9289,12 @@
       </c>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
-      <c r="K45">
+      <c r="K45" s="2"/>
+      <c r="L45">
         <v>14.214862498864701</v>
       </c>
     </row>
-    <row r="46" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D46" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9195,11 +9314,12 @@
       </c>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
-      <c r="K46">
+      <c r="K46" s="2"/>
+      <c r="L46">
         <v>0.179228357755223</v>
       </c>
     </row>
-    <row r="47" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D47" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9219,11 +9339,12 @@
       </c>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
-      <c r="K47">
+      <c r="K47" s="2"/>
+      <c r="L47">
         <v>0.30107381041032272</v>
       </c>
     </row>
-    <row r="48" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D48" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9243,11 +9364,12 @@
       </c>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
-      <c r="K48">
+      <c r="K48" s="2"/>
+      <c r="L48">
         <v>0.2535562807901901</v>
       </c>
     </row>
-    <row r="49" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D49" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9267,11 +9389,12 @@
       </c>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
-      <c r="K49">
+      <c r="K49" s="2"/>
+      <c r="L49">
         <v>5.3250910380053398</v>
       </c>
     </row>
-    <row r="50" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D50" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9291,11 +9414,12 @@
       </c>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
-      <c r="K50">
+      <c r="K50" s="2"/>
+      <c r="L50">
         <v>8.9452666401358414</v>
       </c>
     </row>
-    <row r="51" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D51" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9315,11 +9439,12 @@
       </c>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
-      <c r="K51">
+      <c r="K51" s="2"/>
+      <c r="L51">
         <v>7.5334634283143167</v>
       </c>
     </row>
-    <row r="52" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D52" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9339,11 +9464,12 @@
       </c>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
-      <c r="K52">
+      <c r="K52" s="2"/>
+      <c r="L52">
         <v>0.89996641800005883</v>
       </c>
     </row>
-    <row r="53" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D53" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9363,11 +9489,12 @@
       </c>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
-      <c r="K53">
+      <c r="K53" s="2"/>
+      <c r="L53">
         <v>1.5117937925797396</v>
       </c>
     </row>
-    <row r="54" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D54" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9387,11 +9514,12 @@
       </c>
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
-      <c r="K54">
+      <c r="K54" s="2"/>
+      <c r="L54">
         <v>1.2731921479513455</v>
       </c>
     </row>
-    <row r="55" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D55" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9411,11 +9539,12 @@
       </c>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
-      <c r="K55">
+      <c r="K55" s="2"/>
+      <c r="L55">
         <v>1.4030879288454441</v>
       </c>
     </row>
-    <row r="56" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D56" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9435,11 +9564,12 @@
       </c>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
-      <c r="K56">
+      <c r="K56" s="2"/>
+      <c r="L56">
         <v>2.3569541916751464</v>
       </c>
     </row>
-    <row r="57" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D57" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9459,7 +9589,8 @@
       </c>
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
-      <c r="K57">
+      <c r="K57" s="2"/>
+      <c r="L57">
         <v>1.9849635477078642</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update LED scenario file
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_Demands_LED.xlsx
+++ b/SuppXLS/Scen_SYS_Demands_LED.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uccireland-my.sharepoint.com/personal/agaur_ucc_ie/Documents/TIM-2.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="93" documentId="13_ncr:1_{C69F530E-E3CE-485A-943C-5B1B3FC47B5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{063A455A-82FA-45DE-BC87-194ABD9AAF51}"/>
+  <xr:revisionPtr revIDLastSave="106" documentId="13_ncr:1_{C69F530E-E3CE-485A-943C-5B1B3FC47B5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{3F95F6CE-D2D2-43BD-AC95-2271ABB22125}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BY-Demands" sheetId="5" r:id="rId1"/>
@@ -931,7 +931,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -984,6 +984,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Attrib" xfId="2" xr:uid="{16EBE39D-6598-42BD-A97C-1EF313EA2EC2}"/>
@@ -6745,8 +6746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:P44"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29:F32"/>
+    <sheetView tabSelected="1" topLeftCell="E7" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7273,9 +7274,8 @@
       <c r="J17" s="36">
         <v>10.76129175</v>
       </c>
-      <c r="K17" s="36">
-        <f t="shared" ref="K17:K25" si="1">(J17*2/3)+(L17/3)</f>
-        <v>13.357743891204088</v>
+      <c r="K17" s="39">
+        <v>16.798154247711324</v>
       </c>
       <c r="L17" s="36">
         <v>18.550648173612263</v>
@@ -7306,9 +7306,8 @@
       <c r="J18" s="36">
         <v>23.13677727</v>
       </c>
-      <c r="K18" s="36">
-        <f t="shared" si="1"/>
-        <v>25.428376071694668</v>
+      <c r="K18" s="39">
+        <v>30.018312954312446</v>
       </c>
       <c r="L18" s="36">
         <v>30.011573675084005</v>
@@ -7339,9 +7338,8 @@
       <c r="J19" s="36">
         <v>19.908389740000001</v>
       </c>
-      <c r="K19" s="36">
-        <f t="shared" si="1"/>
-        <v>21.868356543767916</v>
+      <c r="K19" s="39">
+        <v>25.857221286837778</v>
       </c>
       <c r="L19" s="36">
         <v>25.788290151303741</v>
@@ -7373,7 +7371,7 @@
         <v>11.754512350000001</v>
       </c>
       <c r="K20" s="36">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="K17:K25" si="1">(J20*2/3)+(L20/3)</f>
         <v>10.986341566666667</v>
       </c>
       <c r="L20" s="36">
@@ -7836,7 +7834,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1E982DE-1A8D-4D0C-9CD3-51B0DFFDA372}">
   <dimension ref="C4:N51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
@@ -9010,7 +9008,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2523A896-A3FC-4F9A-B5DF-A205D08521A3}">
   <dimension ref="C3:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update housing numbers for LED scenario
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_Demands_LED.xlsx
+++ b/SuppXLS/Scen_SYS_Demands_LED.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uccireland-my.sharepoint.com/personal/agaur_ucc_ie/Documents/TIM-2.0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uccireland-my.sharepoint.com/personal/agaur_ucc_ie/Documents/TIM-2.0/TIM/SuppXLS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="106" documentId="13_ncr:1_{C69F530E-E3CE-485A-943C-5B1B3FC47B5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{3F95F6CE-D2D2-43BD-AC95-2271ABB22125}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="113_{293D1C48-0FAE-4514-9C4F-F95949ADE232}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{CBD545CB-4069-4125-80D8-739C9EBC099F}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BY-Demands" sheetId="5" r:id="rId1"/>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="186">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -651,6 +651,15 @@
   </si>
   <si>
     <t>SRVOEL-PU</t>
+  </si>
+  <si>
+    <t>Attrib_Cond</t>
+  </si>
+  <si>
+    <t>Val_Cond</t>
+  </si>
+  <si>
+    <t>IE,National</t>
   </si>
 </sst>
 </file>
@@ -6744,10 +6753,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C1:P44"/>
+  <dimension ref="C1:AP42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E7" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7250,7 +7259,7 @@
       </c>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="4:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:16" x14ac:dyDescent="0.35">
       <c r="D17" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -7282,7 +7291,7 @@
       </c>
       <c r="P17" s="1"/>
     </row>
-    <row r="18" spans="4:16" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:16" x14ac:dyDescent="0.35">
       <c r="D18" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -7314,7 +7323,7 @@
       </c>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="4:16" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:16" x14ac:dyDescent="0.35">
       <c r="D19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -7346,7 +7355,7 @@
       </c>
       <c r="P19" s="1"/>
     </row>
-    <row r="20" spans="4:16" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:16" x14ac:dyDescent="0.35">
       <c r="D20" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -7371,7 +7380,7 @@
         <v>11.754512350000001</v>
       </c>
       <c r="K20" s="36">
-        <f t="shared" ref="K17:K25" si="1">(J20*2/3)+(L20/3)</f>
+        <f t="shared" ref="K20:K25" si="1">(J20*2/3)+(L20/3)</f>
         <v>10.986341566666667</v>
       </c>
       <c r="L20" s="36">
@@ -7379,7 +7388,7 @@
       </c>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="4:16" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:16" x14ac:dyDescent="0.35">
       <c r="D21" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -7411,7 +7420,7 @@
       </c>
       <c r="P21" s="1"/>
     </row>
-    <row r="22" spans="4:16" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:16" x14ac:dyDescent="0.35">
       <c r="D22" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -7445,7 +7454,7 @@
       </c>
       <c r="P22" s="1"/>
     </row>
-    <row r="23" spans="4:16" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:16" x14ac:dyDescent="0.35">
       <c r="D23" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -7477,7 +7486,7 @@
       </c>
       <c r="P23" s="1"/>
     </row>
-    <row r="24" spans="4:16" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:16" x14ac:dyDescent="0.35">
       <c r="D24" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -7511,7 +7520,7 @@
       </c>
       <c r="P24" s="1"/>
     </row>
-    <row r="25" spans="4:16" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:16" x14ac:dyDescent="0.35">
       <c r="D25" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -7545,7 +7554,7 @@
       </c>
       <c r="P25" s="1"/>
     </row>
-    <row r="26" spans="4:16" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:16" x14ac:dyDescent="0.35">
       <c r="D26" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -7554,29 +7563,29 @@
         <v>59</v>
       </c>
       <c r="F26" t="s">
-        <v>52</v>
+        <v>160</v>
       </c>
       <c r="G26" t="s">
-        <v>53</v>
+        <v>161</v>
       </c>
       <c r="H26" s="37">
-        <v>206.79888500000001</v>
-      </c>
-      <c r="I26" s="36">
-        <v>227.33367966704699</v>
-      </c>
-      <c r="J26" s="36">
-        <v>234.01489904006499</v>
+        <v>28.901664567933956</v>
+      </c>
+      <c r="I26" s="38">
+        <v>29.285472960899106</v>
+      </c>
+      <c r="J26" s="38">
+        <v>29.618106901468909</v>
       </c>
       <c r="K26" s="36">
-        <v>355.09166996739799</v>
+        <f>J26*2/3+L26*1/3</f>
+        <v>30.669454951005577</v>
       </c>
       <c r="L26" s="36">
-        <v>614.82387830734103</v>
-      </c>
-      <c r="P26" s="1"/>
-    </row>
-    <row r="27" spans="4:16" x14ac:dyDescent="0.35">
+        <v>32.772151050078904</v>
+      </c>
+    </row>
+    <row r="27" spans="3:16" x14ac:dyDescent="0.35">
       <c r="D27" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -7585,29 +7594,29 @@
         <v>59</v>
       </c>
       <c r="F27" t="s">
-        <v>54</v>
+        <v>162</v>
       </c>
       <c r="G27" t="s">
-        <v>55</v>
+        <v>163</v>
       </c>
       <c r="H27" s="37">
-        <v>766.351721</v>
-      </c>
-      <c r="I27" s="36">
-        <v>805.70916346620595</v>
-      </c>
-      <c r="J27" s="36">
-        <v>818.79213614191099</v>
+        <v>58.151541961987604</v>
+      </c>
+      <c r="I27" s="38">
+        <v>58.923782945423504</v>
+      </c>
+      <c r="J27" s="38">
+        <v>59.593058464401295</v>
       </c>
       <c r="K27" s="36">
-        <v>918.02415110284801</v>
+        <f>J27*2/3+L27*1/3</f>
+        <v>61.758486976267527</v>
       </c>
       <c r="L27" s="36">
-        <v>1051.6575592105</v>
-      </c>
-      <c r="P27" s="1"/>
-    </row>
-    <row r="28" spans="4:16" x14ac:dyDescent="0.35">
+        <v>66.089343999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="3:16" x14ac:dyDescent="0.35">
       <c r="D28" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -7616,29 +7625,24 @@
         <v>59</v>
       </c>
       <c r="F28" t="s">
-        <v>56</v>
+        <v>164</v>
       </c>
       <c r="G28" t="s">
-        <v>57</v>
+        <v>165</v>
       </c>
       <c r="H28" s="37">
-        <v>724.42972899999995</v>
-      </c>
-      <c r="I28" s="36">
-        <v>756.93265686674704</v>
-      </c>
-      <c r="J28" s="36">
-        <v>768.29446481802404</v>
-      </c>
-      <c r="K28" s="36">
-        <v>832.59337892975498</v>
+        <v>5.6291760000000002</v>
+      </c>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
+      <c r="K28" s="38">
+        <v>40.299999999999997</v>
       </c>
       <c r="L28" s="36">
-        <v>889.16483547498206</v>
-      </c>
-      <c r="P28" s="1"/>
-    </row>
-    <row r="29" spans="4:16" x14ac:dyDescent="0.35">
+        <v>40.299999999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="3:16" x14ac:dyDescent="0.35">
       <c r="D29" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -7647,182 +7651,549 @@
         <v>59</v>
       </c>
       <c r="F29" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="G29" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="H29" s="37">
-        <v>28.901664567933956</v>
-      </c>
-      <c r="I29" s="38">
-        <v>29.285472960899106</v>
-      </c>
-      <c r="J29" s="38">
-        <v>29.618106901468909</v>
-      </c>
-      <c r="K29" s="36">
-        <f>J29*2/3+L29*1/3</f>
-        <v>30.669454951005577</v>
+        <v>0.48</v>
+      </c>
+      <c r="I29" s="37"/>
+      <c r="J29" s="37"/>
+      <c r="K29" s="37">
+        <v>0.5</v>
       </c>
       <c r="L29" s="36">
-        <v>32.772151050078904</v>
-      </c>
-    </row>
-    <row r="30" spans="4:16" x14ac:dyDescent="0.35">
-      <c r="D30" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
-        <v>IE,National</v>
-      </c>
-      <c r="E30" t="s">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="30" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+    </row>
+    <row r="31" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+    </row>
+    <row r="32" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="C32" t="s">
+        <v>149</v>
+      </c>
+      <c r="D32" t="s">
+        <v>0</v>
+      </c>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+    </row>
+    <row r="33" spans="3:42" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C33" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="G33" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="H33" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="I33" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="J33" s="13">
+        <v>2018</v>
+      </c>
+      <c r="K33" s="13">
+        <v>2019</v>
+      </c>
+      <c r="L33" s="13">
+        <v>2020</v>
+      </c>
+      <c r="M33" s="13">
+        <v>2021</v>
+      </c>
+      <c r="N33" s="13">
+        <v>2022</v>
+      </c>
+      <c r="O33" s="13">
+        <v>2023</v>
+      </c>
+      <c r="P33" s="13">
+        <v>2024</v>
+      </c>
+      <c r="Q33" s="13">
+        <v>2025</v>
+      </c>
+      <c r="R33" s="13">
+        <v>2026</v>
+      </c>
+      <c r="S33" s="13">
+        <v>2027</v>
+      </c>
+      <c r="T33" s="13">
+        <v>2028</v>
+      </c>
+      <c r="U33" s="13">
+        <v>2029</v>
+      </c>
+      <c r="V33" s="13">
+        <v>2030</v>
+      </c>
+      <c r="W33" s="13">
+        <v>2031</v>
+      </c>
+      <c r="X33" s="13">
+        <v>2032</v>
+      </c>
+      <c r="Y33" s="13">
+        <v>2033</v>
+      </c>
+      <c r="Z33" s="13">
+        <v>2034</v>
+      </c>
+      <c r="AA33" s="13">
+        <v>2035</v>
+      </c>
+      <c r="AB33" s="13">
+        <v>2036</v>
+      </c>
+      <c r="AC33" s="13">
+        <v>2037</v>
+      </c>
+      <c r="AD33" s="13">
+        <v>2038</v>
+      </c>
+      <c r="AE33" s="13">
+        <v>2039</v>
+      </c>
+      <c r="AF33" s="13">
+        <v>2040</v>
+      </c>
+      <c r="AG33" s="13">
+        <v>2041</v>
+      </c>
+      <c r="AH33" s="13">
+        <v>2042</v>
+      </c>
+      <c r="AI33" s="13">
+        <v>2043</v>
+      </c>
+      <c r="AJ33" s="13">
+        <v>2044</v>
+      </c>
+      <c r="AK33" s="13">
+        <v>2045</v>
+      </c>
+      <c r="AL33" s="13">
+        <v>2046</v>
+      </c>
+      <c r="AM33" s="13">
+        <v>2047</v>
+      </c>
+      <c r="AN33" s="13">
+        <v>2048</v>
+      </c>
+      <c r="AO33" s="13">
+        <v>2049</v>
+      </c>
+      <c r="AP33" s="13">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="34" spans="3:42" x14ac:dyDescent="0.35">
+      <c r="D34" t="s">
         <v>59</v>
       </c>
-      <c r="F30" t="s">
-        <v>162</v>
-      </c>
-      <c r="G30" t="s">
-        <v>163</v>
-      </c>
-      <c r="H30" s="37">
-        <v>58.151541961987604</v>
-      </c>
-      <c r="I30" s="38">
-        <v>58.923782945423504</v>
-      </c>
-      <c r="J30" s="38">
-        <v>59.593058464401295</v>
-      </c>
-      <c r="K30" s="36">
-        <f>J30*2/3+L30*1/3</f>
-        <v>61.758486976267527</v>
-      </c>
-      <c r="L30" s="36">
-        <v>66.089343999999997</v>
-      </c>
-    </row>
-    <row r="31" spans="4:16" x14ac:dyDescent="0.35">
-      <c r="D31" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
-        <v>IE,National</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="E34" t="s">
+        <v>185</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J34" s="1">
+        <v>206.79888500000001</v>
+      </c>
+      <c r="K34" s="1">
+        <v>227.33367966704699</v>
+      </c>
+      <c r="L34">
+        <v>234.01489904006499</v>
+      </c>
+      <c r="M34">
+        <v>250.52243040236399</v>
+      </c>
+      <c r="N34">
+        <v>265.47273899323898</v>
+      </c>
+      <c r="O34">
+        <v>279.23643876610601</v>
+      </c>
+      <c r="P34">
+        <v>291.97758934464099</v>
+      </c>
+      <c r="Q34">
+        <v>303.745747309416</v>
+      </c>
+      <c r="R34">
+        <v>314.88867210903697</v>
+      </c>
+      <c r="S34">
+        <v>325.448418136599</v>
+      </c>
+      <c r="T34">
+        <v>335.72138230120601</v>
+      </c>
+      <c r="U34">
+        <v>345.60194314472</v>
+      </c>
+      <c r="V34">
+        <v>355.09166996739799</v>
+      </c>
+      <c r="W34">
+        <v>372.33998569365798</v>
+      </c>
+      <c r="X34">
+        <v>385.16674421872602</v>
+      </c>
+      <c r="Y34">
+        <v>398.22461473825501</v>
+      </c>
+      <c r="Z34">
+        <v>411.45770972769901</v>
+      </c>
+      <c r="AA34">
+        <v>424.76161479887702</v>
+      </c>
+      <c r="AB34">
+        <v>438.12862011422999</v>
+      </c>
+      <c r="AC34">
+        <v>451.68804802308699</v>
+      </c>
+      <c r="AD34">
+        <v>465.40875684082903</v>
+      </c>
+      <c r="AE34">
+        <v>479.13103817121703</v>
+      </c>
+      <c r="AF34">
+        <v>492.828423833106</v>
+      </c>
+      <c r="AG34">
+        <v>502.36472594874499</v>
+      </c>
+      <c r="AH34">
+        <v>516.22001380752999</v>
+      </c>
+      <c r="AI34">
+        <v>530.17405404626902</v>
+      </c>
+      <c r="AJ34">
+        <v>544.19495314722303</v>
+      </c>
+      <c r="AK34">
+        <v>558.26962802562196</v>
+      </c>
+      <c r="AL34">
+        <v>572.38852326507094</v>
+      </c>
+      <c r="AM34">
+        <v>586.53294139438299</v>
+      </c>
+      <c r="AN34">
+        <v>600.68795864299398</v>
+      </c>
+      <c r="AO34">
+        <v>614.82387830734103</v>
+      </c>
+      <c r="AP34">
+        <v>628.93152164032301</v>
+      </c>
+    </row>
+    <row r="35" spans="3:42" x14ac:dyDescent="0.35">
+      <c r="D35" t="s">
         <v>59</v>
       </c>
-      <c r="F31" t="s">
-        <v>164</v>
-      </c>
-      <c r="G31" t="s">
-        <v>165</v>
-      </c>
-      <c r="H31" s="37">
-        <v>5.6291760000000002</v>
-      </c>
-      <c r="I31" s="37"/>
-      <c r="J31" s="37"/>
-      <c r="K31" s="38">
-        <v>40.299999999999997</v>
-      </c>
-      <c r="L31" s="36">
-        <v>40.299999999999997</v>
-      </c>
-    </row>
-    <row r="32" spans="4:16" x14ac:dyDescent="0.35">
-      <c r="D32" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
-        <v>IE,National</v>
-      </c>
-      <c r="E32" t="s">
+      <c r="E35" t="s">
+        <v>185</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J35" s="1">
+        <v>766.351721</v>
+      </c>
+      <c r="K35" s="1">
+        <v>805.70916346620595</v>
+      </c>
+      <c r="L35">
+        <v>818.79213614191099</v>
+      </c>
+      <c r="M35">
+        <v>828.23348265178799</v>
+      </c>
+      <c r="N35">
+        <v>837.71211748108306</v>
+      </c>
+      <c r="O35">
+        <v>847.44596259241098</v>
+      </c>
+      <c r="P35">
+        <v>857.22660991181897</v>
+      </c>
+      <c r="Q35">
+        <v>866.69288183161598</v>
+      </c>
+      <c r="R35">
+        <v>876.45317782380505</v>
+      </c>
+      <c r="S35">
+        <v>886.30184769788696</v>
+      </c>
+      <c r="T35">
+        <v>896.78868422421601</v>
+      </c>
+      <c r="U35">
+        <v>907.41397234982298</v>
+      </c>
+      <c r="V35">
+        <v>918.02415110284801</v>
+      </c>
+      <c r="W35">
+        <v>926.06233489012698</v>
+      </c>
+      <c r="X35">
+        <v>935.42249419952896</v>
+      </c>
+      <c r="Y35">
+        <v>944.78624082315798</v>
+      </c>
+      <c r="Z35">
+        <v>954.01952778809903</v>
+      </c>
+      <c r="AA35">
+        <v>962.89022086688499</v>
+      </c>
+      <c r="AB35">
+        <v>971.40101477560995</v>
+      </c>
+      <c r="AC35">
+        <v>979.85184308314797</v>
+      </c>
+      <c r="AD35">
+        <v>988.17666058914301</v>
+      </c>
+      <c r="AE35">
+        <v>996.04767237168198</v>
+      </c>
+      <c r="AF35">
+        <v>1003.43540212397</v>
+      </c>
+      <c r="AG35">
+        <v>1002.11497030569</v>
+      </c>
+      <c r="AH35">
+        <v>1009.1830944926101</v>
+      </c>
+      <c r="AI35">
+        <v>1016.05596064786</v>
+      </c>
+      <c r="AJ35">
+        <v>1022.6819321704</v>
+      </c>
+      <c r="AK35">
+        <v>1029.0480878439801</v>
+      </c>
+      <c r="AL35">
+        <v>1035.14898193112</v>
+      </c>
+      <c r="AM35">
+        <v>1040.9634765099099</v>
+      </c>
+      <c r="AN35">
+        <v>1046.47869262623</v>
+      </c>
+      <c r="AO35">
+        <v>1051.6575592105</v>
+      </c>
+      <c r="AP35">
+        <v>1056.50027926231</v>
+      </c>
+    </row>
+    <row r="36" spans="3:42" x14ac:dyDescent="0.35">
+      <c r="D36" t="s">
         <v>59</v>
       </c>
-      <c r="F32" t="s">
-        <v>166</v>
-      </c>
-      <c r="G32" t="s">
-        <v>167</v>
-      </c>
-      <c r="H32" s="37">
-        <v>0.48</v>
-      </c>
-      <c r="I32" s="37"/>
-      <c r="J32" s="37"/>
-      <c r="K32" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="L32" s="36">
-        <v>0.54</v>
-      </c>
-    </row>
-    <row r="33" spans="8:11" x14ac:dyDescent="0.35">
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
-    </row>
-    <row r="34" spans="8:11" x14ac:dyDescent="0.35">
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-    </row>
-    <row r="35" spans="8:11" x14ac:dyDescent="0.35">
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-    </row>
-    <row r="36" spans="8:11" x14ac:dyDescent="0.35">
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
-    </row>
-    <row r="37" spans="8:11" x14ac:dyDescent="0.35">
+      <c r="E36" t="s">
+        <v>185</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J36" s="1">
+        <v>724.42972899999995</v>
+      </c>
+      <c r="K36" s="1">
+        <v>756.93265686674704</v>
+      </c>
+      <c r="L36">
+        <v>768.29446481802404</v>
+      </c>
+      <c r="M36">
+        <v>772.86208694584798</v>
+      </c>
+      <c r="N36">
+        <v>777.95194352567796</v>
+      </c>
+      <c r="O36">
+        <v>783.67269864148204</v>
+      </c>
+      <c r="P36">
+        <v>789.75930268250397</v>
+      </c>
+      <c r="Q36">
+        <v>795.82537085896797</v>
+      </c>
+      <c r="R36">
+        <v>802.38775006715798</v>
+      </c>
+      <c r="S36">
+        <v>809.22213416551403</v>
+      </c>
+      <c r="T36">
+        <v>816.80113347457802</v>
+      </c>
+      <c r="U36">
+        <v>824.64428658311704</v>
+      </c>
+      <c r="V36">
+        <v>832.59337892975498</v>
+      </c>
+      <c r="W36">
+        <v>835.494721776652</v>
+      </c>
+      <c r="X36">
+        <v>841.12386901591697</v>
+      </c>
+      <c r="Y36">
+        <v>846.68490394820003</v>
+      </c>
+      <c r="Z36">
+        <v>852.05750789504805</v>
+      </c>
+      <c r="AA36">
+        <v>857.03569133233998</v>
+      </c>
+      <c r="AB36">
+        <v>861.62461714738197</v>
+      </c>
+      <c r="AC36">
+        <v>866.09217418652202</v>
+      </c>
+      <c r="AD36">
+        <v>870.38020137632998</v>
+      </c>
+      <c r="AE36">
+        <v>874.20163295403097</v>
+      </c>
+      <c r="AF36">
+        <v>877.53441615506995</v>
+      </c>
+      <c r="AG36">
+        <v>873.21565965240802</v>
+      </c>
+      <c r="AH36">
+        <v>876.17112006521802</v>
+      </c>
+      <c r="AI36">
+        <v>878.89535131181003</v>
+      </c>
+      <c r="AJ36">
+        <v>881.34522505719599</v>
+      </c>
+      <c r="AK36">
+        <v>883.51153419697505</v>
+      </c>
+      <c r="AL36">
+        <v>885.39165384489604</v>
+      </c>
+      <c r="AM36">
+        <v>886.96968161539996</v>
+      </c>
+      <c r="AN36">
+        <v>888.23702563617996</v>
+      </c>
+      <c r="AO36">
+        <v>889.16483547498206</v>
+      </c>
+      <c r="AP36">
+        <v>889.75617108824804</v>
+      </c>
+    </row>
+    <row r="37" spans="3:42" x14ac:dyDescent="0.35">
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="8:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:42" x14ac:dyDescent="0.35">
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
     </row>
-    <row r="39" spans="8:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:42" x14ac:dyDescent="0.35">
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
     </row>
-    <row r="40" spans="8:11" x14ac:dyDescent="0.35">
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
-    </row>
-    <row r="41" spans="8:11" x14ac:dyDescent="0.35">
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
-    </row>
-    <row r="42" spans="8:11" x14ac:dyDescent="0.35">
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
-    </row>
-    <row r="43" spans="8:11" x14ac:dyDescent="0.35">
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
-      <c r="K43" s="1"/>
-    </row>
-    <row r="44" spans="8:11" x14ac:dyDescent="0.35">
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-      <c r="K44" s="1"/>
+    <row r="40" spans="3:42" x14ac:dyDescent="0.35">
+      <c r="H40" s="37"/>
+      <c r="I40" s="36"/>
+      <c r="J40" s="36"/>
+      <c r="K40" s="36"/>
+      <c r="L40" s="36"/>
+      <c r="P40" s="1"/>
+    </row>
+    <row r="41" spans="3:42" x14ac:dyDescent="0.35">
+      <c r="H41" s="37"/>
+      <c r="I41" s="36"/>
+      <c r="J41" s="36"/>
+      <c r="K41" s="36"/>
+      <c r="L41" s="36"/>
+      <c r="P41" s="1"/>
+    </row>
+    <row r="42" spans="3:42" x14ac:dyDescent="0.35">
+      <c r="H42" s="37"/>
+      <c r="I42" s="36"/>
+      <c r="J42" s="36"/>
+      <c r="K42" s="36"/>
+      <c r="L42" s="36"/>
+      <c r="P42" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7834,7 +8205,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1E982DE-1A8D-4D0C-9CD3-51B0DFFDA372}">
   <dimension ref="C4:N51"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Remove the reduction in RSD stock numbers in 2041
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_Demands_LED.xlsx
+++ b/SuppXLS/Scen_SYS_Demands_LED.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85AA639-E78C-4374-896F-B440DCF12F08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7739537-8951-4A2E-B852-3C58479764D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BY-Demands" sheetId="5" r:id="rId1"/>
@@ -671,8 +671,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="\Te\x\t"/>
-    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="\Te\x\t"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -975,7 +975,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="12" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="12" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -987,8 +987,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -3765,8 +3765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCA64845-990F-4F8F-9F7F-F4DBD3794313}">
   <dimension ref="B2:AF39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8840,10 +8840,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C1:AQ42"/>
+  <dimension ref="C1:AQ39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="Z9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AO40" sqref="AO40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10071,10 +10071,10 @@
         <v>492.828423833106</v>
       </c>
       <c r="AG34">
-        <v>502.36472594874499</v>
+        <v>496.36472594874499</v>
       </c>
       <c r="AH34">
-        <v>516.22001380752999</v>
+        <v>514.52001380752995</v>
       </c>
       <c r="AI34">
         <v>530.17405404626902</v>
@@ -10187,7 +10187,7 @@
         <v>1003.43540212397</v>
       </c>
       <c r="AG35">
-        <v>1002.11497030569</v>
+        <v>1003.61497030569</v>
       </c>
       <c r="AH35">
         <v>1009.1830944926101</v>
@@ -10303,10 +10303,10 @@
         <v>877.53441615506995</v>
       </c>
       <c r="AG36">
-        <v>873.21565965240802</v>
+        <v>877.71565965240802</v>
       </c>
       <c r="AH36">
-        <v>876.17112006521802</v>
+        <v>877.87112006521807</v>
       </c>
       <c r="AI36">
         <v>878.89535131181003</v>
@@ -10353,30 +10353,6 @@
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
-    </row>
-    <row r="40" spans="3:43" x14ac:dyDescent="0.25">
-      <c r="H40" s="36"/>
-      <c r="I40" s="35"/>
-      <c r="J40" s="35"/>
-      <c r="K40" s="35"/>
-      <c r="L40" s="35"/>
-      <c r="P40" s="1"/>
-    </row>
-    <row r="41" spans="3:43" x14ac:dyDescent="0.25">
-      <c r="H41" s="36"/>
-      <c r="I41" s="35"/>
-      <c r="J41" s="35"/>
-      <c r="K41" s="35"/>
-      <c r="L41" s="35"/>
-      <c r="P41" s="1"/>
-    </row>
-    <row r="42" spans="3:43" x14ac:dyDescent="0.25">
-      <c r="H42" s="36"/>
-      <c r="I42" s="35"/>
-      <c r="J42" s="35"/>
-      <c r="K42" s="35"/>
-      <c r="L42" s="35"/>
-      <c r="P42" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10388,8 +10364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1E982DE-1A8D-4D0C-9CD3-51B0DFFDA372}">
   <dimension ref="C4:N51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11563,7 +11539,7 @@
   <dimension ref="C3:N33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>